<commit_message>
add more qubit data
</commit_message>
<xml_diff>
--- a/analyses/master-qubit.xlsx
+++ b/analyses/master-qubit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03BB36E-A887-5643-BF29-35B744C4FD46}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4613FE5C-426E-164D-BBDA-A3BB64B9ACC2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="14900" xr2:uid="{C961D9B2-DEF5-3E45-BFAA-11F0CD1F34D4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3181" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3336" uniqueCount="644">
   <si>
     <t>tube_number</t>
   </si>
@@ -1885,6 +1885,87 @@
   </si>
   <si>
     <t>516-3</t>
+  </si>
+  <si>
+    <t>2019-10-25_110714</t>
+  </si>
+  <si>
+    <t>Sample_#191025-111133</t>
+  </si>
+  <si>
+    <t>Sample_#191025-111124</t>
+  </si>
+  <si>
+    <t>Sample_#191025-111115</t>
+  </si>
+  <si>
+    <t>Sample_#191025-111106</t>
+  </si>
+  <si>
+    <t>Sample_#191025-111056</t>
+  </si>
+  <si>
+    <t>Sample_#191025-111046</t>
+  </si>
+  <si>
+    <t>Sample_#191025-111036</t>
+  </si>
+  <si>
+    <t>Sample_#191025-111027</t>
+  </si>
+  <si>
+    <t>Sample_#191025-111015</t>
+  </si>
+  <si>
+    <t>Sample_#191025-111005</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110955</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110945</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110935</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110927</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110915</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110906</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110854</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110844</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110833</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110823</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110813</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110803</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110752</t>
+  </si>
+  <si>
+    <t>Sample_#191025-110739</t>
+  </si>
+  <si>
+    <t>https://grace-ac.github.io/extract-RNA/</t>
+  </si>
+  <si>
+    <t>extracted / missing</t>
   </si>
 </sst>
 </file>
@@ -1950,7 +2031,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1959,6 +2040,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2274,10 +2356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EE0E31-7CFF-2843-B4D6-D974DF19D232}">
-  <dimension ref="A1:U398"/>
+  <dimension ref="A1:U425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A312" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D332" sqref="D332"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2390,7 +2472,7 @@
         <v>50</v>
       </c>
       <c r="M2">
-        <f>(F2)*(L2-G2)</f>
+        <f t="shared" ref="M2:M65" si="0">(F2)*(L2-G2)</f>
         <v>35.840000000000003</v>
       </c>
       <c r="N2" t="s">
@@ -2438,7 +2520,7 @@
         <v>50</v>
       </c>
       <c r="M3" t="e">
-        <f>(F3)*(L3-G3)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="N3" t="s">
@@ -2486,7 +2568,7 @@
         <v>50</v>
       </c>
       <c r="M4">
-        <f>(F4)*(L4-G4)</f>
+        <f t="shared" si="0"/>
         <v>76.95</v>
       </c>
       <c r="N4" t="s">
@@ -2534,7 +2616,7 @@
         <v>50</v>
       </c>
       <c r="M5">
-        <f>(F5)*(L5-G5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N5" t="s">
@@ -2582,7 +2664,7 @@
         <v>50</v>
       </c>
       <c r="M6">
-        <f>(F6)*(L6-G6)</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="N6" t="s">
@@ -2630,7 +2712,7 @@
         <v>50</v>
       </c>
       <c r="M7">
-        <f>(F7)*(L7-G7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N7" t="s">
@@ -2678,7 +2760,7 @@
         <v>50</v>
       </c>
       <c r="M8">
-        <f>(F8)*(L8-G8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N8" t="s">
@@ -2726,7 +2808,7 @@
         <v>50</v>
       </c>
       <c r="M9">
-        <f>(F9)*(L9-G9)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="N9" t="s">
@@ -2774,7 +2856,7 @@
         <v>50</v>
       </c>
       <c r="M10">
-        <f>(F10)*(L10-G10)</f>
+        <f t="shared" si="0"/>
         <v>52.199999999999996</v>
       </c>
       <c r="N10" t="s">
@@ -2822,7 +2904,7 @@
         <v>50</v>
       </c>
       <c r="M11">
-        <f>(F11)*(L11-G11)</f>
+        <f t="shared" si="0"/>
         <v>232.20000000000002</v>
       </c>
       <c r="N11" t="s">
@@ -2870,7 +2952,7 @@
         <v>50</v>
       </c>
       <c r="M12">
-        <f>(F12)*(L12-G12)</f>
+        <f t="shared" si="0"/>
         <v>226.8</v>
       </c>
       <c r="N12" t="s">
@@ -2915,7 +2997,7 @@
         <v>50</v>
       </c>
       <c r="M13">
-        <f>(F13)*(L13-G13)</f>
+        <f t="shared" si="0"/>
         <v>161.1</v>
       </c>
       <c r="N13" t="s">
@@ -2960,7 +3042,7 @@
         <v>50</v>
       </c>
       <c r="M14">
-        <f>(F14)*(L14-G14)</f>
+        <f t="shared" si="0"/>
         <v>59.400000000000006</v>
       </c>
       <c r="N14" t="s">
@@ -3008,7 +3090,7 @@
         <v>50</v>
       </c>
       <c r="M15">
-        <f>(F15)*(L15-G15)</f>
+        <f t="shared" si="0"/>
         <v>123.75</v>
       </c>
       <c r="N15" t="s">
@@ -3056,7 +3138,7 @@
         <v>50</v>
       </c>
       <c r="M16">
-        <f>(F16)*(L16-G16)</f>
+        <f t="shared" si="0"/>
         <v>158.4</v>
       </c>
       <c r="N16" t="s">
@@ -3104,7 +3186,7 @@
         <v>50</v>
       </c>
       <c r="M17">
-        <f>(F17)*(L17-G17)</f>
+        <f t="shared" si="0"/>
         <v>221.4</v>
       </c>
       <c r="N17" t="s">
@@ -3152,7 +3234,7 @@
         <v>50</v>
       </c>
       <c r="M18">
-        <f>(F18)*(L18-G18)</f>
+        <f t="shared" si="0"/>
         <v>90.449999999999989</v>
       </c>
       <c r="N18" t="s">
@@ -3200,7 +3282,7 @@
         <v>50</v>
       </c>
       <c r="M19">
-        <f>(F19)*(L19-G19)</f>
+        <f t="shared" si="0"/>
         <v>259.2</v>
       </c>
       <c r="N19" t="s">
@@ -3248,7 +3330,7 @@
         <v>50</v>
       </c>
       <c r="M20">
-        <f>(F20)*(L20-G20)</f>
+        <f t="shared" si="0"/>
         <v>120.60000000000001</v>
       </c>
       <c r="N20" t="s">
@@ -3296,7 +3378,7 @@
         <v>50</v>
       </c>
       <c r="M21">
-        <f>(F21)*(L21-G21)</f>
+        <f t="shared" si="0"/>
         <v>82.8</v>
       </c>
       <c r="N21" t="s">
@@ -3344,7 +3426,7 @@
         <v>50</v>
       </c>
       <c r="M22">
-        <f>(F22)*(L22-G22)</f>
+        <f t="shared" si="0"/>
         <v>48.6</v>
       </c>
       <c r="N22" t="s">
@@ -3392,7 +3474,7 @@
         <v>50</v>
       </c>
       <c r="M23">
-        <f>(F23)*(L23-G23)</f>
+        <f t="shared" si="0"/>
         <v>62.099999999999994</v>
       </c>
       <c r="N23" t="s">
@@ -3440,7 +3522,7 @@
         <v>50</v>
       </c>
       <c r="M24">
-        <f>(F24)*(L24-G24)</f>
+        <f t="shared" si="0"/>
         <v>105.3</v>
       </c>
       <c r="N24" t="s">
@@ -3488,7 +3570,7 @@
         <v>50</v>
       </c>
       <c r="M25">
-        <f>(F25)*(L25-G25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N25" t="s">
@@ -3536,7 +3618,7 @@
         <v>50</v>
       </c>
       <c r="M26">
-        <f>(F26)*(L26-G26)</f>
+        <f t="shared" si="0"/>
         <v>109.8</v>
       </c>
       <c r="N26" t="s">
@@ -3584,7 +3666,7 @@
         <v>50</v>
       </c>
       <c r="M27">
-        <f>(F27)*(L27-G27)</f>
+        <f t="shared" si="0"/>
         <v>166.95</v>
       </c>
       <c r="N27" t="s">
@@ -3632,7 +3714,7 @@
         <v>50</v>
       </c>
       <c r="M28">
-        <f>(F28)*(L28-G28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N28" t="s">
@@ -3680,7 +3762,7 @@
         <v>50</v>
       </c>
       <c r="M29">
-        <f>(F29)*(L29-G29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N29" t="s">
@@ -3728,7 +3810,7 @@
         <v>50</v>
       </c>
       <c r="M30">
-        <f>(F30)*(L30-G30)</f>
+        <f t="shared" si="0"/>
         <v>329.40000000000003</v>
       </c>
       <c r="N30" t="s">
@@ -3776,7 +3858,7 @@
         <v>50</v>
       </c>
       <c r="M31">
-        <f>(F31)*(L31-G31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N31" t="s">
@@ -3824,7 +3906,7 @@
         <v>50</v>
       </c>
       <c r="M32">
-        <f>(F32)*(L32-G32)</f>
+        <f t="shared" si="0"/>
         <v>63.9</v>
       </c>
       <c r="N32" t="s">
@@ -3872,7 +3954,7 @@
         <v>50</v>
       </c>
       <c r="M33">
-        <f>(F33)*(L33-G33)</f>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="N33" t="s">
@@ -3920,7 +4002,7 @@
         <v>50</v>
       </c>
       <c r="M34">
-        <f>(F34)*(L34-G34)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="N34" t="s">
@@ -3968,7 +4050,7 @@
         <v>50</v>
       </c>
       <c r="M35">
-        <f>(F35)*(L35-G35)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N35" t="s">
@@ -4016,7 +4098,7 @@
         <v>50</v>
       </c>
       <c r="M36">
-        <f>(F36)*(L36-G36)</f>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="N36" t="s">
@@ -4064,7 +4146,7 @@
         <v>50</v>
       </c>
       <c r="M37">
-        <f>(F37)*(L37-G37)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N37" t="s">
@@ -4112,7 +4194,7 @@
         <v>50</v>
       </c>
       <c r="M38">
-        <f>(F38)*(L38-G38)</f>
+        <f t="shared" si="0"/>
         <v>77.400000000000006</v>
       </c>
       <c r="N38" t="s">
@@ -4160,7 +4242,7 @@
         <v>50</v>
       </c>
       <c r="M39">
-        <f>(F39)*(L39-G39)</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="N39" t="s">
@@ -4208,7 +4290,7 @@
         <v>50</v>
       </c>
       <c r="M40">
-        <f>(F40)*(L40-G40)</f>
+        <f t="shared" si="0"/>
         <v>69.75</v>
       </c>
       <c r="N40" t="s">
@@ -4256,7 +4338,7 @@
         <v>50</v>
       </c>
       <c r="M41">
-        <f>(F41)*(L41-G41)</f>
+        <f t="shared" si="0"/>
         <v>250.2</v>
       </c>
       <c r="N41" t="s">
@@ -4304,7 +4386,7 @@
         <v>50</v>
       </c>
       <c r="M42">
-        <f>(F42)*(L42-G42)</f>
+        <f t="shared" si="0"/>
         <v>232.20000000000002</v>
       </c>
       <c r="N42" t="s">
@@ -4352,7 +4434,7 @@
         <v>50</v>
       </c>
       <c r="M43">
-        <f>(F43)*(L43-G43)</f>
+        <f t="shared" si="0"/>
         <v>98.100000000000009</v>
       </c>
       <c r="N43" t="s">
@@ -4400,7 +4482,7 @@
         <v>50</v>
       </c>
       <c r="M44">
-        <f>(F44)*(L44-G44)</f>
+        <f t="shared" si="0"/>
         <v>187.20000000000002</v>
       </c>
       <c r="N44" t="s">
@@ -4448,7 +4530,7 @@
         <v>50</v>
       </c>
       <c r="M45">
-        <f>(F45)*(L45-G45)</f>
+        <f t="shared" si="0"/>
         <v>126.45</v>
       </c>
       <c r="N45" t="s">
@@ -4496,7 +4578,7 @@
         <v>50</v>
       </c>
       <c r="M46">
-        <f>(F46)*(L46-G46)</f>
+        <f t="shared" si="0"/>
         <v>90.9</v>
       </c>
       <c r="N46" t="s">
@@ -4544,7 +4626,7 @@
         <v>50</v>
       </c>
       <c r="M47">
-        <f>(F47)*(L47-G47)</f>
+        <f t="shared" si="0"/>
         <v>173.7</v>
       </c>
       <c r="N47" t="s">
@@ -4592,7 +4674,7 @@
         <v>50</v>
       </c>
       <c r="M48">
-        <f>(F48)*(L48-G48)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N48" t="s">
@@ -4640,7 +4722,7 @@
         <v>50</v>
       </c>
       <c r="M49">
-        <f>(F49)*(L49-G49)</f>
+        <f t="shared" si="0"/>
         <v>73.8</v>
       </c>
       <c r="N49" t="s">
@@ -4688,7 +4770,7 @@
         <v>50</v>
       </c>
       <c r="M50">
-        <f>(F50)*(L50-G50)</f>
+        <f t="shared" si="0"/>
         <v>370.8</v>
       </c>
       <c r="N50" t="s">
@@ -4736,7 +4818,7 @@
         <v>50</v>
       </c>
       <c r="M51">
-        <f>(F51)*(L51-G51)</f>
+        <f t="shared" si="0"/>
         <v>175.5</v>
       </c>
       <c r="N51" t="s">
@@ -4784,7 +4866,7 @@
         <v>50</v>
       </c>
       <c r="M52">
-        <f>(F52)*(L52-G52)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N52" t="s">
@@ -4832,7 +4914,7 @@
         <v>50</v>
       </c>
       <c r="M53">
-        <f>(F53)*(L53-G53)</f>
+        <f t="shared" si="0"/>
         <v>139.04999999999998</v>
       </c>
       <c r="N53" t="s">
@@ -4880,7 +4962,7 @@
         <v>50</v>
       </c>
       <c r="M54">
-        <f>(F54)*(L54-G54)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N54" t="s">
@@ -4928,7 +5010,7 @@
         <v>50</v>
       </c>
       <c r="M55">
-        <f>(F55)*(L55-G55)</f>
+        <f t="shared" si="0"/>
         <v>98.100000000000009</v>
       </c>
       <c r="N55" t="s">
@@ -4976,7 +5058,7 @@
         <v>50</v>
       </c>
       <c r="M56">
-        <f>(F56)*(L56-G56)</f>
+        <f t="shared" si="0"/>
         <v>65.7</v>
       </c>
       <c r="N56" t="s">
@@ -5024,7 +5106,7 @@
         <v>50</v>
       </c>
       <c r="M57">
-        <f>(F57)*(L57-G57)</f>
+        <f t="shared" si="0"/>
         <v>118.80000000000001</v>
       </c>
       <c r="N57" t="s">
@@ -5072,7 +5154,7 @@
         <v>50</v>
       </c>
       <c r="M58">
-        <f>(F58)*(L58-G58)</f>
+        <f t="shared" si="0"/>
         <v>112.94999999999999</v>
       </c>
       <c r="N58" t="s">
@@ -5120,7 +5202,7 @@
         <v>50</v>
       </c>
       <c r="M59">
-        <f>(F59)*(L59-G59)</f>
+        <f t="shared" si="0"/>
         <v>109.8</v>
       </c>
       <c r="N59" t="s">
@@ -5168,7 +5250,7 @@
         <v>50</v>
       </c>
       <c r="M60">
-        <f>(F60)*(L60-G60)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N60" t="s">
@@ -5216,7 +5298,7 @@
         <v>50</v>
       </c>
       <c r="M61">
-        <f>(F61)*(L61-G61)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="N61" t="s">
@@ -5264,7 +5346,7 @@
         <v>50</v>
       </c>
       <c r="M62">
-        <f>(F62)*(L62-G62)</f>
+        <f t="shared" si="0"/>
         <v>264.60000000000002</v>
       </c>
       <c r="N62" t="s">
@@ -5309,7 +5391,7 @@
         <v>50</v>
       </c>
       <c r="M63">
-        <f>(F63)*(L63-G63)</f>
+        <f t="shared" si="0"/>
         <v>216</v>
       </c>
       <c r="N63" t="s">
@@ -5354,7 +5436,7 @@
         <v>50</v>
       </c>
       <c r="M64">
-        <f>(F64)*(L64-G64)</f>
+        <f t="shared" si="0"/>
         <v>370.8</v>
       </c>
       <c r="N64" t="s">
@@ -5399,7 +5481,7 @@
         <v>50</v>
       </c>
       <c r="M65">
-        <f>(F65)*(L65-G65)</f>
+        <f t="shared" si="0"/>
         <v>361.79999999999995</v>
       </c>
       <c r="N65" t="s">
@@ -5444,7 +5526,7 @@
         <v>50</v>
       </c>
       <c r="M66">
-        <f>(F66)*(L66-G66)</f>
+        <f t="shared" ref="M66:M129" si="1">(F66)*(L66-G66)</f>
         <v>52.199999999999996</v>
       </c>
       <c r="N66" t="s">
@@ -5489,7 +5571,7 @@
         <v>50</v>
       </c>
       <c r="M67">
-        <f>(F67)*(L67-G67)</f>
+        <f t="shared" si="1"/>
         <v>300.59999999999997</v>
       </c>
       <c r="N67" t="s">
@@ -5534,7 +5616,7 @@
         <v>50</v>
       </c>
       <c r="M68">
-        <f>(F68)*(L68-G68)</f>
+        <f t="shared" si="1"/>
         <v>37.799999999999997</v>
       </c>
       <c r="N68" t="s">
@@ -5579,7 +5661,7 @@
         <v>50</v>
       </c>
       <c r="M69">
-        <f>(F69)*(L69-G69)</f>
+        <f t="shared" si="1"/>
         <v>239.4</v>
       </c>
       <c r="N69" t="s">
@@ -5624,7 +5706,7 @@
         <v>50</v>
       </c>
       <c r="M70">
-        <f>(F70)*(L70-G70)</f>
+        <f t="shared" si="1"/>
         <v>225</v>
       </c>
       <c r="N70" t="s">
@@ -5669,7 +5751,7 @@
         <v>50</v>
       </c>
       <c r="M71">
-        <f>(F71)*(L71-G71)</f>
+        <f t="shared" si="1"/>
         <v>139.5</v>
       </c>
       <c r="N71" t="s">
@@ -5714,7 +5796,7 @@
         <v>50</v>
       </c>
       <c r="M72">
-        <f>(F72)*(L72-G72)</f>
+        <f t="shared" si="1"/>
         <v>210.6</v>
       </c>
       <c r="N72" t="s">
@@ -5759,7 +5841,7 @@
         <v>50</v>
       </c>
       <c r="M73">
-        <f>(F73)*(L73-G73)</f>
+        <f t="shared" si="1"/>
         <v>95.4</v>
       </c>
       <c r="N73" t="s">
@@ -5804,7 +5886,7 @@
         <v>50</v>
       </c>
       <c r="M74">
-        <f>(F74)*(L74-G74)</f>
+        <f t="shared" si="1"/>
         <v>279</v>
       </c>
       <c r="N74" t="s">
@@ -5849,7 +5931,7 @@
         <v>50</v>
       </c>
       <c r="M75">
-        <f>(F75)*(L75-G75)</f>
+        <f t="shared" si="1"/>
         <v>41.4</v>
       </c>
       <c r="N75" t="s">
@@ -5894,7 +5976,7 @@
         <v>50</v>
       </c>
       <c r="M76">
-        <f>(F76)*(L76-G76)</f>
+        <f t="shared" si="1"/>
         <v>119.7</v>
       </c>
       <c r="N76" t="s">
@@ -5942,7 +6024,7 @@
         <v>50</v>
       </c>
       <c r="M77">
-        <f>(F77)*(L77-G77)</f>
+        <f t="shared" si="1"/>
         <v>289.8</v>
       </c>
       <c r="N77" t="s">
@@ -5990,7 +6072,7 @@
         <v>50</v>
       </c>
       <c r="M78">
-        <f>(F78)*(L78-G78)</f>
+        <f t="shared" si="1"/>
         <v>277.2</v>
       </c>
       <c r="N78" t="s">
@@ -6038,7 +6120,7 @@
         <v>50</v>
       </c>
       <c r="M79">
-        <f>(F79)*(L79-G79)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N79" t="s">
@@ -6086,7 +6168,7 @@
         <v>50</v>
       </c>
       <c r="M80">
-        <f>(F80)*(L80-G80)</f>
+        <f t="shared" si="1"/>
         <v>98.55</v>
       </c>
       <c r="N80" t="s">
@@ -6134,7 +6216,7 @@
         <v>50</v>
       </c>
       <c r="M81">
-        <f>(F81)*(L81-G81)</f>
+        <f t="shared" si="1"/>
         <v>159.75</v>
       </c>
       <c r="N81" t="s">
@@ -6182,7 +6264,7 @@
         <v>50</v>
       </c>
       <c r="M82">
-        <f>(F82)*(L82-G82)</f>
+        <f t="shared" si="1"/>
         <v>79.2</v>
       </c>
       <c r="N82" t="s">
@@ -6230,7 +6312,7 @@
         <v>50</v>
       </c>
       <c r="M83">
-        <f>(F83)*(L83-G83)</f>
+        <f t="shared" si="1"/>
         <v>253.79999999999998</v>
       </c>
       <c r="N83" t="s">
@@ -6278,7 +6360,7 @@
         <v>50</v>
       </c>
       <c r="M84">
-        <f>(F84)*(L84-G84)</f>
+        <f t="shared" si="1"/>
         <v>79.650000000000006</v>
       </c>
       <c r="N84" t="s">
@@ -6326,7 +6408,7 @@
         <v>50</v>
       </c>
       <c r="M85">
-        <f>(F85)*(L85-G85)</f>
+        <f t="shared" si="1"/>
         <v>264.60000000000002</v>
       </c>
       <c r="N85" t="s">
@@ -6362,7 +6444,7 @@
         <v>50</v>
       </c>
       <c r="M86" t="e">
-        <f>(F86)*(L86-G86)</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="N86" t="s">
@@ -6401,7 +6483,7 @@
         <v>50</v>
       </c>
       <c r="M87" t="e">
-        <f>(F87)*(L87-G87)</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="N87" t="s">
@@ -6440,7 +6522,7 @@
         <v>50</v>
       </c>
       <c r="M88" t="e">
-        <f>(F88)*(L88-G88)</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="N88" t="s">
@@ -6479,7 +6561,7 @@
         <v>50</v>
       </c>
       <c r="M89" t="e">
-        <f>(F89)*(L89-G89)</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="N89" t="s">
@@ -6518,7 +6600,7 @@
         <v>50</v>
       </c>
       <c r="M90" t="e">
-        <f>(F90)*(L90-G90)</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="N90" t="s">
@@ -6557,7 +6639,7 @@
         <v>50</v>
       </c>
       <c r="M91" t="e">
-        <f>(F91)*(L91-G91)</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="N91" t="s">
@@ -6596,7 +6678,7 @@
         <v>50</v>
       </c>
       <c r="M92" t="e">
-        <f>(F92)*(L92-G92)</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="N92" t="s">
@@ -6635,7 +6717,7 @@
         <v>50</v>
       </c>
       <c r="M93" t="e">
-        <f>(F93)*(L93-G93)</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="N93" t="s">
@@ -6674,7 +6756,7 @@
         <v>50</v>
       </c>
       <c r="M94" t="e">
-        <f>(F94)*(L94-G94)</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="N94" t="s">
@@ -6725,7 +6807,7 @@
         <v>50</v>
       </c>
       <c r="M95">
-        <f>(F95)*(L95-G95)</f>
+        <f t="shared" si="1"/>
         <v>198.00000000000003</v>
       </c>
       <c r="N95" t="s">
@@ -6773,7 +6855,7 @@
         <v>50</v>
       </c>
       <c r="M96">
-        <f>(F96)*(L96-G96)</f>
+        <f t="shared" si="1"/>
         <v>153.45000000000002</v>
       </c>
       <c r="N96" t="s">
@@ -6821,7 +6903,7 @@
         <v>50</v>
       </c>
       <c r="M97">
-        <f>(F97)*(L97-G97)</f>
+        <f t="shared" si="1"/>
         <v>73.8</v>
       </c>
       <c r="N97" t="s">
@@ -6869,7 +6951,7 @@
         <v>50</v>
       </c>
       <c r="M98">
-        <f>(F98)*(L98-G98)</f>
+        <f t="shared" si="1"/>
         <v>117.9</v>
       </c>
       <c r="N98" t="s">
@@ -6917,7 +6999,7 @@
         <v>50</v>
       </c>
       <c r="M99">
-        <f>(F99)*(L99-G99)</f>
+        <f t="shared" si="1"/>
         <v>149.4</v>
       </c>
       <c r="N99" t="s">
@@ -6965,7 +7047,7 @@
         <v>50</v>
       </c>
       <c r="M100">
-        <f>(F100)*(L100-G100)</f>
+        <f t="shared" si="1"/>
         <v>136.35</v>
       </c>
       <c r="N100" t="s">
@@ -7013,7 +7095,7 @@
         <v>50</v>
       </c>
       <c r="M101">
-        <f>(F101)*(L101-G101)</f>
+        <f t="shared" si="1"/>
         <v>237.60000000000002</v>
       </c>
       <c r="N101" t="s">
@@ -7061,7 +7143,7 @@
         <v>50</v>
       </c>
       <c r="M102">
-        <f>(F102)*(L102-G102)</f>
+        <f t="shared" si="1"/>
         <v>157.94999999999999</v>
       </c>
       <c r="N102" t="s">
@@ -7109,7 +7191,7 @@
         <v>50</v>
       </c>
       <c r="M103">
-        <f>(F103)*(L103-G103)</f>
+        <f t="shared" si="1"/>
         <v>72.900000000000006</v>
       </c>
       <c r="N103" t="s">
@@ -7157,7 +7239,7 @@
         <v>50</v>
       </c>
       <c r="M104">
-        <f>(F104)*(L104-G104)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N104" t="s">
@@ -7205,7 +7287,7 @@
         <v>50</v>
       </c>
       <c r="M105">
-        <f>(F105)*(L105-G105)</f>
+        <f t="shared" si="1"/>
         <v>243.00000000000003</v>
       </c>
       <c r="N105" t="s">
@@ -7253,7 +7335,7 @@
         <v>50</v>
       </c>
       <c r="M106">
-        <f>(F106)*(L106-G106)</f>
+        <f t="shared" si="1"/>
         <v>94.5</v>
       </c>
       <c r="N106" t="s">
@@ -7301,7 +7383,7 @@
         <v>50</v>
       </c>
       <c r="M107">
-        <f>(F107)*(L107-G107)</f>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="N107" t="s">
@@ -7349,7 +7431,7 @@
         <v>50</v>
       </c>
       <c r="M108">
-        <f>(F108)*(L108-G108)</f>
+        <f t="shared" si="1"/>
         <v>84.6</v>
       </c>
       <c r="N108" t="s">
@@ -7397,7 +7479,7 @@
         <v>50</v>
       </c>
       <c r="M109">
-        <f>(F109)*(L109-G109)</f>
+        <f t="shared" si="1"/>
         <v>107.1</v>
       </c>
       <c r="N109" t="s">
@@ -7445,7 +7527,7 @@
         <v>50</v>
       </c>
       <c r="M110">
-        <f>(F110)*(L110-G110)</f>
+        <f t="shared" si="1"/>
         <v>338.4</v>
       </c>
       <c r="N110" t="s">
@@ -7493,7 +7575,7 @@
         <v>50</v>
       </c>
       <c r="M111">
-        <f>(F111)*(L111-G111)</f>
+        <f t="shared" si="1"/>
         <v>163.80000000000001</v>
       </c>
       <c r="N111" t="s">
@@ -7541,7 +7623,7 @@
         <v>50</v>
       </c>
       <c r="M112">
-        <f>(F112)*(L112-G112)</f>
+        <f t="shared" si="1"/>
         <v>226.8</v>
       </c>
       <c r="N112" t="s">
@@ -7589,7 +7671,7 @@
         <v>50</v>
       </c>
       <c r="M113">
-        <f>(F113)*(L113-G113)</f>
+        <f t="shared" si="1"/>
         <v>228.6</v>
       </c>
       <c r="N113" t="s">
@@ -7637,7 +7719,7 @@
         <v>50</v>
       </c>
       <c r="M114">
-        <f>(F114)*(L114-G114)</f>
+        <f t="shared" si="1"/>
         <v>1170</v>
       </c>
       <c r="N114" t="s">
@@ -7685,7 +7767,7 @@
         <v>50</v>
       </c>
       <c r="M115">
-        <f>(F115)*(L115-G115)</f>
+        <f t="shared" si="1"/>
         <v>151.19999999999999</v>
       </c>
       <c r="N115" t="s">
@@ -7733,7 +7815,7 @@
         <v>50</v>
       </c>
       <c r="M116">
-        <f>(F116)*(L116-G116)</f>
+        <f t="shared" si="1"/>
         <v>127.8</v>
       </c>
       <c r="N116" t="s">
@@ -7781,7 +7863,7 @@
         <v>50</v>
       </c>
       <c r="M117">
-        <f>(F117)*(L117-G117)</f>
+        <f t="shared" si="1"/>
         <v>273.60000000000002</v>
       </c>
       <c r="N117" t="s">
@@ -7829,7 +7911,7 @@
         <v>50</v>
       </c>
       <c r="M118">
-        <f>(F118)*(L118-G118)</f>
+        <f t="shared" si="1"/>
         <v>255.6</v>
       </c>
       <c r="N118" t="s">
@@ -7877,7 +7959,7 @@
         <v>50</v>
       </c>
       <c r="M119">
-        <f>(F119)*(L119-G119)</f>
+        <f t="shared" si="1"/>
         <v>127.35000000000001</v>
       </c>
       <c r="N119" t="s">
@@ -7925,7 +8007,7 @@
         <v>50</v>
       </c>
       <c r="M120">
-        <f>(F120)*(L120-G120)</f>
+        <f t="shared" si="1"/>
         <v>64.8</v>
       </c>
       <c r="N120" t="s">
@@ -7973,7 +8055,7 @@
         <v>50</v>
       </c>
       <c r="M121">
-        <f>(F121)*(L121-G121)</f>
+        <f t="shared" si="1"/>
         <v>230.4</v>
       </c>
       <c r="N121" t="s">
@@ -8021,7 +8103,7 @@
         <v>50</v>
       </c>
       <c r="M122">
-        <f>(F122)*(L122-G122)</f>
+        <f t="shared" si="1"/>
         <v>152.1</v>
       </c>
       <c r="N122" t="s">
@@ -8069,7 +8151,7 @@
         <v>50</v>
       </c>
       <c r="M123" t="e">
-        <f>(F123)*(L123-G123)</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="N123" t="s">
@@ -8117,7 +8199,7 @@
         <v>50</v>
       </c>
       <c r="M124">
-        <f>(F124)*(L124-G124)</f>
+        <f t="shared" si="1"/>
         <v>226.8</v>
       </c>
       <c r="N124" t="s">
@@ -8165,7 +8247,7 @@
         <v>50</v>
       </c>
       <c r="M125">
-        <f>(F125)*(L125-G125)</f>
+        <f t="shared" si="1"/>
         <v>144.9</v>
       </c>
       <c r="N125" t="s">
@@ -8213,7 +8295,7 @@
         <v>50</v>
       </c>
       <c r="M126">
-        <f>(F126)*(L126-G126)</f>
+        <f t="shared" si="1"/>
         <v>121.05</v>
       </c>
       <c r="N126" t="s">
@@ -8261,7 +8343,7 @@
         <v>50</v>
       </c>
       <c r="M127">
-        <f>(F127)*(L127-G127)</f>
+        <f t="shared" si="1"/>
         <v>121.05</v>
       </c>
       <c r="N127" t="s">
@@ -8309,7 +8391,7 @@
         <v>50</v>
       </c>
       <c r="M128">
-        <f>(F128)*(L128-G128)</f>
+        <f t="shared" si="1"/>
         <v>166.95</v>
       </c>
       <c r="N128" t="s">
@@ -8357,7 +8439,7 @@
         <v>50</v>
       </c>
       <c r="M129">
-        <f>(F129)*(L129-G129)</f>
+        <f t="shared" si="1"/>
         <v>119.7</v>
       </c>
       <c r="N129" t="s">
@@ -8405,7 +8487,7 @@
         <v>50</v>
       </c>
       <c r="M130">
-        <f>(F130)*(L130-G130)</f>
+        <f t="shared" ref="M130:M193" si="2">(F130)*(L130-G130)</f>
         <v>153.45000000000002</v>
       </c>
       <c r="N130" t="s">
@@ -8453,7 +8535,7 @@
         <v>50</v>
       </c>
       <c r="M131">
-        <f>(F131)*(L131-G131)</f>
+        <f t="shared" si="2"/>
         <v>116.55</v>
       </c>
       <c r="N131" t="s">
@@ -8501,7 +8583,7 @@
         <v>50</v>
       </c>
       <c r="M132">
-        <f>(F132)*(L132-G132)</f>
+        <f t="shared" si="2"/>
         <v>237.60000000000002</v>
       </c>
       <c r="N132" t="s">
@@ -8549,7 +8631,7 @@
         <v>50</v>
       </c>
       <c r="M133">
-        <f>(F133)*(L133-G133)</f>
+        <f t="shared" si="2"/>
         <v>92.249999999999986</v>
       </c>
       <c r="N133" t="s">
@@ -8597,7 +8679,7 @@
         <v>50</v>
       </c>
       <c r="M134">
-        <f>(F134)*(L134-G134)</f>
+        <f t="shared" si="2"/>
         <v>155.69999999999999</v>
       </c>
       <c r="N134" t="s">
@@ -8645,7 +8727,7 @@
         <v>50</v>
       </c>
       <c r="M135">
-        <f>(F135)*(L135-G135)</f>
+        <f t="shared" si="2"/>
         <v>196.20000000000002</v>
       </c>
       <c r="N135" t="s">
@@ -8693,7 +8775,7 @@
         <v>50</v>
       </c>
       <c r="M136">
-        <f>(F136)*(L136-G136)</f>
+        <f t="shared" si="2"/>
         <v>697.5</v>
       </c>
       <c r="N136" t="s">
@@ -8741,7 +8823,7 @@
         <v>50</v>
       </c>
       <c r="M137">
-        <f>(F137)*(L137-G137)</f>
+        <f t="shared" si="2"/>
         <v>78.75</v>
       </c>
       <c r="N137" t="s">
@@ -8789,7 +8871,7 @@
         <v>50</v>
       </c>
       <c r="M138">
-        <f>(F138)*(L138-G138)</f>
+        <f t="shared" si="2"/>
         <v>219.6</v>
       </c>
       <c r="N138" t="s">
@@ -8837,7 +8919,7 @@
         <v>50</v>
       </c>
       <c r="M139">
-        <f>(F139)*(L139-G139)</f>
+        <f t="shared" si="2"/>
         <v>486.00000000000006</v>
       </c>
       <c r="N139" t="s">
@@ -8885,7 +8967,7 @@
         <v>50</v>
       </c>
       <c r="M140">
-        <f>(F140)*(L140-G140)</f>
+        <f t="shared" si="2"/>
         <v>223.2</v>
       </c>
       <c r="N140" t="s">
@@ -8933,7 +9015,7 @@
         <v>50</v>
       </c>
       <c r="M141">
-        <f>(F141)*(L141-G141)</f>
+        <f t="shared" si="2"/>
         <v>342</v>
       </c>
       <c r="N141" t="s">
@@ -8981,7 +9063,7 @@
         <v>50</v>
       </c>
       <c r="M142">
-        <f>(F142)*(L142-G142)</f>
+        <f t="shared" si="2"/>
         <v>372.59999999999997</v>
       </c>
       <c r="N142" t="s">
@@ -9029,7 +9111,7 @@
         <v>50</v>
       </c>
       <c r="M143">
-        <f>(F143)*(L143-G143)</f>
+        <f t="shared" si="2"/>
         <v>293.39999999999998</v>
       </c>
       <c r="N143" t="s">
@@ -9077,7 +9159,7 @@
         <v>50</v>
       </c>
       <c r="M144">
-        <f>(F144)*(L144-G144)</f>
+        <f t="shared" si="2"/>
         <v>177.3</v>
       </c>
       <c r="N144" t="s">
@@ -9125,7 +9207,7 @@
         <v>50</v>
       </c>
       <c r="M145">
-        <f>(F145)*(L145-G145)</f>
+        <f t="shared" si="2"/>
         <v>324</v>
       </c>
       <c r="N145" t="s">
@@ -9173,7 +9255,7 @@
         <v>50</v>
       </c>
       <c r="M146">
-        <f>(F146)*(L146-G146)</f>
+        <f t="shared" si="2"/>
         <v>325.8</v>
       </c>
       <c r="N146" t="s">
@@ -9221,7 +9303,7 @@
         <v>50</v>
       </c>
       <c r="M147">
-        <f>(F147)*(L147-G147)</f>
+        <f t="shared" si="2"/>
         <v>189</v>
       </c>
       <c r="N147" t="s">
@@ -9269,7 +9351,7 @@
         <v>50</v>
       </c>
       <c r="M148">
-        <f>(F148)*(L148-G148)</f>
+        <f t="shared" si="2"/>
         <v>110.7</v>
       </c>
       <c r="N148" t="s">
@@ -9317,7 +9399,7 @@
         <v>50</v>
       </c>
       <c r="M149">
-        <f>(F149)*(L149-G149)</f>
+        <f t="shared" si="2"/>
         <v>129.6</v>
       </c>
       <c r="N149" t="s">
@@ -9365,7 +9447,7 @@
         <v>50</v>
       </c>
       <c r="M150">
-        <f>(F150)*(L150-G150)</f>
+        <f t="shared" si="2"/>
         <v>189</v>
       </c>
       <c r="N150" t="s">
@@ -9413,7 +9495,7 @@
         <v>50</v>
       </c>
       <c r="M151">
-        <f>(F151)*(L151-G151)</f>
+        <f t="shared" si="2"/>
         <v>248.39999999999998</v>
       </c>
       <c r="N151" t="s">
@@ -9461,7 +9543,7 @@
         <v>50</v>
       </c>
       <c r="M152">
-        <f>(F152)*(L152-G152)</f>
+        <f t="shared" si="2"/>
         <v>383.4</v>
       </c>
       <c r="N152" t="s">
@@ -9509,7 +9591,7 @@
         <v>50</v>
       </c>
       <c r="M153">
-        <f>(F153)*(L153-G153)</f>
+        <f t="shared" si="2"/>
         <v>458.99999999999994</v>
       </c>
       <c r="N153" t="s">
@@ -9557,7 +9639,7 @@
         <v>50</v>
       </c>
       <c r="M154">
-        <f>(F154)*(L154-G154)</f>
+        <f t="shared" si="2"/>
         <v>458.99999999999994</v>
       </c>
       <c r="N154" t="s">
@@ -9605,7 +9687,7 @@
         <v>50</v>
       </c>
       <c r="M155">
-        <f>(F155)*(L155-G155)</f>
+        <f t="shared" si="2"/>
         <v>206.99999999999997</v>
       </c>
       <c r="N155" t="s">
@@ -9653,7 +9735,7 @@
         <v>50</v>
       </c>
       <c r="M156">
-        <f>(F156)*(L156-G156)</f>
+        <f t="shared" si="2"/>
         <v>295.2</v>
       </c>
       <c r="N156" t="s">
@@ -9701,7 +9783,7 @@
         <v>50</v>
       </c>
       <c r="M157">
-        <f>(F157)*(L157-G157)</f>
+        <f t="shared" si="2"/>
         <v>419.40000000000003</v>
       </c>
       <c r="N157" t="s">
@@ -9749,7 +9831,7 @@
         <v>50</v>
       </c>
       <c r="M158">
-        <f>(F158)*(L158-G158)</f>
+        <f t="shared" si="2"/>
         <v>136.35</v>
       </c>
       <c r="N158" t="s">
@@ -9797,7 +9879,7 @@
         <v>50</v>
       </c>
       <c r="M159">
-        <f>(F159)*(L159-G159)</f>
+        <f t="shared" si="2"/>
         <v>154.80000000000001</v>
       </c>
       <c r="N159" t="s">
@@ -9845,7 +9927,7 @@
         <v>50</v>
       </c>
       <c r="M160">
-        <f>(F160)*(L160-G160)</f>
+        <f t="shared" si="2"/>
         <v>94.5</v>
       </c>
       <c r="N160" t="s">
@@ -9893,7 +9975,7 @@
         <v>50</v>
       </c>
       <c r="M161">
-        <f>(F161)*(L161-G161)</f>
+        <f t="shared" si="2"/>
         <v>108.45</v>
       </c>
       <c r="N161" t="s">
@@ -9929,7 +10011,7 @@
         <v>50</v>
       </c>
       <c r="M162" t="e">
-        <f>(F162)*(L162-G162)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N162" t="s">
@@ -9968,7 +10050,7 @@
         <v>50</v>
       </c>
       <c r="M163" t="e">
-        <f>(F163)*(L163-G163)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N163" t="s">
@@ -10007,7 +10089,7 @@
         <v>50</v>
       </c>
       <c r="M164" t="e">
-        <f>(F164)*(L164-G164)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N164" t="s">
@@ -10046,7 +10128,7 @@
         <v>50</v>
       </c>
       <c r="M165" t="e">
-        <f>(F165)*(L165-G165)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N165" t="s">
@@ -10097,7 +10179,7 @@
         <v>30</v>
       </c>
       <c r="M166">
-        <f>(F166)*(L166-G166)</f>
+        <f t="shared" si="2"/>
         <v>113.99999999999999</v>
       </c>
       <c r="N166" t="s">
@@ -10145,7 +10227,7 @@
         <v>30</v>
       </c>
       <c r="M167">
-        <f>(F167)*(L167-G167)</f>
+        <f t="shared" si="2"/>
         <v>247.00000000000003</v>
       </c>
       <c r="N167" t="s">
@@ -10193,7 +10275,7 @@
         <v>30</v>
       </c>
       <c r="M168">
-        <f>(F168)*(L168-G168)</f>
+        <f t="shared" si="2"/>
         <v>38.5</v>
       </c>
       <c r="N168" t="s">
@@ -10241,7 +10323,7 @@
         <v>30</v>
       </c>
       <c r="M169">
-        <f>(F169)*(L169-G169)</f>
+        <f t="shared" si="2"/>
         <v>352.5</v>
       </c>
       <c r="N169" t="s">
@@ -10289,7 +10371,7 @@
         <v>14</v>
       </c>
       <c r="M170" t="e">
-        <f>(F170)*(L170-G170)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N170" t="s">
@@ -10337,7 +10419,7 @@
         <v>14</v>
       </c>
       <c r="M171">
-        <f>(F171)*(L171-G171)</f>
+        <f t="shared" si="2"/>
         <v>234</v>
       </c>
       <c r="N171" t="s">
@@ -10394,7 +10476,7 @@
         <v>14</v>
       </c>
       <c r="M172" t="e">
-        <f>(F172)*(L172-G172)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N172" t="s">
@@ -10442,7 +10524,7 @@
         <v>14</v>
       </c>
       <c r="M173" t="e">
-        <f>(F173)*(L173-G173)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N173" t="s">
@@ -10490,7 +10572,7 @@
         <v>14</v>
       </c>
       <c r="M174">
-        <f>(F174)*(L174-G174)</f>
+        <f t="shared" si="2"/>
         <v>224.9</v>
       </c>
       <c r="N174" t="s">
@@ -10547,7 +10629,7 @@
         <v>14</v>
       </c>
       <c r="M175">
-        <f>(F175)*(L175-G175)</f>
+        <f t="shared" si="2"/>
         <v>387.40000000000003</v>
       </c>
       <c r="N175" t="s">
@@ -10604,7 +10686,7 @@
         <v>14</v>
       </c>
       <c r="M176" t="e">
-        <f>(F176)*(L176-G176)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N176" t="s">
@@ -10652,7 +10734,7 @@
         <v>14</v>
       </c>
       <c r="M177">
-        <f>(F177)*(L177-G177)</f>
+        <f t="shared" si="2"/>
         <v>68.64</v>
       </c>
       <c r="N177" t="s">
@@ -10709,7 +10791,7 @@
         <v>14</v>
       </c>
       <c r="M178">
-        <f>(F178)*(L178-G178)</f>
+        <f t="shared" si="2"/>
         <v>108.94000000000001</v>
       </c>
       <c r="N178" t="s">
@@ -10766,7 +10848,7 @@
         <v>14</v>
       </c>
       <c r="M179" t="e">
-        <f>(F179)*(L179-G179)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N179" t="s">
@@ -10814,7 +10896,7 @@
         <v>14</v>
       </c>
       <c r="M180">
-        <f>(F180)*(L180-G180)</f>
+        <f t="shared" si="2"/>
         <v>90.22</v>
       </c>
       <c r="N180" t="s">
@@ -10871,7 +10953,7 @@
         <v>14</v>
       </c>
       <c r="M181">
-        <f>(F181)*(L181-G181)</f>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="N181" t="s">
@@ -10928,7 +11010,7 @@
         <v>14</v>
       </c>
       <c r="M182">
-        <f>(F182)*(L182-G182)</f>
+        <f t="shared" si="2"/>
         <v>94.64</v>
       </c>
       <c r="N182" t="s">
@@ -10985,7 +11067,7 @@
         <v>14</v>
       </c>
       <c r="M183" t="e">
-        <f>(F183)*(L183-G183)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N183" t="s">
@@ -11033,7 +11115,7 @@
         <v>14</v>
       </c>
       <c r="M184" t="e">
-        <f>(F184)*(L184-G184)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N184" t="s">
@@ -11081,7 +11163,7 @@
         <v>14</v>
       </c>
       <c r="M185">
-        <f>(F185)*(L185-G185)</f>
+        <f t="shared" si="2"/>
         <v>93.600000000000009</v>
       </c>
       <c r="N185" t="s">
@@ -11138,7 +11220,7 @@
         <v>14</v>
       </c>
       <c r="M186">
-        <f>(F186)*(L186-G186)</f>
+        <f t="shared" si="2"/>
         <v>206.70000000000002</v>
       </c>
       <c r="N186" t="s">
@@ -11195,7 +11277,7 @@
         <v>14</v>
       </c>
       <c r="M187" t="e">
-        <f>(F187)*(L187-G187)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N187" t="s">
@@ -11243,7 +11325,7 @@
         <v>14</v>
       </c>
       <c r="M188" t="e">
-        <f>(F188)*(L188-G188)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N188" t="s">
@@ -11291,7 +11373,7 @@
         <v>14</v>
       </c>
       <c r="M189" t="e">
-        <f>(F189)*(L189-G189)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N189" t="s">
@@ -11339,7 +11421,7 @@
         <v>14</v>
       </c>
       <c r="M190" t="e">
-        <f>(F190)*(L190-G190)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N190" t="s">
@@ -11387,7 +11469,7 @@
         <v>14</v>
       </c>
       <c r="M191" t="e">
-        <f>(F191)*(L191-G191)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N191" t="s">
@@ -11435,7 +11517,7 @@
         <v>14</v>
       </c>
       <c r="M192">
-        <f>(F192)*(L192-G192)</f>
+        <f t="shared" si="2"/>
         <v>62.4</v>
       </c>
       <c r="N192" t="s">
@@ -11492,7 +11574,7 @@
         <v>14</v>
       </c>
       <c r="M193" t="e">
-        <f>(F193)*(L193-G193)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N193" t="s">
@@ -11540,7 +11622,7 @@
         <v>14</v>
       </c>
       <c r="M194" t="e">
-        <f>(F194)*(L194-G194)</f>
+        <f t="shared" ref="M194:M257" si="3">(F194)*(L194-G194)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N194" t="s">
@@ -11588,7 +11670,7 @@
         <v>14</v>
       </c>
       <c r="M195">
-        <f>(F195)*(L195-G195)</f>
+        <f t="shared" si="3"/>
         <v>89.18</v>
       </c>
       <c r="N195" t="s">
@@ -11645,7 +11727,7 @@
         <v>14</v>
       </c>
       <c r="M196" t="e">
-        <f>(F196)*(L196-G196)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N196" t="s">
@@ -11693,7 +11775,7 @@
         <v>14</v>
       </c>
       <c r="M197" t="e">
-        <f>(F197)*(L197-G197)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N197" t="s">
@@ -11741,7 +11823,7 @@
         <v>14</v>
       </c>
       <c r="M198">
-        <f>(F198)*(L198-G198)</f>
+        <f t="shared" si="3"/>
         <v>118.55999999999999</v>
       </c>
       <c r="N198" t="s">
@@ -11798,7 +11880,7 @@
         <v>14</v>
       </c>
       <c r="M199">
-        <f>(F199)*(L199-G199)</f>
+        <f t="shared" si="3"/>
         <v>71.759999999999991</v>
       </c>
       <c r="N199" t="s">
@@ -11855,7 +11937,7 @@
         <v>14</v>
       </c>
       <c r="M200">
-        <f>(F200)*(L200-G200)</f>
+        <f t="shared" si="3"/>
         <v>126.62</v>
       </c>
       <c r="N200" t="s">
@@ -11912,7 +11994,7 @@
         <v>14</v>
       </c>
       <c r="M201" t="e">
-        <f>(F201)*(L201-G201)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N201" t="s">
@@ -11960,7 +12042,7 @@
         <v>14</v>
       </c>
       <c r="M202" t="e">
-        <f>(F202)*(L202-G202)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N202" t="s">
@@ -12008,7 +12090,7 @@
         <v>14</v>
       </c>
       <c r="M203" t="e">
-        <f>(F203)*(L203-G203)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N203" t="s">
@@ -12056,7 +12138,7 @@
         <v>14</v>
       </c>
       <c r="M204" t="e">
-        <f>(F204)*(L204-G204)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N204" t="s">
@@ -12104,7 +12186,7 @@
         <v>14</v>
       </c>
       <c r="M205" t="e">
-        <f>(F205)*(L205-G205)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N205" t="s">
@@ -12152,7 +12234,7 @@
         <v>14</v>
       </c>
       <c r="M206" t="e">
-        <f>(F206)*(L206-G206)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N206" t="s">
@@ -12200,7 +12282,7 @@
         <v>14</v>
       </c>
       <c r="M207" t="e">
-        <f>(F207)*(L207-G207)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N207" t="s">
@@ -12248,7 +12330,7 @@
         <v>14</v>
       </c>
       <c r="M208" t="e">
-        <f>(F208)*(L208-G208)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N208" t="s">
@@ -12296,7 +12378,7 @@
         <v>14</v>
       </c>
       <c r="M209" t="e">
-        <f>(F209)*(L209-G209)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N209" t="s">
@@ -12344,7 +12426,7 @@
         <v>10</v>
       </c>
       <c r="M210">
-        <f>(F210)*(L210-G210)</f>
+        <f t="shared" si="3"/>
         <v>6.2</v>
       </c>
       <c r="N210" t="s">
@@ -12392,7 +12474,7 @@
         <v>10</v>
       </c>
       <c r="M211">
-        <f>(F211)*(L211-G211)</f>
+        <f t="shared" si="3"/>
         <v>16.5</v>
       </c>
       <c r="N211" t="s">
@@ -12440,7 +12522,7 @@
         <v>10</v>
       </c>
       <c r="M212">
-        <f>(F212)*(L212-G212)</f>
+        <f t="shared" si="3"/>
         <v>7.65</v>
       </c>
       <c r="N212" t="s">
@@ -12488,7 +12570,7 @@
         <v>10</v>
       </c>
       <c r="M213" t="e">
-        <f>(F213)*(L213-G213)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N213" t="s">
@@ -12536,7 +12618,7 @@
         <v>10</v>
       </c>
       <c r="M214" t="e">
-        <f>(F214)*(L214-G214)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N214" t="s">
@@ -12584,7 +12666,7 @@
         <v>10</v>
       </c>
       <c r="M215">
-        <f>(F215)*(L215-G215)</f>
+        <f t="shared" si="3"/>
         <v>14.2</v>
       </c>
       <c r="N215" t="s">
@@ -12632,7 +12714,7 @@
         <v>10</v>
       </c>
       <c r="M216">
-        <f>(F216)*(L216-G216)</f>
+        <f t="shared" si="3"/>
         <v>19.099999999999998</v>
       </c>
       <c r="N216" t="s">
@@ -12680,7 +12762,7 @@
         <v>10</v>
       </c>
       <c r="M217" t="e">
-        <f>(F217)*(L217-G217)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N217" t="s">
@@ -12728,7 +12810,7 @@
         <v>10</v>
       </c>
       <c r="M218">
-        <f>(F218)*(L218-G218)</f>
+        <f t="shared" si="3"/>
         <v>15.600000000000001</v>
       </c>
       <c r="N218" t="s">
@@ -12776,7 +12858,7 @@
         <v>10</v>
       </c>
       <c r="M219">
-        <f>(F219)*(L219-G219)</f>
+        <f t="shared" si="3"/>
         <v>9.3999999999999986</v>
       </c>
       <c r="N219" t="s">
@@ -12824,7 +12906,7 @@
         <v>10</v>
       </c>
       <c r="M220">
-        <f>(F220)*(L220-G220)</f>
+        <f t="shared" si="3"/>
         <v>15.75</v>
       </c>
       <c r="N220" t="s">
@@ -12872,7 +12954,7 @@
         <v>10</v>
       </c>
       <c r="M221">
-        <f>(F221)*(L221-G221)</f>
+        <f t="shared" si="3"/>
         <v>24.4</v>
       </c>
       <c r="N221" t="s">
@@ -12920,7 +13002,7 @@
         <v>10</v>
       </c>
       <c r="M222">
-        <f>(F222)*(L222-G222)</f>
+        <f t="shared" si="3"/>
         <v>13.200000000000001</v>
       </c>
       <c r="N222" t="s">
@@ -12968,7 +13050,7 @@
         <v>10</v>
       </c>
       <c r="M223" t="e">
-        <f>(F223)*(L223-G223)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N223" t="s">
@@ -13016,7 +13098,7 @@
         <v>10</v>
       </c>
       <c r="M224" t="e">
-        <f>(F224)*(L224-G224)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N224" t="s">
@@ -13064,7 +13146,7 @@
         <v>10</v>
       </c>
       <c r="M225">
-        <f>(F225)*(L225-G225)</f>
+        <f t="shared" si="3"/>
         <v>21.8</v>
       </c>
       <c r="N225" t="s">
@@ -13112,7 +13194,7 @@
         <v>10</v>
       </c>
       <c r="M226" t="e">
-        <f>(F226)*(L226-G226)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N226" t="s">
@@ -13160,7 +13242,7 @@
         <v>10</v>
       </c>
       <c r="M227">
-        <f>(F227)*(L227-G227)</f>
+        <f t="shared" si="3"/>
         <v>17.549999999999997</v>
       </c>
       <c r="N227" t="s">
@@ -13208,7 +13290,7 @@
         <v>10</v>
       </c>
       <c r="M228" t="e">
-        <f>(F228)*(L228-G228)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N228" t="s">
@@ -13256,7 +13338,7 @@
         <v>10</v>
       </c>
       <c r="M229">
-        <f>(F229)*(L229-G229)</f>
+        <f t="shared" si="3"/>
         <v>4.6000000000000005</v>
       </c>
       <c r="N229" t="s">
@@ -13304,7 +13386,7 @@
         <v>10</v>
       </c>
       <c r="M230">
-        <f>(F230)*(L230-G230)</f>
+        <f t="shared" si="3"/>
         <v>14.7</v>
       </c>
       <c r="N230" t="s">
@@ -13352,7 +13434,7 @@
         <v>10</v>
       </c>
       <c r="M231">
-        <f>(F231)*(L231-G231)</f>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="N231" t="s">
@@ -13400,7 +13482,7 @@
         <v>10</v>
       </c>
       <c r="M232">
-        <f>(F232)*(L232-G232)</f>
+        <f t="shared" si="3"/>
         <v>32.400000000000006</v>
       </c>
       <c r="N232" t="s">
@@ -13448,7 +13530,7 @@
         <v>10</v>
       </c>
       <c r="M233">
-        <f>(F233)*(L233-G233)</f>
+        <f t="shared" si="3"/>
         <v>7.75</v>
       </c>
       <c r="N233" t="s">
@@ -13496,7 +13578,7 @@
         <v>12</v>
       </c>
       <c r="M234">
-        <f>(F234)*(L234-G234)</f>
+        <f t="shared" si="3"/>
         <v>314.60000000000002</v>
       </c>
       <c r="N234" t="s">
@@ -13638,7 +13720,7 @@
         <v>14</v>
       </c>
       <c r="M238">
-        <f>(F238)*(L238-G238)</f>
+        <f t="shared" ref="M238:M245" si="4">(F238)*(L238-G238)</f>
         <v>522.6</v>
       </c>
       <c r="N238" t="s">
@@ -13686,7 +13768,7 @@
         <v>14</v>
       </c>
       <c r="M239">
-        <f>(F239)*(L239-G239)</f>
+        <f t="shared" si="4"/>
         <v>852.8</v>
       </c>
       <c r="N239" t="s">
@@ -13734,7 +13816,7 @@
         <v>14</v>
       </c>
       <c r="M240">
-        <f>(F240)*(L240-G240)</f>
+        <f t="shared" si="4"/>
         <v>270.40000000000003</v>
       </c>
       <c r="N240" t="s">
@@ -13782,7 +13864,7 @@
         <v>14</v>
       </c>
       <c r="M241">
-        <f>(F241)*(L241-G241)</f>
+        <f t="shared" si="4"/>
         <v>483.6</v>
       </c>
       <c r="N241" t="s">
@@ -13830,7 +13912,7 @@
         <v>14</v>
       </c>
       <c r="M242">
-        <f>(F242)*(L242-G242)</f>
+        <f t="shared" si="4"/>
         <v>772.19999999999993</v>
       </c>
       <c r="N242" t="s">
@@ -13878,7 +13960,7 @@
         <v>14</v>
       </c>
       <c r="M243">
-        <f>(F243)*(L243-G243)</f>
+        <f t="shared" si="4"/>
         <v>231.4</v>
       </c>
       <c r="N243" t="s">
@@ -13926,7 +14008,7 @@
         <v>14</v>
       </c>
       <c r="M244" t="e">
-        <f>(F244)*(L244-G244)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N244" t="s">
@@ -13974,7 +14056,7 @@
         <v>14</v>
       </c>
       <c r="M245" t="e">
-        <f>(F245)*(L245-G245)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N245" t="s">
@@ -14079,7 +14161,7 @@
         <v>20</v>
       </c>
       <c r="M249" t="e">
-        <f>(F249)*(L249-G249)</f>
+        <f t="shared" ref="M249:M280" si="5">(F249)*(L249-G249)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N249" t="s">
@@ -14115,7 +14197,7 @@
         <v>20</v>
       </c>
       <c r="M250" t="e">
-        <f>(F250)*(L250-G250)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N250" t="s">
@@ -14151,7 +14233,7 @@
         <v>20</v>
       </c>
       <c r="M251" t="e">
-        <f>(F251)*(L251-G251)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N251" t="s">
@@ -14187,7 +14269,7 @@
         <v>20</v>
       </c>
       <c r="M252" t="e">
-        <f>(F252)*(L252-G252)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N252" t="s">
@@ -14223,7 +14305,7 @@
         <v>20</v>
       </c>
       <c r="M253" t="e">
-        <f>(F253)*(L253-G253)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N253" t="s">
@@ -14259,7 +14341,7 @@
         <v>20</v>
       </c>
       <c r="M254" t="e">
-        <f>(F254)*(L254-G254)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N254" t="s">
@@ -14298,7 +14380,7 @@
         <v>14</v>
       </c>
       <c r="M255" t="e">
-        <f>(F255)*(L255-G255)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N255" t="s">
@@ -14337,7 +14419,7 @@
         <v>14</v>
       </c>
       <c r="M256" t="e">
-        <f>(F256)*(L256-G256)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N256" t="s">
@@ -14376,7 +14458,7 @@
         <v>14</v>
       </c>
       <c r="M257" t="e">
-        <f>(F257)*(L257-G257)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N257" t="s">
@@ -14415,7 +14497,7 @@
         <v>14</v>
       </c>
       <c r="M258" t="e">
-        <f>(F258)*(L258-G258)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N258" t="s">
@@ -14454,7 +14536,7 @@
         <v>14</v>
       </c>
       <c r="M259" t="e">
-        <f>(F259)*(L259-G259)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N259" t="s">
@@ -14493,7 +14575,7 @@
         <v>14</v>
       </c>
       <c r="M260" t="e">
-        <f>(F260)*(L260-G260)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N260" t="s">
@@ -14532,7 +14614,7 @@
         <v>14</v>
       </c>
       <c r="M261" t="e">
-        <f>(F261)*(L261-G261)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N261" t="s">
@@ -14568,7 +14650,7 @@
         <v>14</v>
       </c>
       <c r="M262">
-        <f>(F262)*(L262-G262)</f>
+        <f t="shared" si="5"/>
         <v>91</v>
       </c>
       <c r="N262" t="s">
@@ -14613,7 +14695,7 @@
         <v>14</v>
       </c>
       <c r="M263">
-        <f>(F263)*(L263-G263)</f>
+        <f t="shared" si="5"/>
         <v>182</v>
       </c>
       <c r="N263" t="s">
@@ -14661,7 +14743,7 @@
         <v>14</v>
       </c>
       <c r="M264">
-        <f>(F264)*(L264-G264)</f>
+        <f t="shared" si="5"/>
         <v>59.8</v>
       </c>
       <c r="N264" t="s">
@@ -14703,7 +14785,7 @@
         <v>14</v>
       </c>
       <c r="M265" t="e">
-        <f>(F265)*(L265-G265)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N265" t="s">
@@ -14742,7 +14824,7 @@
         <v>14</v>
       </c>
       <c r="M266" t="e">
-        <f>(F266)*(L266-G266)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N266" t="s">
@@ -14781,7 +14863,7 @@
         <v>14</v>
       </c>
       <c r="M267" t="e">
-        <f>(F267)*(L267-G267)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N267" t="s">
@@ -14820,7 +14902,7 @@
         <v>14</v>
       </c>
       <c r="M268" t="e">
-        <f>(F268)*(L268-G268)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N268" t="s">
@@ -14859,7 +14941,7 @@
         <v>14</v>
       </c>
       <c r="M269" t="e">
-        <f>(F269)*(L269-G269)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N269" t="s">
@@ -14898,7 +14980,7 @@
         <v>14</v>
       </c>
       <c r="M270" t="e">
-        <f>(F270)*(L270-G270)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N270" t="s">
@@ -14937,7 +15019,7 @@
         <v>14</v>
       </c>
       <c r="M271" t="e">
-        <f>(F271)*(L271-G271)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N271" t="s">
@@ -14976,7 +15058,7 @@
         <v>14</v>
       </c>
       <c r="M272" t="e">
-        <f>(F272)*(L272-G272)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N272" t="s">
@@ -15015,7 +15097,7 @@
         <v>14</v>
       </c>
       <c r="M273" t="e">
-        <f>(F273)*(L273-G273)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N273" t="s">
@@ -15054,7 +15136,7 @@
         <v>14</v>
       </c>
       <c r="M274" t="e">
-        <f>(F274)*(L274-G274)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N274" t="s">
@@ -15093,7 +15175,7 @@
         <v>14</v>
       </c>
       <c r="M275" t="e">
-        <f>(F275)*(L275-G275)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N275" t="s">
@@ -15132,7 +15214,7 @@
         <v>14</v>
       </c>
       <c r="M276" t="e">
-        <f>(F276)*(L276-G276)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N276" t="s">
@@ -15171,7 +15253,7 @@
         <v>14</v>
       </c>
       <c r="M277" t="e">
-        <f>(F277)*(L277-G277)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N277" t="s">
@@ -15210,7 +15292,7 @@
         <v>14</v>
       </c>
       <c r="M278" t="e">
-        <f>(F278)*(L278-G278)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N278" t="s">
@@ -15249,7 +15331,7 @@
         <v>14</v>
       </c>
       <c r="M279" t="e">
-        <f>(F279)*(L279-G279)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N279" t="s">
@@ -15288,7 +15370,7 @@
         <v>14</v>
       </c>
       <c r="M280" t="e">
-        <f>(F280)*(L280-G280)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N280" t="s">
@@ -15327,7 +15409,7 @@
         <v>14</v>
       </c>
       <c r="M281" t="e">
-        <f>(F281)*(L281-G281)</f>
+        <f t="shared" ref="M281:M312" si="6">(F281)*(L281-G281)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N281" t="s">
@@ -15366,7 +15448,7 @@
         <v>14</v>
       </c>
       <c r="M282" t="e">
-        <f>(F282)*(L282-G282)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N282" t="s">
@@ -15405,7 +15487,7 @@
         <v>14</v>
       </c>
       <c r="M283" t="e">
-        <f>(F283)*(L283-G283)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N283" t="s">
@@ -15444,7 +15526,7 @@
         <v>14</v>
       </c>
       <c r="M284" t="e">
-        <f>(F284)*(L284-G284)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N284" t="s">
@@ -15483,7 +15565,7 @@
         <v>14</v>
       </c>
       <c r="M285" t="e">
-        <f>(F285)*(L285-G285)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N285" t="s">
@@ -15522,7 +15604,7 @@
         <v>14</v>
       </c>
       <c r="M286" t="e">
-        <f>(F286)*(L286-G286)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N286" t="s">
@@ -15562,7 +15644,7 @@
         <v>14</v>
       </c>
       <c r="M287" t="e">
-        <f>(F287)*(L287-G287)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N287" t="s">
@@ -15602,7 +15684,7 @@
         <v>14</v>
       </c>
       <c r="M288" t="e">
-        <f>(F288)*(L288-G288)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N288" t="s">
@@ -15651,7 +15733,7 @@
         <v>10</v>
       </c>
       <c r="M289" t="e">
-        <f>(F289)*(L289-G289)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N289" t="s">
@@ -15703,7 +15785,7 @@
         <v>10</v>
       </c>
       <c r="M290" t="e">
-        <f>(F290)*(L290-G290)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N290" t="s">
@@ -15755,7 +15837,7 @@
         <v>10</v>
       </c>
       <c r="M291" t="e">
-        <f>(F291)*(L291-G291)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N291" t="s">
@@ -15807,7 +15889,7 @@
         <v>10</v>
       </c>
       <c r="M292" t="e">
-        <f>(F292)*(L292-G292)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N292" t="s">
@@ -15859,7 +15941,7 @@
         <v>10</v>
       </c>
       <c r="M293" t="e">
-        <f>(F293)*(L293-G293)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N293" t="s">
@@ -15911,7 +15993,7 @@
         <v>10</v>
       </c>
       <c r="M294" t="e">
-        <f>(F294)*(L294-G294)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N294" t="s">
@@ -15963,7 +16045,7 @@
         <v>10</v>
       </c>
       <c r="M295" t="e">
-        <f>(F295)*(L295-G295)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N295" t="s">
@@ -16015,7 +16097,7 @@
         <v>10</v>
       </c>
       <c r="M296" t="e">
-        <f>(F296)*(L296-G296)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N296" t="s">
@@ -16067,7 +16149,7 @@
         <v>10</v>
       </c>
       <c r="M297">
-        <f>(F297)*(L297-G297)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N297" t="s">
@@ -16118,7 +16200,7 @@
         <v>10</v>
       </c>
       <c r="M298" t="e">
-        <f>(F298)*(L298-G298)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N298" t="s">
@@ -16169,7 +16251,7 @@
         <v>10</v>
       </c>
       <c r="M299" t="e">
-        <f>(F299)*(L299-G299)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N299" t="s">
@@ -16220,7 +16302,7 @@
         <v>10</v>
       </c>
       <c r="M300" t="e">
-        <f>(F300)*(L300-G300)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N300" t="s">
@@ -16271,7 +16353,7 @@
         <v>10</v>
       </c>
       <c r="M301" t="e">
-        <f>(F301)*(L301-G301)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N301" t="s">
@@ -16322,7 +16404,7 @@
         <v>10</v>
       </c>
       <c r="M302" t="e">
-        <f>(F302)*(L302-G302)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N302" t="s">
@@ -16373,7 +16455,7 @@
         <v>10</v>
       </c>
       <c r="M303" t="e">
-        <f>(F303)*(L303-G303)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N303" t="s">
@@ -16424,7 +16506,7 @@
         <v>10</v>
       </c>
       <c r="M304">
-        <f>(F304)*(L304-G304)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N304" t="s">
@@ -16475,7 +16557,7 @@
         <v>10</v>
       </c>
       <c r="M305" t="e">
-        <f>(F305)*(L305-G305)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N305" t="s">
@@ -16526,7 +16608,7 @@
         <v>10</v>
       </c>
       <c r="M306">
-        <f>(F306)*(L306-G306)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N306" t="s">
@@ -16577,7 +16659,7 @@
         <v>10</v>
       </c>
       <c r="M307" t="e">
-        <f>(F307)*(L307-G307)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N307" t="s">
@@ -16628,7 +16710,7 @@
         <v>10</v>
       </c>
       <c r="M308">
-        <f>(F308)*(L308-G308)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N308" t="s">
@@ -16679,7 +16761,7 @@
         <v>10</v>
       </c>
       <c r="M309" t="e">
-        <f>(F309)*(L309-G309)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N309" t="s">
@@ -16730,7 +16812,7 @@
         <v>10</v>
       </c>
       <c r="M310" t="e">
-        <f>(F310)*(L310-G310)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N310" t="s">
@@ -16781,7 +16863,7 @@
         <v>10</v>
       </c>
       <c r="M311" t="e">
-        <f>(F311)*(L311-G311)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N311" t="s">
@@ -16832,7 +16914,7 @@
         <v>10</v>
       </c>
       <c r="M312" t="e">
-        <f>(F312)*(L312-G312)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N312" t="s">
@@ -16883,7 +16965,7 @@
         <v>14</v>
       </c>
       <c r="M313" t="e">
-        <f>(F313)*(L313-G313)</f>
+        <f t="shared" ref="M313:M344" si="7">(F313)*(L313-G313)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N313" t="s">
@@ -16932,7 +17014,7 @@
         <v>14</v>
       </c>
       <c r="M314">
-        <f>(F314)*(L314-G314)</f>
+        <f t="shared" si="7"/>
         <v>59.8</v>
       </c>
       <c r="N314" t="s">
@@ -16980,7 +17062,7 @@
         <v>14</v>
       </c>
       <c r="M315" t="e">
-        <f>(F315)*(L315-G315)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N315" t="s">
@@ -17029,7 +17111,7 @@
         <v>14</v>
       </c>
       <c r="M316">
-        <f>(F316)*(L316-G316)</f>
+        <f t="shared" si="7"/>
         <v>59.8</v>
       </c>
       <c r="N316" t="s">
@@ -17080,7 +17162,7 @@
         <v>14</v>
       </c>
       <c r="M317" t="e">
-        <f>(F317)*(L317-G317)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N317" t="s">
@@ -17131,7 +17213,7 @@
         <v>14</v>
       </c>
       <c r="M318" t="e">
-        <f>(F318)*(L318-G318)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N318" t="s">
@@ -17182,7 +17264,7 @@
         <v>14</v>
       </c>
       <c r="M319" t="e">
-        <f>(F319)*(L319-G319)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N319" t="s">
@@ -17233,7 +17315,7 @@
         <v>14</v>
       </c>
       <c r="M320" t="e">
-        <f>(F320)*(L320-G320)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N320" t="s">
@@ -17284,7 +17366,7 @@
         <v>14</v>
       </c>
       <c r="M321" t="e">
-        <f>(F321)*(L321-G321)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N321" t="s">
@@ -17335,7 +17417,7 @@
         <v>14</v>
       </c>
       <c r="M322" t="e">
-        <f>(F322)*(L322-G322)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N322" t="s">
@@ -17384,7 +17466,7 @@
         <v>14</v>
       </c>
       <c r="M323" t="e">
-        <f>(F323)*(L323-G323)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N323" t="s">
@@ -17433,7 +17515,7 @@
         <v>14</v>
       </c>
       <c r="M324" t="e">
-        <f>(F324)*(L324-G324)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N324" t="s">
@@ -17482,7 +17564,7 @@
         <v>14</v>
       </c>
       <c r="M325" t="e">
-        <f>(F325)*(L325-G325)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N325" t="s">
@@ -17531,7 +17613,7 @@
         <v>14</v>
       </c>
       <c r="M326" t="e">
-        <f>(F326)*(L326-G326)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N326" t="s">
@@ -17580,7 +17662,7 @@
         <v>14</v>
       </c>
       <c r="M327" t="e">
-        <f>(F327)*(L327-G327)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N327" t="s">
@@ -17631,7 +17713,7 @@
         <v>14</v>
       </c>
       <c r="M328" t="e">
-        <f>(F328)*(L328-G328)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N328" t="s">
@@ -17682,7 +17764,7 @@
         <v>14</v>
       </c>
       <c r="M329" t="e">
-        <f>(F329)*(L329-G329)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N329" t="s">
@@ -17733,7 +17815,7 @@
         <v>14</v>
       </c>
       <c r="M330" t="e">
-        <f>(F330)*(L330-G330)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N330" t="s">
@@ -17784,7 +17866,7 @@
         <v>14</v>
       </c>
       <c r="M331" t="e">
-        <f>(F331)*(L331-G331)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N331" t="s">
@@ -17835,7 +17917,7 @@
         <v>14</v>
       </c>
       <c r="M332" t="e">
-        <f>(F332)*(L332-G332)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N332" t="s">
@@ -17886,7 +17968,7 @@
         <v>15</v>
       </c>
       <c r="M333" s="2">
-        <f>(F333)*(L333-G333)</f>
+        <f t="shared" si="7"/>
         <v>107.76999999999998</v>
       </c>
       <c r="N333" t="s">
@@ -17940,7 +18022,7 @@
         <v>15</v>
       </c>
       <c r="M334" s="2">
-        <f>(F334)*(L334-G334)</f>
+        <f t="shared" si="7"/>
         <v>57.98</v>
       </c>
       <c r="N334" t="s">
@@ -17994,7 +18076,7 @@
         <v>15</v>
       </c>
       <c r="M335" s="2">
-        <f>(F335)*(L335-G335)</f>
+        <f t="shared" si="7"/>
         <v>265.2</v>
       </c>
       <c r="N335" t="s">
@@ -18048,7 +18130,7 @@
         <v>15</v>
       </c>
       <c r="M336" s="2">
-        <f>(F336)*(L336-G336)</f>
+        <f t="shared" si="7"/>
         <v>273</v>
       </c>
       <c r="N336" t="s">
@@ -18102,7 +18184,7 @@
         <v>15</v>
       </c>
       <c r="M337" s="2">
-        <f>(F337)*(L337-G337)</f>
+        <f t="shared" si="7"/>
         <v>427.7</v>
       </c>
       <c r="N337" t="s">
@@ -18156,7 +18238,7 @@
         <v>15</v>
       </c>
       <c r="M338" s="2" t="e">
-        <f>(F338)*(L338-G338)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N338" t="s">
@@ -18204,7 +18286,7 @@
         <v>15</v>
       </c>
       <c r="M339" s="2">
-        <f>(F339)*(L339-G339)</f>
+        <f t="shared" si="7"/>
         <v>451.1</v>
       </c>
       <c r="N339" t="s">
@@ -18258,7 +18340,7 @@
         <v>15</v>
       </c>
       <c r="M340" s="2">
-        <f>(F340)*(L340-G340)</f>
+        <f t="shared" si="7"/>
         <v>172.9</v>
       </c>
       <c r="N340" t="s">
@@ -18312,7 +18394,7 @@
         <v>15</v>
       </c>
       <c r="M341" s="2">
-        <f>(F341)*(L341-G341)</f>
+        <f t="shared" si="7"/>
         <v>378.3</v>
       </c>
       <c r="N341" t="s">
@@ -18366,7 +18448,7 @@
         <v>15</v>
       </c>
       <c r="M342" s="2">
-        <f>(F342)*(L342-G342)</f>
+        <f t="shared" si="7"/>
         <v>553.80000000000007</v>
       </c>
       <c r="N342" t="s">
@@ -18420,7 +18502,7 @@
         <v>15</v>
       </c>
       <c r="M343" s="2">
-        <f>(F343)*(L343-G343)</f>
+        <f t="shared" si="7"/>
         <v>495.3</v>
       </c>
       <c r="N343" t="s">
@@ -18474,7 +18556,7 @@
         <v>15</v>
       </c>
       <c r="M344" s="2">
-        <f>(F344)*(L344-G344)</f>
+        <f t="shared" si="7"/>
         <v>345.8</v>
       </c>
       <c r="N344" t="s">
@@ -18528,7 +18610,7 @@
         <v>15</v>
       </c>
       <c r="M345" s="2">
-        <f>(F345)*(L345-G345)</f>
+        <f t="shared" ref="M345:M376" si="8">(F345)*(L345-G345)</f>
         <v>663</v>
       </c>
       <c r="N345" t="s">
@@ -18582,7 +18664,7 @@
         <v>15</v>
       </c>
       <c r="M346" s="2">
-        <f>(F346)*(L346-G346)</f>
+        <f t="shared" si="8"/>
         <v>231.4</v>
       </c>
       <c r="N346" t="s">
@@ -18636,7 +18718,7 @@
         <v>15</v>
       </c>
       <c r="M347" s="2">
-        <f>(F347)*(L347-G347)</f>
+        <f t="shared" si="8"/>
         <v>936</v>
       </c>
       <c r="N347" t="s">
@@ -18690,7 +18772,7 @@
         <v>15</v>
       </c>
       <c r="M348" s="2">
-        <f>(F348)*(L348-G348)</f>
+        <f t="shared" si="8"/>
         <v>217.1</v>
       </c>
       <c r="N348" t="s">
@@ -18744,7 +18826,7 @@
         <v>15</v>
       </c>
       <c r="M349" s="2">
-        <f>(F349)*(L349-G349)</f>
+        <f t="shared" si="8"/>
         <v>590.19999999999993</v>
       </c>
       <c r="N349" t="s">
@@ -18798,7 +18880,7 @@
         <v>15</v>
       </c>
       <c r="M350" s="2">
-        <f>(F350)*(L350-G350)</f>
+        <f t="shared" si="8"/>
         <v>146.9</v>
       </c>
       <c r="N350" t="s">
@@ -18852,7 +18934,7 @@
         <v>15</v>
       </c>
       <c r="M351" s="2">
-        <f>(F351)*(L351-G351)</f>
+        <f t="shared" si="8"/>
         <v>198.9</v>
       </c>
       <c r="N351" t="s">
@@ -18906,7 +18988,7 @@
         <v>15</v>
       </c>
       <c r="M352" s="2">
-        <f>(F352)*(L352-G352)</f>
+        <f t="shared" si="8"/>
         <v>261.3</v>
       </c>
       <c r="N352" t="s">
@@ -18960,7 +19042,7 @@
         <v>15</v>
       </c>
       <c r="M353" s="2">
-        <f>(F353)*(L353-G353)</f>
+        <f t="shared" si="8"/>
         <v>319.8</v>
       </c>
       <c r="N353" t="s">
@@ -19014,7 +19096,7 @@
         <v>15</v>
       </c>
       <c r="M354" s="2">
-        <f>(F354)*(L354-G354)</f>
+        <f t="shared" si="8"/>
         <v>219.7</v>
       </c>
       <c r="N354" t="s">
@@ -19068,7 +19150,7 @@
         <v>15</v>
       </c>
       <c r="M355" s="2">
-        <f>(F355)*(L355-G355)</f>
+        <f t="shared" si="8"/>
         <v>258.7</v>
       </c>
       <c r="N355" t="s">
@@ -19122,7 +19204,7 @@
         <v>15</v>
       </c>
       <c r="M356" s="2">
-        <f>(F356)*(L356-G356)</f>
+        <f t="shared" si="8"/>
         <v>250.9</v>
       </c>
       <c r="N356" t="s">
@@ -19176,7 +19258,7 @@
         <v>15</v>
       </c>
       <c r="M357" s="2">
-        <f>(F357)*(L357-G357)</f>
+        <f t="shared" si="8"/>
         <v>397.8</v>
       </c>
       <c r="N357" t="s">
@@ -19230,7 +19312,7 @@
         <v>15</v>
       </c>
       <c r="M358" s="2">
-        <f>(F358)*(L358-G358)</f>
+        <f t="shared" si="8"/>
         <v>178.1</v>
       </c>
       <c r="N358" t="s">
@@ -19284,7 +19366,7 @@
         <v>15</v>
       </c>
       <c r="M359" s="2">
-        <f>(F359)*(L359-G359)</f>
+        <f t="shared" si="8"/>
         <v>310.7</v>
       </c>
       <c r="N359" t="s">
@@ -19338,7 +19420,7 @@
         <v>15</v>
       </c>
       <c r="M360" s="2">
-        <f>(F360)*(L360-G360)</f>
+        <f t="shared" si="8"/>
         <v>215.8</v>
       </c>
       <c r="N360" t="s">
@@ -19392,7 +19474,7 @@
         <v>15</v>
       </c>
       <c r="M361" s="2">
-        <f>(F361)*(L361-G361)</f>
+        <f t="shared" si="8"/>
         <v>232.7</v>
       </c>
       <c r="N361" t="s">
@@ -19446,7 +19528,7 @@
         <v>15</v>
       </c>
       <c r="M362" s="2">
-        <f>(F362)*(L362-G362)</f>
+        <f t="shared" si="8"/>
         <v>322.40000000000003</v>
       </c>
       <c r="N362" t="s">
@@ -19500,7 +19582,7 @@
         <v>15</v>
       </c>
       <c r="M363" s="2">
-        <f>(F363)*(L363-G363)</f>
+        <f t="shared" si="8"/>
         <v>98.02</v>
       </c>
       <c r="N363" t="s">
@@ -19554,7 +19636,7 @@
         <v>15</v>
       </c>
       <c r="M364" s="2">
-        <f>(F364)*(L364-G364)</f>
+        <f t="shared" si="8"/>
         <v>143</v>
       </c>
       <c r="N364" t="s">
@@ -19608,7 +19690,7 @@
         <v>15</v>
       </c>
       <c r="M365" s="2">
-        <f>(F365)*(L365-G365)</f>
+        <f t="shared" si="8"/>
         <v>284.7</v>
       </c>
       <c r="N365" t="s">
@@ -19662,7 +19744,7 @@
         <v>15</v>
       </c>
       <c r="M366" s="2">
-        <f>(F366)*(L366-G366)</f>
+        <f t="shared" si="8"/>
         <v>208</v>
       </c>
       <c r="N366" t="s">
@@ -19716,7 +19798,7 @@
         <v>15</v>
       </c>
       <c r="M367" s="2">
-        <f>(F367)*(L367-G367)</f>
+        <f t="shared" si="8"/>
         <v>202.79999999999998</v>
       </c>
       <c r="N367" t="s">
@@ -19770,7 +19852,7 @@
         <v>15</v>
       </c>
       <c r="M368" s="2">
-        <f>(F368)*(L368-G368)</f>
+        <f t="shared" si="8"/>
         <v>248.3</v>
       </c>
       <c r="N368" t="s">
@@ -19824,7 +19906,7 @@
         <v>15</v>
       </c>
       <c r="M369" s="2">
-        <f>(F369)*(L369-G369)</f>
+        <f t="shared" si="8"/>
         <v>244.4</v>
       </c>
       <c r="N369" t="s">
@@ -19878,7 +19960,7 @@
         <v>15</v>
       </c>
       <c r="M370" s="2">
-        <f>(F370)*(L370-G370)</f>
+        <f t="shared" si="8"/>
         <v>265.2</v>
       </c>
       <c r="N370" t="s">
@@ -19932,7 +20014,7 @@
         <v>15</v>
       </c>
       <c r="M371" s="2">
-        <f>(F371)*(L371-G371)</f>
+        <f t="shared" si="8"/>
         <v>176.79999999999998</v>
       </c>
       <c r="N371" t="s">
@@ -19986,7 +20068,7 @@
         <v>15</v>
       </c>
       <c r="M372" s="2">
-        <f>(F372)*(L372-G372)</f>
+        <f t="shared" si="8"/>
         <v>276.90000000000003</v>
       </c>
       <c r="N372" t="s">
@@ -20040,7 +20122,7 @@
         <v>15</v>
       </c>
       <c r="M373" s="2">
-        <f>(F373)*(L373-G373)</f>
+        <f t="shared" si="8"/>
         <v>274.3</v>
       </c>
       <c r="N373" t="s">
@@ -20094,7 +20176,7 @@
         <v>15</v>
       </c>
       <c r="M374" s="2">
-        <f>(F374)*(L374-G374)</f>
+        <f t="shared" si="8"/>
         <v>315.90000000000003</v>
       </c>
       <c r="N374" t="s">
@@ -20148,7 +20230,7 @@
         <v>15</v>
       </c>
       <c r="M375" s="2">
-        <f>(F375)*(L375-G375)</f>
+        <f t="shared" si="8"/>
         <v>409.5</v>
       </c>
       <c r="N375" t="s">
@@ -20202,7 +20284,7 @@
         <v>15</v>
       </c>
       <c r="M376" s="2">
-        <f>(F376)*(L376-G376)</f>
+        <f t="shared" si="8"/>
         <v>68.509999999999991</v>
       </c>
       <c r="N376" t="s">
@@ -20256,7 +20338,7 @@
         <v>15</v>
       </c>
       <c r="M377" s="2">
-        <f>(F377)*(L377-G377)</f>
+        <f t="shared" ref="M377:M422" si="9">(F377)*(L377-G377)</f>
         <v>133.9</v>
       </c>
       <c r="N377" t="s">
@@ -20310,7 +20392,7 @@
         <v>15</v>
       </c>
       <c r="M378" s="2" t="e">
-        <f>(F378)*(L378-G378)</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="N378" t="s">
@@ -20358,7 +20440,7 @@
         <v>15</v>
       </c>
       <c r="M379" s="2">
-        <f>(F379)*(L379-G379)</f>
+        <f t="shared" si="9"/>
         <v>158.6</v>
       </c>
       <c r="N379" t="s">
@@ -20412,7 +20494,7 @@
         <v>15</v>
       </c>
       <c r="M380" s="2">
-        <f>(F380)*(L380-G380)</f>
+        <f t="shared" si="9"/>
         <v>146.9</v>
       </c>
       <c r="N380" t="s">
@@ -20466,7 +20548,7 @@
         <v>15</v>
       </c>
       <c r="M381" s="2">
-        <f>(F381)*(L381-G381)</f>
+        <f t="shared" si="9"/>
         <v>82.94</v>
       </c>
       <c r="N381" t="s">
@@ -20520,7 +20602,7 @@
         <v>15</v>
       </c>
       <c r="M382" s="2">
-        <f>(F382)*(L382-G382)</f>
+        <f t="shared" si="9"/>
         <v>159.9</v>
       </c>
       <c r="N382" t="s">
@@ -20574,7 +20656,7 @@
         <v>15</v>
       </c>
       <c r="M383" s="2">
-        <f>(F383)*(L383-G383)</f>
+        <f t="shared" si="9"/>
         <v>388.7</v>
       </c>
       <c r="N383" t="s">
@@ -20628,7 +20710,7 @@
         <v>15</v>
       </c>
       <c r="M384" s="2">
-        <f>(F384)*(L384-G384)</f>
+        <f t="shared" si="9"/>
         <v>347.09999999999997</v>
       </c>
       <c r="N384" t="s">
@@ -20682,7 +20764,7 @@
         <v>15</v>
       </c>
       <c r="M385" s="2">
-        <f>(F385)*(L385-G385)</f>
+        <f t="shared" si="9"/>
         <v>280.8</v>
       </c>
       <c r="N385" t="s">
@@ -20736,7 +20818,7 @@
         <v>15</v>
       </c>
       <c r="M386" s="2">
-        <f>(F386)*(L386-G386)</f>
+        <f t="shared" si="9"/>
         <v>257.40000000000003</v>
       </c>
       <c r="N386" t="s">
@@ -20790,7 +20872,7 @@
         <v>15</v>
       </c>
       <c r="M387" s="2">
-        <f>(F387)*(L387-G387)</f>
+        <f t="shared" si="9"/>
         <v>132.6</v>
       </c>
       <c r="N387" t="s">
@@ -20844,7 +20926,7 @@
         <v>15</v>
       </c>
       <c r="M388" s="2">
-        <f>(F388)*(L388-G388)</f>
+        <f t="shared" si="9"/>
         <v>130</v>
       </c>
       <c r="N388" t="s">
@@ -20898,7 +20980,7 @@
         <v>15</v>
       </c>
       <c r="M389" s="2">
-        <f>(F389)*(L389-G389)</f>
+        <f t="shared" si="9"/>
         <v>258.7</v>
       </c>
       <c r="N389" t="s">
@@ -20952,7 +21034,7 @@
         <v>15</v>
       </c>
       <c r="M390" s="2">
-        <f>(F390)*(L390-G390)</f>
+        <f t="shared" si="9"/>
         <v>128.83000000000001</v>
       </c>
       <c r="N390" t="s">
@@ -21006,7 +21088,7 @@
         <v>15</v>
       </c>
       <c r="M391" s="2">
-        <f>(F391)*(L391-G391)</f>
+        <f t="shared" si="9"/>
         <v>257.40000000000003</v>
       </c>
       <c r="N391" t="s">
@@ -21060,7 +21142,7 @@
         <v>15</v>
       </c>
       <c r="M392" s="2">
-        <f>(F392)*(L392-G392)</f>
+        <f t="shared" si="9"/>
         <v>232.7</v>
       </c>
       <c r="N392" t="s">
@@ -21114,7 +21196,7 @@
         <v>15</v>
       </c>
       <c r="M393" s="2">
-        <f>(F393)*(L393-G393)</f>
+        <f t="shared" si="9"/>
         <v>309.40000000000003</v>
       </c>
       <c r="N393" t="s">
@@ -21168,7 +21250,7 @@
         <v>15</v>
       </c>
       <c r="M394" s="2">
-        <f>(F394)*(L394-G394)</f>
+        <f t="shared" si="9"/>
         <v>98.93</v>
       </c>
       <c r="N394" t="s">
@@ -21222,7 +21304,7 @@
         <v>15</v>
       </c>
       <c r="M395" s="2">
-        <f>(F395)*(L395-G395)</f>
+        <f t="shared" si="9"/>
         <v>304.2</v>
       </c>
       <c r="N395" t="s">
@@ -21276,7 +21358,7 @@
         <v>15</v>
       </c>
       <c r="M396" s="2">
-        <f>(F396)*(L396-G396)</f>
+        <f t="shared" si="9"/>
         <v>52.259999999999991</v>
       </c>
       <c r="N396" t="s">
@@ -21330,7 +21412,7 @@
         <v>15</v>
       </c>
       <c r="M397" s="2">
-        <f>(F397)*(L397-G397)</f>
+        <f t="shared" si="9"/>
         <v>253.5</v>
       </c>
       <c r="N397" t="s">
@@ -21384,7 +21466,7 @@
         <v>15</v>
       </c>
       <c r="M398" s="2">
-        <f>(F398)*(L398-G398)</f>
+        <f t="shared" si="9"/>
         <v>171.6</v>
       </c>
       <c r="N398" t="s">
@@ -21398,6 +21480,1182 @@
       </c>
       <c r="R398" t="s">
         <v>479</v>
+      </c>
+    </row>
+    <row r="399" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A399" t="s">
+        <v>617</v>
+      </c>
+      <c r="B399" t="s">
+        <v>2</v>
+      </c>
+      <c r="C399" t="s">
+        <v>618</v>
+      </c>
+      <c r="D399" s="8">
+        <v>43763.466354166667</v>
+      </c>
+      <c r="E399">
+        <v>39.5</v>
+      </c>
+      <c r="F399">
+        <v>3.95</v>
+      </c>
+      <c r="G399">
+        <v>2</v>
+      </c>
+      <c r="H399">
+        <v>100</v>
+      </c>
+      <c r="I399" s="2">
+        <v>41</v>
+      </c>
+      <c r="J399" t="s">
+        <v>484</v>
+      </c>
+      <c r="K399" s="2">
+        <v>35</v>
+      </c>
+      <c r="L399" s="2">
+        <v>15</v>
+      </c>
+      <c r="M399" s="2">
+        <f t="shared" si="9"/>
+        <v>51.35</v>
+      </c>
+      <c r="N399" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q399" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="400" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A400" t="s">
+        <v>617</v>
+      </c>
+      <c r="B400" t="s">
+        <v>2</v>
+      </c>
+      <c r="C400" t="s">
+        <v>619</v>
+      </c>
+      <c r="D400" s="8">
+        <v>43763.466249999998</v>
+      </c>
+      <c r="E400">
+        <v>126</v>
+      </c>
+      <c r="F400">
+        <v>12.6</v>
+      </c>
+      <c r="G400">
+        <v>2</v>
+      </c>
+      <c r="H400">
+        <v>100</v>
+      </c>
+      <c r="I400" s="2">
+        <v>50</v>
+      </c>
+      <c r="J400" t="s">
+        <v>484</v>
+      </c>
+      <c r="K400" s="2">
+        <v>35</v>
+      </c>
+      <c r="L400" s="2">
+        <v>15</v>
+      </c>
+      <c r="M400" s="2">
+        <f t="shared" si="9"/>
+        <v>163.79999999999998</v>
+      </c>
+      <c r="N400" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q400" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="401" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A401" t="s">
+        <v>617</v>
+      </c>
+      <c r="B401" t="s">
+        <v>2</v>
+      </c>
+      <c r="C401" t="s">
+        <v>620</v>
+      </c>
+      <c r="D401" s="8">
+        <v>43763.466145833336</v>
+      </c>
+      <c r="E401">
+        <v>200</v>
+      </c>
+      <c r="F401">
+        <v>20</v>
+      </c>
+      <c r="G401">
+        <v>2</v>
+      </c>
+      <c r="H401">
+        <v>100</v>
+      </c>
+      <c r="I401" s="2">
+        <v>111</v>
+      </c>
+      <c r="J401" t="s">
+        <v>484</v>
+      </c>
+      <c r="K401" s="2">
+        <v>35</v>
+      </c>
+      <c r="L401" s="2">
+        <v>15</v>
+      </c>
+      <c r="M401" s="2">
+        <f t="shared" si="9"/>
+        <v>260</v>
+      </c>
+      <c r="N401" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q401" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="402" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A402" t="s">
+        <v>617</v>
+      </c>
+      <c r="B402" t="s">
+        <v>2</v>
+      </c>
+      <c r="C402" t="s">
+        <v>621</v>
+      </c>
+      <c r="D402" s="8">
+        <v>43763.466041666667</v>
+      </c>
+      <c r="E402">
+        <v>136</v>
+      </c>
+      <c r="F402">
+        <v>13.6</v>
+      </c>
+      <c r="G402">
+        <v>2</v>
+      </c>
+      <c r="H402">
+        <v>100</v>
+      </c>
+      <c r="I402" s="2">
+        <v>108</v>
+      </c>
+      <c r="J402" t="s">
+        <v>484</v>
+      </c>
+      <c r="K402" s="2">
+        <v>35</v>
+      </c>
+      <c r="L402" s="2">
+        <v>15</v>
+      </c>
+      <c r="M402" s="2">
+        <f t="shared" si="9"/>
+        <v>176.79999999999998</v>
+      </c>
+      <c r="N402" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q402" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="403" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A403" t="s">
+        <v>617</v>
+      </c>
+      <c r="B403" t="s">
+        <v>2</v>
+      </c>
+      <c r="C403" t="s">
+        <v>622</v>
+      </c>
+      <c r="D403" s="8">
+        <v>43763.465925925928</v>
+      </c>
+      <c r="E403">
+        <v>62.3</v>
+      </c>
+      <c r="F403">
+        <v>6.23</v>
+      </c>
+      <c r="G403">
+        <v>2</v>
+      </c>
+      <c r="H403">
+        <v>100</v>
+      </c>
+      <c r="I403" s="2">
+        <v>121</v>
+      </c>
+      <c r="J403" t="s">
+        <v>484</v>
+      </c>
+      <c r="K403" s="2">
+        <v>35</v>
+      </c>
+      <c r="L403" s="2">
+        <v>15</v>
+      </c>
+      <c r="M403" s="2">
+        <f t="shared" si="9"/>
+        <v>80.990000000000009</v>
+      </c>
+      <c r="N403" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q403" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="404" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A404" t="s">
+        <v>617</v>
+      </c>
+      <c r="B404" t="s">
+        <v>2</v>
+      </c>
+      <c r="C404" t="s">
+        <v>623</v>
+      </c>
+      <c r="D404" s="8">
+        <v>43763.465810185182</v>
+      </c>
+      <c r="E404">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="F404">
+        <v>7.84</v>
+      </c>
+      <c r="G404">
+        <v>2</v>
+      </c>
+      <c r="H404">
+        <v>100</v>
+      </c>
+      <c r="I404" s="2">
+        <v>34</v>
+      </c>
+      <c r="J404" t="s">
+        <v>484</v>
+      </c>
+      <c r="K404" s="2">
+        <v>35</v>
+      </c>
+      <c r="L404" s="2">
+        <v>15</v>
+      </c>
+      <c r="M404" s="2">
+        <f t="shared" si="9"/>
+        <v>101.92</v>
+      </c>
+      <c r="N404" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q404" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="405" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A405" t="s">
+        <v>617</v>
+      </c>
+      <c r="B405" t="s">
+        <v>2</v>
+      </c>
+      <c r="C405" t="s">
+        <v>624</v>
+      </c>
+      <c r="D405" s="8">
+        <v>43763.465694444443</v>
+      </c>
+      <c r="E405">
+        <v>31</v>
+      </c>
+      <c r="F405">
+        <v>3.1</v>
+      </c>
+      <c r="G405">
+        <v>2</v>
+      </c>
+      <c r="H405">
+        <v>100</v>
+      </c>
+      <c r="I405" s="2">
+        <v>48</v>
+      </c>
+      <c r="J405" t="s">
+        <v>484</v>
+      </c>
+      <c r="K405" s="2">
+        <v>35</v>
+      </c>
+      <c r="L405" s="2">
+        <v>15</v>
+      </c>
+      <c r="M405" s="2">
+        <f t="shared" si="9"/>
+        <v>40.300000000000004</v>
+      </c>
+      <c r="N405" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q405" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="406" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A406" t="s">
+        <v>617</v>
+      </c>
+      <c r="B406" t="s">
+        <v>2</v>
+      </c>
+      <c r="C406" t="s">
+        <v>625</v>
+      </c>
+      <c r="D406" s="8">
+        <v>43763.465590277781</v>
+      </c>
+      <c r="E406">
+        <v>155</v>
+      </c>
+      <c r="F406">
+        <v>15.5</v>
+      </c>
+      <c r="G406">
+        <v>2</v>
+      </c>
+      <c r="H406">
+        <v>100</v>
+      </c>
+      <c r="I406" s="2">
+        <v>53</v>
+      </c>
+      <c r="J406" t="s">
+        <v>484</v>
+      </c>
+      <c r="K406" s="2">
+        <v>35</v>
+      </c>
+      <c r="L406" s="2">
+        <v>15</v>
+      </c>
+      <c r="M406" s="2">
+        <f t="shared" si="9"/>
+        <v>201.5</v>
+      </c>
+      <c r="N406" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q406" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="407" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A407" t="s">
+        <v>617</v>
+      </c>
+      <c r="B407" t="s">
+        <v>2</v>
+      </c>
+      <c r="C407" t="s">
+        <v>626</v>
+      </c>
+      <c r="D407" s="8">
+        <v>43763.465451388889</v>
+      </c>
+      <c r="E407" t="s">
+        <v>4</v>
+      </c>
+      <c r="F407" t="s">
+        <v>4</v>
+      </c>
+      <c r="G407">
+        <v>2</v>
+      </c>
+      <c r="H407">
+        <v>100</v>
+      </c>
+      <c r="I407" s="2">
+        <v>32</v>
+      </c>
+      <c r="J407" t="s">
+        <v>484</v>
+      </c>
+      <c r="K407" s="2">
+        <v>35</v>
+      </c>
+      <c r="L407" s="2">
+        <v>15</v>
+      </c>
+      <c r="M407" s="2" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N407" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q407" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="408" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A408" t="s">
+        <v>617</v>
+      </c>
+      <c r="B408" t="s">
+        <v>2</v>
+      </c>
+      <c r="C408" t="s">
+        <v>627</v>
+      </c>
+      <c r="D408" s="8">
+        <v>43763.46533564815</v>
+      </c>
+      <c r="E408">
+        <v>249</v>
+      </c>
+      <c r="F408">
+        <v>24.9</v>
+      </c>
+      <c r="G408">
+        <v>2</v>
+      </c>
+      <c r="H408">
+        <v>100</v>
+      </c>
+      <c r="I408" s="2">
+        <v>119</v>
+      </c>
+      <c r="J408" t="s">
+        <v>484</v>
+      </c>
+      <c r="K408" s="2">
+        <v>35</v>
+      </c>
+      <c r="L408" s="2">
+        <v>15</v>
+      </c>
+      <c r="M408" s="2">
+        <f t="shared" si="9"/>
+        <v>323.7</v>
+      </c>
+      <c r="N408" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q408" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="409" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A409" t="s">
+        <v>617</v>
+      </c>
+      <c r="B409" t="s">
+        <v>2</v>
+      </c>
+      <c r="C409" t="s">
+        <v>628</v>
+      </c>
+      <c r="D409" s="8">
+        <v>43763.465219907404</v>
+      </c>
+      <c r="E409">
+        <v>293</v>
+      </c>
+      <c r="F409">
+        <v>29.3</v>
+      </c>
+      <c r="G409">
+        <v>2</v>
+      </c>
+      <c r="H409">
+        <v>100</v>
+      </c>
+      <c r="I409" s="2">
+        <v>10</v>
+      </c>
+      <c r="J409" t="s">
+        <v>484</v>
+      </c>
+      <c r="K409" s="2">
+        <v>35</v>
+      </c>
+      <c r="L409" s="2">
+        <v>15</v>
+      </c>
+      <c r="M409" s="2">
+        <f t="shared" si="9"/>
+        <v>380.90000000000003</v>
+      </c>
+      <c r="N409" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q409" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="410" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A410" t="s">
+        <v>617</v>
+      </c>
+      <c r="B410" t="s">
+        <v>2</v>
+      </c>
+      <c r="C410" t="s">
+        <v>629</v>
+      </c>
+      <c r="D410" s="8">
+        <v>43763.465104166666</v>
+      </c>
+      <c r="E410">
+        <v>148</v>
+      </c>
+      <c r="F410">
+        <v>14.8</v>
+      </c>
+      <c r="G410">
+        <v>2</v>
+      </c>
+      <c r="H410">
+        <v>100</v>
+      </c>
+      <c r="I410" s="2">
+        <v>91</v>
+      </c>
+      <c r="J410" t="s">
+        <v>484</v>
+      </c>
+      <c r="K410" s="2">
+        <v>35</v>
+      </c>
+      <c r="L410" s="2">
+        <v>15</v>
+      </c>
+      <c r="M410" s="2">
+        <f t="shared" si="9"/>
+        <v>192.4</v>
+      </c>
+      <c r="N410" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q410" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="411" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A411" t="s">
+        <v>617</v>
+      </c>
+      <c r="B411" t="s">
+        <v>2</v>
+      </c>
+      <c r="C411" t="s">
+        <v>630</v>
+      </c>
+      <c r="D411" s="8">
+        <v>43763.464988425927</v>
+      </c>
+      <c r="E411">
+        <v>54.5</v>
+      </c>
+      <c r="F411">
+        <v>5.45</v>
+      </c>
+      <c r="G411">
+        <v>2</v>
+      </c>
+      <c r="H411">
+        <v>100</v>
+      </c>
+      <c r="I411" s="2">
+        <v>19</v>
+      </c>
+      <c r="J411" t="s">
+        <v>484</v>
+      </c>
+      <c r="K411" s="2">
+        <v>35</v>
+      </c>
+      <c r="L411" s="2">
+        <v>15</v>
+      </c>
+      <c r="M411" s="2">
+        <f t="shared" si="9"/>
+        <v>70.850000000000009</v>
+      </c>
+      <c r="N411" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q411" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="412" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A412" t="s">
+        <v>617</v>
+      </c>
+      <c r="B412" t="s">
+        <v>2</v>
+      </c>
+      <c r="C412" t="s">
+        <v>631</v>
+      </c>
+      <c r="D412" s="8">
+        <v>43763.464895833335</v>
+      </c>
+      <c r="E412">
+        <v>160</v>
+      </c>
+      <c r="F412">
+        <v>16</v>
+      </c>
+      <c r="G412">
+        <v>2</v>
+      </c>
+      <c r="H412">
+        <v>100</v>
+      </c>
+      <c r="I412" s="2">
+        <v>8</v>
+      </c>
+      <c r="J412" t="s">
+        <v>484</v>
+      </c>
+      <c r="K412" s="2">
+        <v>35</v>
+      </c>
+      <c r="L412" s="2">
+        <v>15</v>
+      </c>
+      <c r="M412" s="2">
+        <f t="shared" si="9"/>
+        <v>208</v>
+      </c>
+      <c r="N412" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q412" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="413" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A413" t="s">
+        <v>617</v>
+      </c>
+      <c r="B413" t="s">
+        <v>2</v>
+      </c>
+      <c r="C413" t="s">
+        <v>632</v>
+      </c>
+      <c r="D413" s="8">
+        <v>43763.464756944442</v>
+      </c>
+      <c r="E413" t="s">
+        <v>4</v>
+      </c>
+      <c r="F413" t="s">
+        <v>4</v>
+      </c>
+      <c r="G413">
+        <v>2</v>
+      </c>
+      <c r="H413">
+        <v>100</v>
+      </c>
+      <c r="I413" s="2">
+        <v>62</v>
+      </c>
+      <c r="J413" t="s">
+        <v>484</v>
+      </c>
+      <c r="K413" s="2">
+        <v>35</v>
+      </c>
+      <c r="L413" s="2">
+        <v>15</v>
+      </c>
+      <c r="M413" s="2" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N413" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q413" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="414" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A414" t="s">
+        <v>617</v>
+      </c>
+      <c r="B414" t="s">
+        <v>2</v>
+      </c>
+      <c r="C414" t="s">
+        <v>633</v>
+      </c>
+      <c r="D414" s="8">
+        <v>43763.46465277778</v>
+      </c>
+      <c r="E414">
+        <v>160</v>
+      </c>
+      <c r="F414">
+        <v>16</v>
+      </c>
+      <c r="G414">
+        <v>2</v>
+      </c>
+      <c r="H414">
+        <v>100</v>
+      </c>
+      <c r="I414" s="2">
+        <v>103</v>
+      </c>
+      <c r="J414" t="s">
+        <v>484</v>
+      </c>
+      <c r="K414" s="2">
+        <v>35</v>
+      </c>
+      <c r="L414" s="2">
+        <v>15</v>
+      </c>
+      <c r="M414" s="2">
+        <f t="shared" si="9"/>
+        <v>208</v>
+      </c>
+      <c r="N414" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q414" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="415" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A415" t="s">
+        <v>617</v>
+      </c>
+      <c r="B415" t="s">
+        <v>2</v>
+      </c>
+      <c r="C415" t="s">
+        <v>634</v>
+      </c>
+      <c r="D415" s="8">
+        <v>43763.464513888888</v>
+      </c>
+      <c r="E415">
+        <v>37.6</v>
+      </c>
+      <c r="F415">
+        <v>3.76</v>
+      </c>
+      <c r="G415">
+        <v>2</v>
+      </c>
+      <c r="H415">
+        <v>100</v>
+      </c>
+      <c r="I415" s="2">
+        <v>109</v>
+      </c>
+      <c r="J415" t="s">
+        <v>484</v>
+      </c>
+      <c r="K415" s="2">
+        <v>35</v>
+      </c>
+      <c r="L415" s="2">
+        <v>15</v>
+      </c>
+      <c r="M415" s="2">
+        <f t="shared" si="9"/>
+        <v>48.879999999999995</v>
+      </c>
+      <c r="N415" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q415" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="416" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A416" t="s">
+        <v>617</v>
+      </c>
+      <c r="B416" t="s">
+        <v>2</v>
+      </c>
+      <c r="C416" t="s">
+        <v>635</v>
+      </c>
+      <c r="D416" s="8">
+        <v>43763.464398148149</v>
+      </c>
+      <c r="E416">
+        <v>163</v>
+      </c>
+      <c r="F416">
+        <v>16.3</v>
+      </c>
+      <c r="G416">
+        <v>2</v>
+      </c>
+      <c r="H416">
+        <v>100</v>
+      </c>
+      <c r="I416" s="2">
+        <v>163</v>
+      </c>
+      <c r="J416" t="s">
+        <v>484</v>
+      </c>
+      <c r="K416" s="2">
+        <v>35</v>
+      </c>
+      <c r="L416" s="2">
+        <v>15</v>
+      </c>
+      <c r="M416" s="2">
+        <f t="shared" si="9"/>
+        <v>211.9</v>
+      </c>
+      <c r="N416" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q416" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="417" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A417" t="s">
+        <v>617</v>
+      </c>
+      <c r="B417" t="s">
+        <v>2</v>
+      </c>
+      <c r="C417" t="s">
+        <v>636</v>
+      </c>
+      <c r="D417" s="8">
+        <v>43763.464270833334</v>
+      </c>
+      <c r="E417" t="s">
+        <v>4</v>
+      </c>
+      <c r="F417" t="s">
+        <v>4</v>
+      </c>
+      <c r="G417">
+        <v>2</v>
+      </c>
+      <c r="H417">
+        <v>100</v>
+      </c>
+      <c r="I417" s="2">
+        <v>27</v>
+      </c>
+      <c r="J417" t="s">
+        <v>484</v>
+      </c>
+      <c r="K417" s="2">
+        <v>35</v>
+      </c>
+      <c r="L417" s="2">
+        <v>15</v>
+      </c>
+      <c r="M417" s="2" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N417" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q417" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="418" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A418" t="s">
+        <v>617</v>
+      </c>
+      <c r="B418" t="s">
+        <v>2</v>
+      </c>
+      <c r="C418" t="s">
+        <v>637</v>
+      </c>
+      <c r="D418" s="8">
+        <v>43763.464155092595</v>
+      </c>
+      <c r="E418">
+        <v>41.8</v>
+      </c>
+      <c r="F418">
+        <v>4.18</v>
+      </c>
+      <c r="G418">
+        <v>2</v>
+      </c>
+      <c r="H418">
+        <v>100</v>
+      </c>
+      <c r="I418" s="2">
+        <v>101</v>
+      </c>
+      <c r="J418" t="s">
+        <v>484</v>
+      </c>
+      <c r="K418" s="2">
+        <v>35</v>
+      </c>
+      <c r="L418" s="2">
+        <v>15</v>
+      </c>
+      <c r="M418" s="2">
+        <f t="shared" si="9"/>
+        <v>54.339999999999996</v>
+      </c>
+      <c r="N418" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q418" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="419" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A419" t="s">
+        <v>617</v>
+      </c>
+      <c r="B419" t="s">
+        <v>2</v>
+      </c>
+      <c r="C419" t="s">
+        <v>638</v>
+      </c>
+      <c r="D419" s="8">
+        <v>43763.464039351849</v>
+      </c>
+      <c r="E419">
+        <v>310</v>
+      </c>
+      <c r="F419">
+        <v>31</v>
+      </c>
+      <c r="G419">
+        <v>2</v>
+      </c>
+      <c r="H419">
+        <v>100</v>
+      </c>
+      <c r="I419" s="2">
+        <v>81</v>
+      </c>
+      <c r="J419" t="s">
+        <v>484</v>
+      </c>
+      <c r="K419" s="2">
+        <v>35</v>
+      </c>
+      <c r="L419" s="2">
+        <v>15</v>
+      </c>
+      <c r="M419" s="2">
+        <f t="shared" si="9"/>
+        <v>403</v>
+      </c>
+      <c r="N419" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q419" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="420" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A420" t="s">
+        <v>617</v>
+      </c>
+      <c r="B420" t="s">
+        <v>2</v>
+      </c>
+      <c r="C420" t="s">
+        <v>639</v>
+      </c>
+      <c r="D420" s="8">
+        <v>43763.463923611111</v>
+      </c>
+      <c r="E420">
+        <v>143</v>
+      </c>
+      <c r="F420">
+        <v>14.3</v>
+      </c>
+      <c r="G420">
+        <v>2</v>
+      </c>
+      <c r="H420">
+        <v>100</v>
+      </c>
+      <c r="I420" s="2">
+        <v>144</v>
+      </c>
+      <c r="J420" t="s">
+        <v>484</v>
+      </c>
+      <c r="K420" s="2">
+        <v>35</v>
+      </c>
+      <c r="L420" s="2">
+        <v>15</v>
+      </c>
+      <c r="M420" s="2">
+        <f t="shared" si="9"/>
+        <v>185.9</v>
+      </c>
+      <c r="N420" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q420" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="421" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A421" t="s">
+        <v>617</v>
+      </c>
+      <c r="B421" t="s">
+        <v>2</v>
+      </c>
+      <c r="C421" t="s">
+        <v>640</v>
+      </c>
+      <c r="D421" s="8">
+        <v>43763.463796296295</v>
+      </c>
+      <c r="E421">
+        <v>235</v>
+      </c>
+      <c r="F421">
+        <v>23.5</v>
+      </c>
+      <c r="G421">
+        <v>2</v>
+      </c>
+      <c r="H421">
+        <v>100</v>
+      </c>
+      <c r="I421" s="2">
+        <v>133</v>
+      </c>
+      <c r="J421" t="s">
+        <v>484</v>
+      </c>
+      <c r="K421" s="2">
+        <v>35</v>
+      </c>
+      <c r="L421" s="2">
+        <v>15</v>
+      </c>
+      <c r="M421" s="2">
+        <f t="shared" si="9"/>
+        <v>305.5</v>
+      </c>
+      <c r="N421" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q421" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="422" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A422" t="s">
+        <v>617</v>
+      </c>
+      <c r="B422" t="s">
+        <v>2</v>
+      </c>
+      <c r="C422" t="s">
+        <v>641</v>
+      </c>
+      <c r="D422" s="8">
+        <v>43763.463645833333</v>
+      </c>
+      <c r="E422" t="s">
+        <v>4</v>
+      </c>
+      <c r="F422" t="s">
+        <v>4</v>
+      </c>
+      <c r="G422">
+        <v>2</v>
+      </c>
+      <c r="H422">
+        <v>100</v>
+      </c>
+      <c r="I422" s="2">
+        <v>15</v>
+      </c>
+      <c r="J422" t="s">
+        <v>484</v>
+      </c>
+      <c r="K422" s="2">
+        <v>35</v>
+      </c>
+      <c r="L422" s="2">
+        <v>15</v>
+      </c>
+      <c r="M422" s="2" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N422" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q422" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="423" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I423">
+        <v>43</v>
+      </c>
+      <c r="P423" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="424" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I424" s="2">
+        <v>6</v>
+      </c>
+      <c r="P424" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="425" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I425" s="2">
+        <v>76</v>
+      </c>
+      <c r="P425" t="s">
+        <v>643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more qubit results from today
</commit_message>
<xml_diff>
--- a/analyses/master-qubit.xlsx
+++ b/analyses/master-qubit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4613FE5C-426E-164D-BBDA-A3BB64B9ACC2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1B9E3E-8EAC-7844-B71B-86CEF25E28B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="14900" xr2:uid="{C961D9B2-DEF5-3E45-BFAA-11F0CD1F34D4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3336" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3479" uniqueCount="669">
   <si>
     <t>tube_number</t>
   </si>
@@ -1965,7 +1965,82 @@
     <t>https://grace-ac.github.io/extract-RNA/</t>
   </si>
   <si>
-    <t>extracted / missing</t>
+    <t>2019-10-25_171528</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171921</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171910</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171902</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171854</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171844</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171836</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171827</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171818</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171810</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171801</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171753</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171744</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171734</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171725</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171716</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171706</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171657</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171648</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171637</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171627</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171618</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171609</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171600</t>
+  </si>
+  <si>
+    <t>Sample_#191025-171550</t>
+  </si>
+  <si>
+    <t>https://grace-ac.github.io/second-batch-extracted-RNA-and-results/</t>
   </si>
 </sst>
 </file>
@@ -2356,17 +2431,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EE0E31-7CFF-2843-B4D6-D974DF19D232}">
-  <dimension ref="A1:U425"/>
+  <dimension ref="A1:U446"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A418" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O451" sqref="O451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="23.83203125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
@@ -11622,7 +11697,7 @@
         <v>14</v>
       </c>
       <c r="M194" t="e">
-        <f t="shared" ref="M194:M257" si="3">(F194)*(L194-G194)</f>
+        <f t="shared" ref="M194:M234" si="3">(F194)*(L194-G194)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N194" t="s">
@@ -20338,7 +20413,7 @@
         <v>15</v>
       </c>
       <c r="M377" s="2">
-        <f t="shared" ref="M377:M422" si="9">(F377)*(L377-G377)</f>
+        <f t="shared" ref="M377:M440" si="9">(F377)*(L377-G377)</f>
         <v>133.9</v>
       </c>
       <c r="N377" t="s">
@@ -22635,27 +22710,1155 @@
       </c>
     </row>
     <row r="423" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I423">
-        <v>43</v>
-      </c>
-      <c r="P423" t="s">
+      <c r="A423" t="s">
         <v>643</v>
       </c>
+      <c r="B423" t="s">
+        <v>2</v>
+      </c>
+      <c r="C423" t="s">
+        <v>644</v>
+      </c>
+      <c r="D423" s="8">
+        <v>43763.721770833334</v>
+      </c>
+      <c r="E423">
+        <v>258</v>
+      </c>
+      <c r="F423">
+        <v>25.8</v>
+      </c>
+      <c r="G423">
+        <v>2</v>
+      </c>
+      <c r="H423">
+        <v>100</v>
+      </c>
+      <c r="I423" s="2">
+        <v>29</v>
+      </c>
+      <c r="J423" t="s">
+        <v>484</v>
+      </c>
+      <c r="K423" s="2">
+        <v>35</v>
+      </c>
+      <c r="L423" s="2">
+        <v>15</v>
+      </c>
+      <c r="M423" s="2">
+        <f t="shared" si="9"/>
+        <v>335.40000000000003</v>
+      </c>
+      <c r="N423" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q423" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="424" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A424" t="s">
+        <v>643</v>
+      </c>
+      <c r="B424" t="s">
+        <v>2</v>
+      </c>
+      <c r="C424" t="s">
+        <v>645</v>
+      </c>
+      <c r="D424" s="8">
+        <v>43763.721643518518</v>
+      </c>
+      <c r="E424" t="s">
+        <v>4</v>
+      </c>
+      <c r="F424" t="s">
+        <v>4</v>
+      </c>
+      <c r="G424">
+        <v>2</v>
+      </c>
+      <c r="H424">
+        <v>100</v>
+      </c>
       <c r="I424" s="2">
-        <v>6</v>
-      </c>
-      <c r="P424" t="s">
+        <v>44</v>
+      </c>
+      <c r="J424" t="s">
+        <v>484</v>
+      </c>
+      <c r="K424" s="2">
+        <v>35</v>
+      </c>
+      <c r="L424" s="2">
+        <v>15</v>
+      </c>
+      <c r="M424" s="2" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N424" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q424" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="425" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A425" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="425" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B425" t="s">
+        <v>2</v>
+      </c>
+      <c r="C425" t="s">
+        <v>646</v>
+      </c>
+      <c r="D425" s="8">
+        <v>43763.721550925926</v>
+      </c>
+      <c r="E425">
+        <v>130</v>
+      </c>
+      <c r="F425">
+        <v>13</v>
+      </c>
+      <c r="G425">
+        <v>2</v>
+      </c>
+      <c r="H425">
+        <v>100</v>
+      </c>
       <c r="I425" s="2">
-        <v>76</v>
-      </c>
-      <c r="P425" t="s">
+        <v>1</v>
+      </c>
+      <c r="J425" t="s">
+        <v>484</v>
+      </c>
+      <c r="K425" s="2">
+        <v>35</v>
+      </c>
+      <c r="L425" s="2">
+        <v>15</v>
+      </c>
+      <c r="M425" s="2">
+        <f t="shared" si="9"/>
+        <v>169</v>
+      </c>
+      <c r="N425" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q425" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="426" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A426" t="s">
         <v>643</v>
+      </c>
+      <c r="B426" t="s">
+        <v>2</v>
+      </c>
+      <c r="C426" t="s">
+        <v>647</v>
+      </c>
+      <c r="D426" s="8">
+        <v>43763.721458333333</v>
+      </c>
+      <c r="E426">
+        <v>228</v>
+      </c>
+      <c r="F426">
+        <v>22.8</v>
+      </c>
+      <c r="G426">
+        <v>2</v>
+      </c>
+      <c r="H426">
+        <v>100</v>
+      </c>
+      <c r="I426" s="2">
+        <v>177</v>
+      </c>
+      <c r="J426" t="s">
+        <v>484</v>
+      </c>
+      <c r="K426" s="2">
+        <v>35</v>
+      </c>
+      <c r="L426" s="2">
+        <v>15</v>
+      </c>
+      <c r="M426" s="2">
+        <f t="shared" si="9"/>
+        <v>296.40000000000003</v>
+      </c>
+      <c r="N426" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q426" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="427" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A427" t="s">
+        <v>643</v>
+      </c>
+      <c r="B427" t="s">
+        <v>2</v>
+      </c>
+      <c r="C427" t="s">
+        <v>648</v>
+      </c>
+      <c r="D427" s="8">
+        <v>43763.721342592595</v>
+      </c>
+      <c r="E427">
+        <v>115</v>
+      </c>
+      <c r="F427">
+        <v>11.5</v>
+      </c>
+      <c r="G427">
+        <v>2</v>
+      </c>
+      <c r="H427">
+        <v>100</v>
+      </c>
+      <c r="I427" s="2">
+        <v>95</v>
+      </c>
+      <c r="J427" t="s">
+        <v>484</v>
+      </c>
+      <c r="K427" s="2">
+        <v>35</v>
+      </c>
+      <c r="L427" s="2">
+        <v>15</v>
+      </c>
+      <c r="M427" s="2">
+        <f t="shared" si="9"/>
+        <v>149.5</v>
+      </c>
+      <c r="N427" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q427" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="428" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A428" t="s">
+        <v>643</v>
+      </c>
+      <c r="B428" t="s">
+        <v>2</v>
+      </c>
+      <c r="C428" t="s">
+        <v>649</v>
+      </c>
+      <c r="D428" s="8">
+        <v>43763.721250000002</v>
+      </c>
+      <c r="E428">
+        <v>166</v>
+      </c>
+      <c r="F428">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G428">
+        <v>2</v>
+      </c>
+      <c r="H428">
+        <v>100</v>
+      </c>
+      <c r="I428" s="2">
+        <v>124</v>
+      </c>
+      <c r="J428" t="s">
+        <v>484</v>
+      </c>
+      <c r="K428" s="2">
+        <v>35</v>
+      </c>
+      <c r="L428" s="2">
+        <v>15</v>
+      </c>
+      <c r="M428" s="2">
+        <f t="shared" si="9"/>
+        <v>215.8</v>
+      </c>
+      <c r="N428" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q428" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="429" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A429" t="s">
+        <v>643</v>
+      </c>
+      <c r="B429" t="s">
+        <v>2</v>
+      </c>
+      <c r="C429" t="s">
+        <v>650</v>
+      </c>
+      <c r="D429" s="8">
+        <v>43763.721145833333</v>
+      </c>
+      <c r="E429">
+        <v>139</v>
+      </c>
+      <c r="F429">
+        <v>13.9</v>
+      </c>
+      <c r="G429">
+        <v>2</v>
+      </c>
+      <c r="H429">
+        <v>100</v>
+      </c>
+      <c r="I429" s="2">
+        <v>67</v>
+      </c>
+      <c r="J429" t="s">
+        <v>484</v>
+      </c>
+      <c r="K429" s="2">
+        <v>35</v>
+      </c>
+      <c r="L429" s="2">
+        <v>15</v>
+      </c>
+      <c r="M429" s="2">
+        <f t="shared" si="9"/>
+        <v>180.70000000000002</v>
+      </c>
+      <c r="N429" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q429" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="430" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A430" t="s">
+        <v>643</v>
+      </c>
+      <c r="B430" t="s">
+        <v>2</v>
+      </c>
+      <c r="C430" t="s">
+        <v>651</v>
+      </c>
+      <c r="D430" s="8">
+        <v>43763.721041666664</v>
+      </c>
+      <c r="E430">
+        <v>118</v>
+      </c>
+      <c r="F430">
+        <v>11.8</v>
+      </c>
+      <c r="G430">
+        <v>2</v>
+      </c>
+      <c r="H430">
+        <v>100</v>
+      </c>
+      <c r="I430" s="2">
+        <v>7</v>
+      </c>
+      <c r="J430" t="s">
+        <v>484</v>
+      </c>
+      <c r="K430" s="2">
+        <v>35</v>
+      </c>
+      <c r="L430" s="2">
+        <v>15</v>
+      </c>
+      <c r="M430" s="2">
+        <f t="shared" si="9"/>
+        <v>153.4</v>
+      </c>
+      <c r="N430" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q430" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="431" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A431" t="s">
+        <v>643</v>
+      </c>
+      <c r="B431" t="s">
+        <v>2</v>
+      </c>
+      <c r="C431" t="s">
+        <v>652</v>
+      </c>
+      <c r="D431" s="8">
+        <v>43763.720949074072</v>
+      </c>
+      <c r="E431">
+        <v>464</v>
+      </c>
+      <c r="F431">
+        <v>46.4</v>
+      </c>
+      <c r="G431">
+        <v>2</v>
+      </c>
+      <c r="H431">
+        <v>100</v>
+      </c>
+      <c r="I431" s="2">
+        <v>169</v>
+      </c>
+      <c r="J431" t="s">
+        <v>484</v>
+      </c>
+      <c r="K431" s="2">
+        <v>35</v>
+      </c>
+      <c r="L431" s="2">
+        <v>15</v>
+      </c>
+      <c r="M431" s="2">
+        <f t="shared" si="9"/>
+        <v>603.19999999999993</v>
+      </c>
+      <c r="N431" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q431" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="432" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A432" t="s">
+        <v>643</v>
+      </c>
+      <c r="B432" t="s">
+        <v>2</v>
+      </c>
+      <c r="C432" t="s">
+        <v>653</v>
+      </c>
+      <c r="D432" s="8">
+        <v>43763.72084490741</v>
+      </c>
+      <c r="E432">
+        <v>212</v>
+      </c>
+      <c r="F432">
+        <v>21.2</v>
+      </c>
+      <c r="G432">
+        <v>2</v>
+      </c>
+      <c r="H432">
+        <v>100</v>
+      </c>
+      <c r="I432" s="2">
+        <v>24</v>
+      </c>
+      <c r="J432" t="s">
+        <v>484</v>
+      </c>
+      <c r="K432" s="2">
+        <v>35</v>
+      </c>
+      <c r="L432" s="2">
+        <v>15</v>
+      </c>
+      <c r="M432" s="2">
+        <f t="shared" si="9"/>
+        <v>275.59999999999997</v>
+      </c>
+      <c r="N432" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q432" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="433" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A433" t="s">
+        <v>643</v>
+      </c>
+      <c r="B433" t="s">
+        <v>2</v>
+      </c>
+      <c r="C433" t="s">
+        <v>654</v>
+      </c>
+      <c r="D433" s="8">
+        <v>43763.720752314817</v>
+      </c>
+      <c r="E433">
+        <v>117</v>
+      </c>
+      <c r="F433">
+        <v>11.7</v>
+      </c>
+      <c r="G433">
+        <v>2</v>
+      </c>
+      <c r="H433">
+        <v>100</v>
+      </c>
+      <c r="I433" s="2">
+        <v>11</v>
+      </c>
+      <c r="J433" t="s">
+        <v>484</v>
+      </c>
+      <c r="K433" s="2">
+        <v>35</v>
+      </c>
+      <c r="L433" s="2">
+        <v>15</v>
+      </c>
+      <c r="M433" s="2">
+        <f t="shared" si="9"/>
+        <v>152.1</v>
+      </c>
+      <c r="N433" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q433" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="434" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A434" t="s">
+        <v>643</v>
+      </c>
+      <c r="B434" t="s">
+        <v>2</v>
+      </c>
+      <c r="C434" t="s">
+        <v>655</v>
+      </c>
+      <c r="D434" s="8">
+        <v>43763.720648148148</v>
+      </c>
+      <c r="E434">
+        <v>134</v>
+      </c>
+      <c r="F434">
+        <v>13.4</v>
+      </c>
+      <c r="G434">
+        <v>2</v>
+      </c>
+      <c r="H434">
+        <v>100</v>
+      </c>
+      <c r="I434" s="2">
+        <v>5</v>
+      </c>
+      <c r="J434" t="s">
+        <v>484</v>
+      </c>
+      <c r="K434" s="2">
+        <v>35</v>
+      </c>
+      <c r="L434" s="2">
+        <v>15</v>
+      </c>
+      <c r="M434" s="2">
+        <f t="shared" si="9"/>
+        <v>174.20000000000002</v>
+      </c>
+      <c r="N434" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q434" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="435" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A435" t="s">
+        <v>643</v>
+      </c>
+      <c r="B435" t="s">
+        <v>2</v>
+      </c>
+      <c r="C435" t="s">
+        <v>656</v>
+      </c>
+      <c r="D435" s="8">
+        <v>43763.720532407409</v>
+      </c>
+      <c r="E435">
+        <v>147</v>
+      </c>
+      <c r="F435">
+        <v>14.7</v>
+      </c>
+      <c r="G435">
+        <v>2</v>
+      </c>
+      <c r="H435">
+        <v>100</v>
+      </c>
+      <c r="I435" s="2">
+        <v>166</v>
+      </c>
+      <c r="J435" t="s">
+        <v>484</v>
+      </c>
+      <c r="K435" s="2">
+        <v>35</v>
+      </c>
+      <c r="L435" s="2">
+        <v>15</v>
+      </c>
+      <c r="M435" s="2">
+        <f t="shared" si="9"/>
+        <v>191.1</v>
+      </c>
+      <c r="N435" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q435" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="436" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A436" t="s">
+        <v>643</v>
+      </c>
+      <c r="B436" t="s">
+        <v>2</v>
+      </c>
+      <c r="C436" t="s">
+        <v>657</v>
+      </c>
+      <c r="D436" s="8">
+        <v>43763.72042824074</v>
+      </c>
+      <c r="E436">
+        <v>174</v>
+      </c>
+      <c r="F436">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G436">
+        <v>2</v>
+      </c>
+      <c r="H436">
+        <v>100</v>
+      </c>
+      <c r="I436" s="2">
+        <v>17</v>
+      </c>
+      <c r="J436" t="s">
+        <v>484</v>
+      </c>
+      <c r="K436" s="2">
+        <v>35</v>
+      </c>
+      <c r="L436" s="2">
+        <v>15</v>
+      </c>
+      <c r="M436" s="2">
+        <f t="shared" si="9"/>
+        <v>226.2</v>
+      </c>
+      <c r="N436" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q436" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="437" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A437" t="s">
+        <v>643</v>
+      </c>
+      <c r="B437" t="s">
+        <v>2</v>
+      </c>
+      <c r="C437" t="s">
+        <v>658</v>
+      </c>
+      <c r="D437" s="8">
+        <v>43763.720324074071</v>
+      </c>
+      <c r="E437">
+        <v>231</v>
+      </c>
+      <c r="F437">
+        <v>23.1</v>
+      </c>
+      <c r="G437">
+        <v>2</v>
+      </c>
+      <c r="H437">
+        <v>100</v>
+      </c>
+      <c r="I437" s="2">
+        <v>117</v>
+      </c>
+      <c r="J437" t="s">
+        <v>484</v>
+      </c>
+      <c r="K437" s="2">
+        <v>35</v>
+      </c>
+      <c r="L437" s="2">
+        <v>15</v>
+      </c>
+      <c r="M437" s="2">
+        <f t="shared" si="9"/>
+        <v>300.3</v>
+      </c>
+      <c r="N437" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q437" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="438" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A438" t="s">
+        <v>643</v>
+      </c>
+      <c r="B438" t="s">
+        <v>2</v>
+      </c>
+      <c r="C438" t="s">
+        <v>659</v>
+      </c>
+      <c r="D438" s="8">
+        <v>43763.720208333332</v>
+      </c>
+      <c r="E438">
+        <v>145</v>
+      </c>
+      <c r="F438">
+        <v>14.5</v>
+      </c>
+      <c r="G438">
+        <v>2</v>
+      </c>
+      <c r="H438">
+        <v>100</v>
+      </c>
+      <c r="I438" s="2">
+        <v>102</v>
+      </c>
+      <c r="J438" t="s">
+        <v>484</v>
+      </c>
+      <c r="K438" s="2">
+        <v>35</v>
+      </c>
+      <c r="L438" s="2">
+        <v>15</v>
+      </c>
+      <c r="M438" s="2">
+        <f t="shared" si="9"/>
+        <v>188.5</v>
+      </c>
+      <c r="N438" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q438" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="439" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A439" t="s">
+        <v>643</v>
+      </c>
+      <c r="B439" t="s">
+        <v>2</v>
+      </c>
+      <c r="C439" t="s">
+        <v>660</v>
+      </c>
+      <c r="D439" s="8">
+        <v>43763.720104166663</v>
+      </c>
+      <c r="E439">
+        <v>186</v>
+      </c>
+      <c r="F439">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="G439">
+        <v>2</v>
+      </c>
+      <c r="H439">
+        <v>100</v>
+      </c>
+      <c r="I439" s="2">
+        <v>151</v>
+      </c>
+      <c r="J439" t="s">
+        <v>484</v>
+      </c>
+      <c r="K439" s="2">
+        <v>35</v>
+      </c>
+      <c r="L439" s="2">
+        <v>15</v>
+      </c>
+      <c r="M439" s="2">
+        <f t="shared" si="9"/>
+        <v>241.8</v>
+      </c>
+      <c r="N439" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q439" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="440" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A440" t="s">
+        <v>643</v>
+      </c>
+      <c r="B440" t="s">
+        <v>2</v>
+      </c>
+      <c r="C440" t="s">
+        <v>661</v>
+      </c>
+      <c r="D440" s="8">
+        <v>43763.72</v>
+      </c>
+      <c r="E440">
+        <v>231</v>
+      </c>
+      <c r="F440">
+        <v>23.1</v>
+      </c>
+      <c r="G440">
+        <v>2</v>
+      </c>
+      <c r="H440">
+        <v>100</v>
+      </c>
+      <c r="I440" s="2">
+        <v>170</v>
+      </c>
+      <c r="J440" t="s">
+        <v>484</v>
+      </c>
+      <c r="K440" s="2">
+        <v>35</v>
+      </c>
+      <c r="L440" s="2">
+        <v>15</v>
+      </c>
+      <c r="M440" s="2">
+        <f t="shared" si="9"/>
+        <v>300.3</v>
+      </c>
+      <c r="N440" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q440" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="441" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A441" t="s">
+        <v>643</v>
+      </c>
+      <c r="B441" t="s">
+        <v>2</v>
+      </c>
+      <c r="C441" t="s">
+        <v>662</v>
+      </c>
+      <c r="D441" s="8">
+        <v>43763.719872685186</v>
+      </c>
+      <c r="E441">
+        <v>840</v>
+      </c>
+      <c r="F441">
+        <v>84</v>
+      </c>
+      <c r="G441">
+        <v>2</v>
+      </c>
+      <c r="H441">
+        <v>100</v>
+      </c>
+      <c r="I441" s="2">
+        <v>172</v>
+      </c>
+      <c r="J441" t="s">
+        <v>484</v>
+      </c>
+      <c r="K441" s="2">
+        <v>35</v>
+      </c>
+      <c r="L441" s="2">
+        <v>15</v>
+      </c>
+      <c r="M441" s="2">
+        <f t="shared" ref="M441:M446" si="10">(F441)*(L441-G441)</f>
+        <v>1092</v>
+      </c>
+      <c r="N441" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q441" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="442" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A442" t="s">
+        <v>643</v>
+      </c>
+      <c r="B442" t="s">
+        <v>2</v>
+      </c>
+      <c r="C442" t="s">
+        <v>663</v>
+      </c>
+      <c r="D442" s="8">
+        <v>43763.719756944447</v>
+      </c>
+      <c r="E442">
+        <v>186</v>
+      </c>
+      <c r="F442">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="G442">
+        <v>2</v>
+      </c>
+      <c r="H442">
+        <v>100</v>
+      </c>
+      <c r="I442" s="2">
+        <v>158</v>
+      </c>
+      <c r="J442" t="s">
+        <v>484</v>
+      </c>
+      <c r="K442" s="2">
+        <v>35</v>
+      </c>
+      <c r="L442" s="2">
+        <v>15</v>
+      </c>
+      <c r="M442" s="2">
+        <f t="shared" si="10"/>
+        <v>241.8</v>
+      </c>
+      <c r="N442" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q442" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="443" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A443" t="s">
+        <v>643</v>
+      </c>
+      <c r="B443" t="s">
+        <v>2</v>
+      </c>
+      <c r="C443" t="s">
+        <v>664</v>
+      </c>
+      <c r="D443" s="8">
+        <v>43763.719652777778</v>
+      </c>
+      <c r="E443">
+        <v>252</v>
+      </c>
+      <c r="F443">
+        <v>25.2</v>
+      </c>
+      <c r="G443">
+        <v>2</v>
+      </c>
+      <c r="H443">
+        <v>100</v>
+      </c>
+      <c r="I443" s="2">
+        <v>54</v>
+      </c>
+      <c r="J443" t="s">
+        <v>484</v>
+      </c>
+      <c r="K443" s="2">
+        <v>35</v>
+      </c>
+      <c r="L443" s="2">
+        <v>15</v>
+      </c>
+      <c r="M443" s="2">
+        <f t="shared" si="10"/>
+        <v>327.59999999999997</v>
+      </c>
+      <c r="N443" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q443" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="444" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A444" t="s">
+        <v>643</v>
+      </c>
+      <c r="B444" t="s">
+        <v>2</v>
+      </c>
+      <c r="C444" t="s">
+        <v>665</v>
+      </c>
+      <c r="D444" s="8">
+        <v>43763.719548611109</v>
+      </c>
+      <c r="E444">
+        <v>277</v>
+      </c>
+      <c r="F444">
+        <v>27.7</v>
+      </c>
+      <c r="G444">
+        <v>2</v>
+      </c>
+      <c r="H444">
+        <v>100</v>
+      </c>
+      <c r="I444" s="2">
+        <v>20</v>
+      </c>
+      <c r="J444" t="s">
+        <v>484</v>
+      </c>
+      <c r="K444" s="2">
+        <v>35</v>
+      </c>
+      <c r="L444" s="2">
+        <v>15</v>
+      </c>
+      <c r="M444" s="2">
+        <f t="shared" si="10"/>
+        <v>360.09999999999997</v>
+      </c>
+      <c r="N444" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q444" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="445" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A445" t="s">
+        <v>643</v>
+      </c>
+      <c r="B445" t="s">
+        <v>2</v>
+      </c>
+      <c r="C445" t="s">
+        <v>666</v>
+      </c>
+      <c r="D445" s="8">
+        <v>43763.719444444447</v>
+      </c>
+      <c r="E445">
+        <v>100</v>
+      </c>
+      <c r="F445">
+        <v>10</v>
+      </c>
+      <c r="G445">
+        <v>2</v>
+      </c>
+      <c r="H445">
+        <v>100</v>
+      </c>
+      <c r="I445" s="2">
+        <v>63</v>
+      </c>
+      <c r="J445" t="s">
+        <v>484</v>
+      </c>
+      <c r="K445" s="2">
+        <v>35</v>
+      </c>
+      <c r="L445" s="2">
+        <v>15</v>
+      </c>
+      <c r="M445" s="2">
+        <f t="shared" si="10"/>
+        <v>130</v>
+      </c>
+      <c r="N445" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q445" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="446" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A446" t="s">
+        <v>643</v>
+      </c>
+      <c r="B446" t="s">
+        <v>2</v>
+      </c>
+      <c r="C446" t="s">
+        <v>667</v>
+      </c>
+      <c r="D446" s="8">
+        <v>43763.719328703701</v>
+      </c>
+      <c r="E446">
+        <v>182</v>
+      </c>
+      <c r="F446">
+        <v>18.2</v>
+      </c>
+      <c r="G446">
+        <v>2</v>
+      </c>
+      <c r="H446">
+        <v>100</v>
+      </c>
+      <c r="I446" s="2">
+        <v>71</v>
+      </c>
+      <c r="J446" t="s">
+        <v>484</v>
+      </c>
+      <c r="K446" s="2">
+        <v>35</v>
+      </c>
+      <c r="L446" s="2">
+        <v>15</v>
+      </c>
+      <c r="M446" s="2">
+        <f t="shared" si="10"/>
+        <v>236.6</v>
+      </c>
+      <c r="N446" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q446" t="s">
+        <v>668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update master qubit with today's
</commit_message>
<xml_diff>
--- a/analyses/master-qubit.xlsx
+++ b/analyses/master-qubit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1B9E3E-8EAC-7844-B71B-86CEF25E28B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534DC644-80A3-7B4E-88CD-34E85EA16CAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="14900" xr2:uid="{C961D9B2-DEF5-3E45-BFAA-11F0CD1F34D4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3479" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3599" uniqueCount="694">
   <si>
     <t>tube_number</t>
   </si>
@@ -2041,6 +2041,81 @@
   </si>
   <si>
     <t>https://grace-ac.github.io/second-batch-extracted-RNA-and-results/</t>
+  </si>
+  <si>
+    <t>2019-10-28_171734</t>
+  </si>
+  <si>
+    <t>Sample_#191028-172129</t>
+  </si>
+  <si>
+    <t>Sample_#191028-172120</t>
+  </si>
+  <si>
+    <t>Sample_#191028-172111</t>
+  </si>
+  <si>
+    <t>Sample_#191028-172102</t>
+  </si>
+  <si>
+    <t>Sample_#191028-172054</t>
+  </si>
+  <si>
+    <t>Sample_#191028-172044</t>
+  </si>
+  <si>
+    <t>Sample_#191028-172035</t>
+  </si>
+  <si>
+    <t>Sample_#191028-172027</t>
+  </si>
+  <si>
+    <t>Sample_#191028-172018</t>
+  </si>
+  <si>
+    <t>Sample_#191028-172009</t>
+  </si>
+  <si>
+    <t>Sample_#191028-172000</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171952</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171943</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171933</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171924</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171916</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171907</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171859</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171850</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171842</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171833</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171824</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171816</t>
+  </si>
+  <si>
+    <t>Sample_#191028-171806</t>
   </si>
 </sst>
 </file>
@@ -2431,10 +2506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EE0E31-7CFF-2843-B4D6-D974DF19D232}">
-  <dimension ref="A1:U446"/>
+  <dimension ref="A1:U470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O451" sqref="O451"/>
+    <sheetView tabSelected="1" topLeftCell="A430" zoomScale="75" workbookViewId="0">
+      <selection activeCell="P459" sqref="P459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23611,7 +23686,7 @@
         <v>15</v>
       </c>
       <c r="M441" s="2">
-        <f t="shared" ref="M441:M446" si="10">(F441)*(L441-G441)</f>
+        <f t="shared" ref="M441:M470" si="10">(F441)*(L441-G441)</f>
         <v>1092</v>
       </c>
       <c r="N441" t="s">
@@ -23859,6 +23934,1086 @@
       </c>
       <c r="Q446" t="s">
         <v>668</v>
+      </c>
+    </row>
+    <row r="447" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A447" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B447" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C447" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D447" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E447" s="1">
+        <v>244</v>
+      </c>
+      <c r="F447" s="1">
+        <v>24.4</v>
+      </c>
+      <c r="G447" s="1">
+        <v>2</v>
+      </c>
+      <c r="H447" s="1">
+        <v>100</v>
+      </c>
+      <c r="I447" s="2">
+        <v>282</v>
+      </c>
+      <c r="J447" t="s">
+        <v>484</v>
+      </c>
+      <c r="K447" s="2">
+        <v>35</v>
+      </c>
+      <c r="L447" s="2">
+        <v>15</v>
+      </c>
+      <c r="M447" s="2">
+        <f t="shared" si="10"/>
+        <v>317.2</v>
+      </c>
+      <c r="N447" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="448" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A448" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B448" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C448" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="D448" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E448" s="1">
+        <v>152</v>
+      </c>
+      <c r="F448" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="G448" s="1">
+        <v>2</v>
+      </c>
+      <c r="H448" s="1">
+        <v>100</v>
+      </c>
+      <c r="I448" s="2">
+        <v>268</v>
+      </c>
+      <c r="J448" t="s">
+        <v>484</v>
+      </c>
+      <c r="K448" s="2">
+        <v>35</v>
+      </c>
+      <c r="L448" s="2">
+        <v>15</v>
+      </c>
+      <c r="M448" s="2">
+        <f t="shared" si="10"/>
+        <v>197.6</v>
+      </c>
+      <c r="N448" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="449" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A449" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B449" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C449" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="D449" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E449" s="1">
+        <v>183</v>
+      </c>
+      <c r="F449" s="1">
+        <v>18.3</v>
+      </c>
+      <c r="G449" s="1">
+        <v>2</v>
+      </c>
+      <c r="H449" s="1">
+        <v>100</v>
+      </c>
+      <c r="I449" s="2">
+        <v>374</v>
+      </c>
+      <c r="J449" t="s">
+        <v>484</v>
+      </c>
+      <c r="K449" s="2">
+        <v>35</v>
+      </c>
+      <c r="L449" s="2">
+        <v>15</v>
+      </c>
+      <c r="M449" s="2">
+        <f t="shared" si="10"/>
+        <v>237.9</v>
+      </c>
+      <c r="N449" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="450" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A450" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B450" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C450" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="D450" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E450" s="1">
+        <v>231</v>
+      </c>
+      <c r="F450" s="1">
+        <v>23.1</v>
+      </c>
+      <c r="G450" s="1">
+        <v>2</v>
+      </c>
+      <c r="H450" s="1">
+        <v>100</v>
+      </c>
+      <c r="I450" s="2">
+        <v>281</v>
+      </c>
+      <c r="J450" t="s">
+        <v>484</v>
+      </c>
+      <c r="K450" s="2">
+        <v>35</v>
+      </c>
+      <c r="L450" s="2">
+        <v>15</v>
+      </c>
+      <c r="M450" s="2">
+        <f t="shared" si="10"/>
+        <v>300.3</v>
+      </c>
+      <c r="N450" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="451" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A451" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B451" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C451" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="D451" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E451" s="1">
+        <v>84.9</v>
+      </c>
+      <c r="F451" s="1">
+        <v>8.49</v>
+      </c>
+      <c r="G451" s="1">
+        <v>2</v>
+      </c>
+      <c r="H451" s="1">
+        <v>100</v>
+      </c>
+      <c r="I451" s="2">
+        <v>296</v>
+      </c>
+      <c r="J451" t="s">
+        <v>484</v>
+      </c>
+      <c r="K451" s="2">
+        <v>35</v>
+      </c>
+      <c r="L451" s="2">
+        <v>15</v>
+      </c>
+      <c r="M451" s="2">
+        <f t="shared" si="10"/>
+        <v>110.37</v>
+      </c>
+      <c r="N451" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="452" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A452" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B452" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C452" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="D452" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E452" s="1">
+        <v>84.7</v>
+      </c>
+      <c r="F452" s="1">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="G452" s="1">
+        <v>2</v>
+      </c>
+      <c r="H452" s="1">
+        <v>100</v>
+      </c>
+      <c r="I452" s="2">
+        <v>376</v>
+      </c>
+      <c r="J452" t="s">
+        <v>484</v>
+      </c>
+      <c r="K452" s="2">
+        <v>35</v>
+      </c>
+      <c r="L452" s="2">
+        <v>15</v>
+      </c>
+      <c r="M452" s="2">
+        <f t="shared" si="10"/>
+        <v>110.11000000000001</v>
+      </c>
+      <c r="N452" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="453" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A453" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B453" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C453" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="D453" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E453" s="1">
+        <v>52.3</v>
+      </c>
+      <c r="F453" s="1">
+        <v>5.23</v>
+      </c>
+      <c r="G453" s="1">
+        <v>2</v>
+      </c>
+      <c r="H453" s="1">
+        <v>100</v>
+      </c>
+      <c r="I453" s="2">
+        <v>294</v>
+      </c>
+      <c r="J453" t="s">
+        <v>484</v>
+      </c>
+      <c r="K453" s="2">
+        <v>35</v>
+      </c>
+      <c r="L453" s="2">
+        <v>15</v>
+      </c>
+      <c r="M453" s="2">
+        <f t="shared" si="10"/>
+        <v>67.990000000000009</v>
+      </c>
+      <c r="N453" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="454" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A454" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B454" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C454" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D454" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E454" s="1">
+        <v>355</v>
+      </c>
+      <c r="F454" s="1">
+        <v>35.5</v>
+      </c>
+      <c r="G454" s="1">
+        <v>2</v>
+      </c>
+      <c r="H454" s="1">
+        <v>100</v>
+      </c>
+      <c r="I454" s="2">
+        <v>279</v>
+      </c>
+      <c r="J454" t="s">
+        <v>484</v>
+      </c>
+      <c r="K454" s="2">
+        <v>35</v>
+      </c>
+      <c r="L454" s="2">
+        <v>15</v>
+      </c>
+      <c r="M454" s="2">
+        <f t="shared" si="10"/>
+        <v>461.5</v>
+      </c>
+      <c r="N454" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="455" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A455" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B455" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C455" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="D455" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E455" s="1">
+        <v>223</v>
+      </c>
+      <c r="F455" s="1">
+        <v>22.3</v>
+      </c>
+      <c r="G455" s="1">
+        <v>2</v>
+      </c>
+      <c r="H455" s="1">
+        <v>100</v>
+      </c>
+      <c r="I455" s="2">
+        <v>377</v>
+      </c>
+      <c r="J455" t="s">
+        <v>484</v>
+      </c>
+      <c r="K455" s="2">
+        <v>35</v>
+      </c>
+      <c r="L455" s="2">
+        <v>15</v>
+      </c>
+      <c r="M455" s="2">
+        <f t="shared" si="10"/>
+        <v>289.90000000000003</v>
+      </c>
+      <c r="N455" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="456" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A456" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C456" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D456" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E456" s="1">
+        <v>23</v>
+      </c>
+      <c r="F456" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G456" s="1">
+        <v>2</v>
+      </c>
+      <c r="H456" s="1">
+        <v>100</v>
+      </c>
+      <c r="I456" s="2">
+        <v>243</v>
+      </c>
+      <c r="J456" t="s">
+        <v>484</v>
+      </c>
+      <c r="K456" s="2">
+        <v>35</v>
+      </c>
+      <c r="L456" s="2">
+        <v>15</v>
+      </c>
+      <c r="M456" s="2">
+        <f t="shared" si="10"/>
+        <v>29.9</v>
+      </c>
+      <c r="N456" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="457" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A457" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B457" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C457" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="D457" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E457" s="1">
+        <v>262</v>
+      </c>
+      <c r="F457" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="G457" s="1">
+        <v>2</v>
+      </c>
+      <c r="H457" s="1">
+        <v>100</v>
+      </c>
+      <c r="I457" s="2">
+        <v>226</v>
+      </c>
+      <c r="J457" t="s">
+        <v>484</v>
+      </c>
+      <c r="K457" s="2">
+        <v>35</v>
+      </c>
+      <c r="L457" s="2">
+        <v>15</v>
+      </c>
+      <c r="M457" s="2">
+        <f t="shared" si="10"/>
+        <v>340.59999999999997</v>
+      </c>
+      <c r="N457" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="458" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A458" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C458" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="D458" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E458" s="1">
+        <v>340</v>
+      </c>
+      <c r="F458" s="1">
+        <v>34</v>
+      </c>
+      <c r="G458" s="1">
+        <v>2</v>
+      </c>
+      <c r="H458" s="1">
+        <v>100</v>
+      </c>
+      <c r="I458" s="2">
+        <v>213</v>
+      </c>
+      <c r="J458" t="s">
+        <v>484</v>
+      </c>
+      <c r="K458" s="2">
+        <v>35</v>
+      </c>
+      <c r="L458" s="2">
+        <v>15</v>
+      </c>
+      <c r="M458" s="2">
+        <f t="shared" si="10"/>
+        <v>442</v>
+      </c>
+      <c r="N458" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="459" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A459" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C459" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="D459" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E459" s="1">
+        <v>180</v>
+      </c>
+      <c r="F459" s="1">
+        <v>18</v>
+      </c>
+      <c r="G459" s="1">
+        <v>2</v>
+      </c>
+      <c r="H459" s="1">
+        <v>100</v>
+      </c>
+      <c r="I459" s="2">
+        <v>227</v>
+      </c>
+      <c r="J459" t="s">
+        <v>484</v>
+      </c>
+      <c r="K459" s="2">
+        <v>35</v>
+      </c>
+      <c r="L459" s="2">
+        <v>15</v>
+      </c>
+      <c r="M459" s="2">
+        <f t="shared" si="10"/>
+        <v>234</v>
+      </c>
+      <c r="N459" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="460" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A460" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C460" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="D460" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E460" s="1">
+        <v>62.7</v>
+      </c>
+      <c r="F460" s="1">
+        <v>6.27</v>
+      </c>
+      <c r="G460" s="1">
+        <v>2</v>
+      </c>
+      <c r="H460" s="1">
+        <v>100</v>
+      </c>
+      <c r="I460" s="2">
+        <v>201</v>
+      </c>
+      <c r="J460" t="s">
+        <v>484</v>
+      </c>
+      <c r="K460" s="2">
+        <v>35</v>
+      </c>
+      <c r="L460" s="2">
+        <v>15</v>
+      </c>
+      <c r="M460" s="2">
+        <f t="shared" si="10"/>
+        <v>81.509999999999991</v>
+      </c>
+      <c r="N460" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="461" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A461" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C461" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="D461" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E461" s="1">
+        <v>134</v>
+      </c>
+      <c r="F461" s="1">
+        <v>13.4</v>
+      </c>
+      <c r="G461" s="1">
+        <v>2</v>
+      </c>
+      <c r="H461" s="1">
+        <v>100</v>
+      </c>
+      <c r="I461" s="2">
+        <v>248</v>
+      </c>
+      <c r="J461" t="s">
+        <v>484</v>
+      </c>
+      <c r="K461" s="2">
+        <v>35</v>
+      </c>
+      <c r="L461" s="2">
+        <v>15</v>
+      </c>
+      <c r="M461" s="2">
+        <f t="shared" si="10"/>
+        <v>174.20000000000002</v>
+      </c>
+      <c r="N461" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="462" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A462" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B462" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C462" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D462" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E462" s="1">
+        <v>216</v>
+      </c>
+      <c r="F462" s="1">
+        <v>21.6</v>
+      </c>
+      <c r="G462" s="1">
+        <v>2</v>
+      </c>
+      <c r="H462" s="1">
+        <v>100</v>
+      </c>
+      <c r="I462" s="2">
+        <v>240</v>
+      </c>
+      <c r="J462" t="s">
+        <v>484</v>
+      </c>
+      <c r="K462" s="2">
+        <v>35</v>
+      </c>
+      <c r="L462" s="2">
+        <v>15</v>
+      </c>
+      <c r="M462" s="2">
+        <f t="shared" si="10"/>
+        <v>280.8</v>
+      </c>
+      <c r="N462" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="463" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A463" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B463" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C463" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="D463" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E463" s="1">
+        <v>130</v>
+      </c>
+      <c r="F463" s="1">
+        <v>13</v>
+      </c>
+      <c r="G463" s="1">
+        <v>2</v>
+      </c>
+      <c r="H463" s="1">
+        <v>100</v>
+      </c>
+      <c r="I463" s="2">
+        <v>241</v>
+      </c>
+      <c r="J463" t="s">
+        <v>484</v>
+      </c>
+      <c r="K463" s="2">
+        <v>35</v>
+      </c>
+      <c r="L463" s="2">
+        <v>15</v>
+      </c>
+      <c r="M463" s="2">
+        <f t="shared" si="10"/>
+        <v>169</v>
+      </c>
+      <c r="N463" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="464" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A464" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B464" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C464" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="D464" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E464" s="1">
+        <v>317</v>
+      </c>
+      <c r="F464" s="1">
+        <v>31.7</v>
+      </c>
+      <c r="G464" s="1">
+        <v>2</v>
+      </c>
+      <c r="H464" s="1">
+        <v>100</v>
+      </c>
+      <c r="I464" s="2">
+        <v>259</v>
+      </c>
+      <c r="J464" t="s">
+        <v>484</v>
+      </c>
+      <c r="K464" s="2">
+        <v>35</v>
+      </c>
+      <c r="L464" s="2">
+        <v>15</v>
+      </c>
+      <c r="M464" s="2">
+        <f t="shared" si="10"/>
+        <v>412.09999999999997</v>
+      </c>
+      <c r="N464" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="465" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A465" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B465" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C465" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="D465" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E465" s="1">
+        <v>273</v>
+      </c>
+      <c r="F465" s="1">
+        <v>27.3</v>
+      </c>
+      <c r="G465" s="1">
+        <v>2</v>
+      </c>
+      <c r="H465" s="1">
+        <v>100</v>
+      </c>
+      <c r="I465" s="2">
+        <v>310</v>
+      </c>
+      <c r="J465" t="s">
+        <v>484</v>
+      </c>
+      <c r="K465" s="2">
+        <v>35</v>
+      </c>
+      <c r="L465" s="2">
+        <v>15</v>
+      </c>
+      <c r="M465" s="2">
+        <f t="shared" si="10"/>
+        <v>354.90000000000003</v>
+      </c>
+      <c r="N465" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="466" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A466" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B466" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C466" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="D466" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E466" s="1">
+        <v>178</v>
+      </c>
+      <c r="F466" s="1">
+        <v>17.8</v>
+      </c>
+      <c r="G466" s="1">
+        <v>2</v>
+      </c>
+      <c r="H466" s="1">
+        <v>100</v>
+      </c>
+      <c r="I466" s="2">
+        <v>315</v>
+      </c>
+      <c r="J466" t="s">
+        <v>484</v>
+      </c>
+      <c r="K466" s="2">
+        <v>35</v>
+      </c>
+      <c r="L466" s="2">
+        <v>15</v>
+      </c>
+      <c r="M466" s="2">
+        <f t="shared" si="10"/>
+        <v>231.4</v>
+      </c>
+      <c r="N466" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="467" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A467" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B467" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C467" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="D467" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E467" s="1">
+        <v>29</v>
+      </c>
+      <c r="F467" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="G467" s="1">
+        <v>2</v>
+      </c>
+      <c r="H467" s="1">
+        <v>100</v>
+      </c>
+      <c r="I467" s="2">
+        <v>329</v>
+      </c>
+      <c r="J467" t="s">
+        <v>484</v>
+      </c>
+      <c r="K467" s="2">
+        <v>35</v>
+      </c>
+      <c r="L467" s="2">
+        <v>15</v>
+      </c>
+      <c r="M467" s="2">
+        <f t="shared" si="10"/>
+        <v>37.699999999999996</v>
+      </c>
+      <c r="N467" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="468" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A468" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B468" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C468" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="D468" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E468" s="1">
+        <v>274</v>
+      </c>
+      <c r="F468" s="1">
+        <v>27.4</v>
+      </c>
+      <c r="G468" s="1">
+        <v>2</v>
+      </c>
+      <c r="H468" s="1">
+        <v>100</v>
+      </c>
+      <c r="I468" s="2">
+        <v>303</v>
+      </c>
+      <c r="J468" t="s">
+        <v>484</v>
+      </c>
+      <c r="K468" s="2">
+        <v>35</v>
+      </c>
+      <c r="L468" s="2">
+        <v>15</v>
+      </c>
+      <c r="M468" s="2">
+        <f t="shared" si="10"/>
+        <v>356.2</v>
+      </c>
+      <c r="N468" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="469" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A469" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B469" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C469" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="D469" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E469" s="1">
+        <v>311</v>
+      </c>
+      <c r="F469" s="1">
+        <v>31.1</v>
+      </c>
+      <c r="G469" s="1">
+        <v>2</v>
+      </c>
+      <c r="H469" s="1">
+        <v>100</v>
+      </c>
+      <c r="I469" s="2">
+        <v>325</v>
+      </c>
+      <c r="J469" t="s">
+        <v>484</v>
+      </c>
+      <c r="K469" s="2">
+        <v>35</v>
+      </c>
+      <c r="L469" s="2">
+        <v>15</v>
+      </c>
+      <c r="M469" s="2">
+        <f t="shared" si="10"/>
+        <v>404.3</v>
+      </c>
+      <c r="N469" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="470" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A470" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B470" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C470" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="D470" s="8">
+        <v>43766.723252314812</v>
+      </c>
+      <c r="E470" s="1">
+        <v>289</v>
+      </c>
+      <c r="F470" s="1">
+        <v>28.9</v>
+      </c>
+      <c r="G470" s="1">
+        <v>2</v>
+      </c>
+      <c r="H470" s="1">
+        <v>100</v>
+      </c>
+      <c r="I470" s="2">
+        <v>301</v>
+      </c>
+      <c r="J470" t="s">
+        <v>484</v>
+      </c>
+      <c r="K470" s="2">
+        <v>35</v>
+      </c>
+      <c r="L470" s="2">
+        <v>15</v>
+      </c>
+      <c r="M470" s="2">
+        <f t="shared" si="10"/>
+        <v>375.7</v>
+      </c>
+      <c r="N470" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with link to notebook post
</commit_message>
<xml_diff>
--- a/analyses/master-qubit.xlsx
+++ b/analyses/master-qubit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534DC644-80A3-7B4E-88CD-34E85EA16CAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D770CBB-181B-E643-9BE2-E39349FBC5D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="14900" xr2:uid="{C961D9B2-DEF5-3E45-BFAA-11F0CD1F34D4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3599" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3623" uniqueCount="695">
   <si>
     <t>tube_number</t>
   </si>
@@ -2116,6 +2116,9 @@
   </si>
   <si>
     <t>Sample_#191028-171806</t>
+  </si>
+  <si>
+    <t>https://grace-ac.github.io/day12-extractions/</t>
   </si>
 </sst>
 </file>
@@ -2508,8 +2511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EE0E31-7CFF-2843-B4D6-D974DF19D232}">
   <dimension ref="A1:U470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A430" zoomScale="75" workbookViewId="0">
-      <selection activeCell="P459" sqref="P459"/>
+    <sheetView tabSelected="1" topLeftCell="A439" zoomScale="75" workbookViewId="0">
+      <selection activeCell="P464" sqref="P464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23980,6 +23983,9 @@
       <c r="N447" t="s">
         <v>395</v>
       </c>
+      <c r="Q447" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="448" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A448" s="1" t="s">
@@ -24025,8 +24031,11 @@
       <c r="N448" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="449" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q448" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="449" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A449" s="1" t="s">
         <v>669</v>
       </c>
@@ -24070,8 +24079,11 @@
       <c r="N449" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="450" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q449" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="450" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A450" s="1" t="s">
         <v>669</v>
       </c>
@@ -24115,8 +24127,11 @@
       <c r="N450" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="451" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q450" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="451" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A451" s="1" t="s">
         <v>669</v>
       </c>
@@ -24160,8 +24175,11 @@
       <c r="N451" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="452" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q451" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="452" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
         <v>669</v>
       </c>
@@ -24205,8 +24223,11 @@
       <c r="N452" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="453" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q452" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="453" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A453" s="1" t="s">
         <v>669</v>
       </c>
@@ -24250,8 +24271,11 @@
       <c r="N453" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="454" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q453" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="454" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A454" s="1" t="s">
         <v>669</v>
       </c>
@@ -24295,8 +24319,11 @@
       <c r="N454" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="455" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q454" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="455" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A455" s="1" t="s">
         <v>669</v>
       </c>
@@ -24340,8 +24367,11 @@
       <c r="N455" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="456" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q455" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="456" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A456" s="1" t="s">
         <v>669</v>
       </c>
@@ -24385,8 +24415,11 @@
       <c r="N456" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="457" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q456" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="457" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A457" s="1" t="s">
         <v>669</v>
       </c>
@@ -24430,8 +24463,11 @@
       <c r="N457" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="458" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q457" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="458" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A458" s="1" t="s">
         <v>669</v>
       </c>
@@ -24475,8 +24511,11 @@
       <c r="N458" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="459" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q458" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="459" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A459" s="1" t="s">
         <v>669</v>
       </c>
@@ -24520,8 +24559,11 @@
       <c r="N459" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="460" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q459" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="460" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A460" s="1" t="s">
         <v>669</v>
       </c>
@@ -24565,8 +24607,11 @@
       <c r="N460" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="461" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q460" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="461" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A461" s="1" t="s">
         <v>669</v>
       </c>
@@ -24610,8 +24655,11 @@
       <c r="N461" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="462" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q461" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="462" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A462" s="1" t="s">
         <v>669</v>
       </c>
@@ -24655,8 +24703,11 @@
       <c r="N462" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="463" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q462" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="463" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A463" s="1" t="s">
         <v>669</v>
       </c>
@@ -24700,8 +24751,11 @@
       <c r="N463" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="464" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q463" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="464" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A464" s="1" t="s">
         <v>669</v>
       </c>
@@ -24745,8 +24799,11 @@
       <c r="N464" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="465" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q464" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="465" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A465" s="1" t="s">
         <v>669</v>
       </c>
@@ -24790,8 +24847,11 @@
       <c r="N465" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="466" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q465" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="466" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A466" s="1" t="s">
         <v>669</v>
       </c>
@@ -24835,8 +24895,11 @@
       <c r="N466" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="467" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q466" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="467" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A467" s="1" t="s">
         <v>669</v>
       </c>
@@ -24880,8 +24943,11 @@
       <c r="N467" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="468" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q467" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="468" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A468" s="1" t="s">
         <v>669</v>
       </c>
@@ -24925,8 +24991,11 @@
       <c r="N468" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="469" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q468" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="469" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A469" s="1" t="s">
         <v>669</v>
       </c>
@@ -24970,8 +25039,11 @@
       <c r="N469" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="470" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q469" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="470" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A470" s="1" t="s">
         <v>669</v>
       </c>
@@ -25014,6 +25086,9 @@
       </c>
       <c r="N470" t="s">
         <v>395</v>
+      </c>
+      <c r="Q470" t="s">
+        <v>694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add today's qubit results
</commit_message>
<xml_diff>
--- a/analyses/master-qubit.xlsx
+++ b/analyses/master-qubit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF766919-7DB8-1444-B16F-2B28F54DAC3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A488026C-40E9-B446-BE45-484F3E93CD61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="14900" xr2:uid="{C961D9B2-DEF5-3E45-BFAA-11F0CD1F34D4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3769" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3913" uniqueCount="747">
   <si>
     <t>tube_number</t>
   </si>
@@ -2197,6 +2197,84 @@
   </si>
   <si>
     <t>https://grace-ac.github.io/rna-day12-results/</t>
+  </si>
+  <si>
+    <t>2019-11-01_172026</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172409</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172359</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172350</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172340</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172331</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172323</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172314</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172306</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172258</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172250</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172242</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172234</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172225</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172216</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172207</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172158</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172149</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172140</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172131</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172123</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172113</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172105</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172057</t>
+  </si>
+  <si>
+    <t>Sample_#191101-172048</t>
+  </si>
+  <si>
+    <t>https://grace-ac.github.io/rna-extractions-day12-qubitresults/</t>
   </si>
 </sst>
 </file>
@@ -2587,10 +2665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EE0E31-7CFF-2843-B4D6-D974DF19D232}">
-  <dimension ref="A1:U494"/>
+  <dimension ref="A1:U518"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A458" zoomScale="75" workbookViewId="0">
-      <selection activeCell="Q484" sqref="Q484"/>
+    <sheetView tabSelected="1" topLeftCell="E482" zoomScale="75" workbookViewId="0">
+      <selection activeCell="P511" sqref="P511"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23767,7 +23845,7 @@
         <v>15</v>
       </c>
       <c r="M441" s="2">
-        <f t="shared" ref="M441:M494" si="10">(F441)*(L441-G441)</f>
+        <f t="shared" ref="M441:M504" si="10">(F441)*(L441-G441)</f>
         <v>1092</v>
       </c>
       <c r="N441" t="s">
@@ -26319,6 +26397,1158 @@
       </c>
       <c r="R494" t="s">
         <v>720</v>
+      </c>
+    </row>
+    <row r="495" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A495" t="s">
+        <v>721</v>
+      </c>
+      <c r="B495" t="s">
+        <v>2</v>
+      </c>
+      <c r="C495" t="s">
+        <v>722</v>
+      </c>
+      <c r="D495" s="8">
+        <v>43770.725104166668</v>
+      </c>
+      <c r="E495">
+        <v>405</v>
+      </c>
+      <c r="F495">
+        <v>40.5</v>
+      </c>
+      <c r="G495">
+        <v>2</v>
+      </c>
+      <c r="H495">
+        <v>100</v>
+      </c>
+      <c r="I495" s="2">
+        <v>264</v>
+      </c>
+      <c r="J495" t="s">
+        <v>484</v>
+      </c>
+      <c r="K495" s="2">
+        <v>35</v>
+      </c>
+      <c r="L495" s="2">
+        <v>15</v>
+      </c>
+      <c r="M495" s="2">
+        <f t="shared" si="10"/>
+        <v>526.5</v>
+      </c>
+      <c r="N495" t="s">
+        <v>395</v>
+      </c>
+      <c r="R495" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="496" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A496" t="s">
+        <v>721</v>
+      </c>
+      <c r="B496" t="s">
+        <v>2</v>
+      </c>
+      <c r="C496" t="s">
+        <v>723</v>
+      </c>
+      <c r="D496" s="8">
+        <v>43770.724988425929</v>
+      </c>
+      <c r="E496">
+        <v>166</v>
+      </c>
+      <c r="F496">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G496">
+        <v>2</v>
+      </c>
+      <c r="H496">
+        <v>100</v>
+      </c>
+      <c r="I496" s="2">
+        <v>368</v>
+      </c>
+      <c r="J496" t="s">
+        <v>484</v>
+      </c>
+      <c r="K496" s="2">
+        <v>35</v>
+      </c>
+      <c r="L496" s="2">
+        <v>15</v>
+      </c>
+      <c r="M496" s="2">
+        <f t="shared" si="10"/>
+        <v>215.8</v>
+      </c>
+      <c r="N496" t="s">
+        <v>395</v>
+      </c>
+      <c r="R496" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="497" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A497" t="s">
+        <v>721</v>
+      </c>
+      <c r="B497" t="s">
+        <v>2</v>
+      </c>
+      <c r="C497" t="s">
+        <v>724</v>
+      </c>
+      <c r="D497" s="8">
+        <v>43770.72488425926</v>
+      </c>
+      <c r="E497">
+        <v>271</v>
+      </c>
+      <c r="F497">
+        <v>27.1</v>
+      </c>
+      <c r="G497">
+        <v>2</v>
+      </c>
+      <c r="H497">
+        <v>100</v>
+      </c>
+      <c r="I497" s="2">
+        <v>289</v>
+      </c>
+      <c r="J497" t="s">
+        <v>484</v>
+      </c>
+      <c r="K497" s="2">
+        <v>35</v>
+      </c>
+      <c r="L497" s="2">
+        <v>15</v>
+      </c>
+      <c r="M497" s="2">
+        <f t="shared" si="10"/>
+        <v>352.3</v>
+      </c>
+      <c r="N497" t="s">
+        <v>395</v>
+      </c>
+      <c r="R497" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="498" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A498" t="s">
+        <v>721</v>
+      </c>
+      <c r="B498" t="s">
+        <v>2</v>
+      </c>
+      <c r="C498" t="s">
+        <v>725</v>
+      </c>
+      <c r="D498" s="8">
+        <v>43770.724768518521</v>
+      </c>
+      <c r="E498">
+        <v>361</v>
+      </c>
+      <c r="F498">
+        <v>36.1</v>
+      </c>
+      <c r="G498">
+        <v>2</v>
+      </c>
+      <c r="H498">
+        <v>100</v>
+      </c>
+      <c r="I498" s="2">
+        <v>273</v>
+      </c>
+      <c r="J498" t="s">
+        <v>484</v>
+      </c>
+      <c r="K498" s="2">
+        <v>35</v>
+      </c>
+      <c r="L498" s="2">
+        <v>15</v>
+      </c>
+      <c r="M498" s="2">
+        <f t="shared" si="10"/>
+        <v>469.3</v>
+      </c>
+      <c r="N498" t="s">
+        <v>395</v>
+      </c>
+      <c r="R498" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="499" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A499" t="s">
+        <v>721</v>
+      </c>
+      <c r="B499" t="s">
+        <v>2</v>
+      </c>
+      <c r="C499" t="s">
+        <v>726</v>
+      </c>
+      <c r="D499" s="8">
+        <v>43770.724664351852</v>
+      </c>
+      <c r="E499">
+        <v>207</v>
+      </c>
+      <c r="F499">
+        <v>20.7</v>
+      </c>
+      <c r="G499">
+        <v>2</v>
+      </c>
+      <c r="H499">
+        <v>100</v>
+      </c>
+      <c r="I499" s="2">
+        <v>363</v>
+      </c>
+      <c r="J499" t="s">
+        <v>484</v>
+      </c>
+      <c r="K499" s="2">
+        <v>35</v>
+      </c>
+      <c r="L499" s="2">
+        <v>15</v>
+      </c>
+      <c r="M499" s="2">
+        <f t="shared" si="10"/>
+        <v>269.09999999999997</v>
+      </c>
+      <c r="N499" t="s">
+        <v>395</v>
+      </c>
+      <c r="R499" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="500" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A500" t="s">
+        <v>721</v>
+      </c>
+      <c r="B500" t="s">
+        <v>2</v>
+      </c>
+      <c r="C500" t="s">
+        <v>727</v>
+      </c>
+      <c r="D500" s="8">
+        <v>43770.72457175926</v>
+      </c>
+      <c r="E500">
+        <v>190</v>
+      </c>
+      <c r="F500">
+        <v>19</v>
+      </c>
+      <c r="G500">
+        <v>2</v>
+      </c>
+      <c r="H500">
+        <v>100</v>
+      </c>
+      <c r="I500" s="2">
+        <v>283</v>
+      </c>
+      <c r="J500" t="s">
+        <v>484</v>
+      </c>
+      <c r="K500" s="2">
+        <v>35</v>
+      </c>
+      <c r="L500" s="2">
+        <v>15</v>
+      </c>
+      <c r="M500" s="2">
+        <f t="shared" si="10"/>
+        <v>247</v>
+      </c>
+      <c r="N500" t="s">
+        <v>395</v>
+      </c>
+      <c r="R500" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="501" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A501" t="s">
+        <v>721</v>
+      </c>
+      <c r="B501" t="s">
+        <v>2</v>
+      </c>
+      <c r="C501" t="s">
+        <v>728</v>
+      </c>
+      <c r="D501" s="8">
+        <v>43770.72446759259</v>
+      </c>
+      <c r="E501">
+        <v>370</v>
+      </c>
+      <c r="F501">
+        <v>37</v>
+      </c>
+      <c r="G501">
+        <v>2</v>
+      </c>
+      <c r="H501">
+        <v>100</v>
+      </c>
+      <c r="I501" s="2">
+        <v>365</v>
+      </c>
+      <c r="J501" t="s">
+        <v>484</v>
+      </c>
+      <c r="K501" s="2">
+        <v>35</v>
+      </c>
+      <c r="L501" s="2">
+        <v>15</v>
+      </c>
+      <c r="M501" s="2">
+        <f t="shared" si="10"/>
+        <v>481</v>
+      </c>
+      <c r="N501" t="s">
+        <v>395</v>
+      </c>
+      <c r="R501" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="502" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A502" t="s">
+        <v>721</v>
+      </c>
+      <c r="B502" t="s">
+        <v>2</v>
+      </c>
+      <c r="C502" t="s">
+        <v>729</v>
+      </c>
+      <c r="D502" s="8">
+        <v>43770.724374999998</v>
+      </c>
+      <c r="E502">
+        <v>232</v>
+      </c>
+      <c r="F502">
+        <v>23.2</v>
+      </c>
+      <c r="G502">
+        <v>2</v>
+      </c>
+      <c r="H502">
+        <v>100</v>
+      </c>
+      <c r="I502" s="2">
+        <v>375</v>
+      </c>
+      <c r="J502" t="s">
+        <v>484</v>
+      </c>
+      <c r="K502" s="2">
+        <v>35</v>
+      </c>
+      <c r="L502" s="2">
+        <v>15</v>
+      </c>
+      <c r="M502" s="2">
+        <f t="shared" si="10"/>
+        <v>301.59999999999997</v>
+      </c>
+      <c r="N502" t="s">
+        <v>395</v>
+      </c>
+      <c r="R502" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="503" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A503" t="s">
+        <v>721</v>
+      </c>
+      <c r="B503" t="s">
+        <v>2</v>
+      </c>
+      <c r="C503" t="s">
+        <v>730</v>
+      </c>
+      <c r="D503" s="8">
+        <v>43770.724282407406</v>
+      </c>
+      <c r="E503">
+        <v>409</v>
+      </c>
+      <c r="F503">
+        <v>40.9</v>
+      </c>
+      <c r="G503">
+        <v>2</v>
+      </c>
+      <c r="H503">
+        <v>100</v>
+      </c>
+      <c r="I503" s="2">
+        <v>297</v>
+      </c>
+      <c r="J503" t="s">
+        <v>484</v>
+      </c>
+      <c r="K503" s="2">
+        <v>35</v>
+      </c>
+      <c r="L503" s="2">
+        <v>15</v>
+      </c>
+      <c r="M503" s="2">
+        <f t="shared" si="10"/>
+        <v>531.69999999999993</v>
+      </c>
+      <c r="N503" t="s">
+        <v>395</v>
+      </c>
+      <c r="R503" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="504" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A504" t="s">
+        <v>721</v>
+      </c>
+      <c r="B504" t="s">
+        <v>2</v>
+      </c>
+      <c r="C504" t="s">
+        <v>731</v>
+      </c>
+      <c r="D504" s="8">
+        <v>43770.724189814813</v>
+      </c>
+      <c r="E504">
+        <v>266</v>
+      </c>
+      <c r="F504">
+        <v>26.6</v>
+      </c>
+      <c r="G504">
+        <v>2</v>
+      </c>
+      <c r="H504">
+        <v>100</v>
+      </c>
+      <c r="I504" s="2">
+        <v>263</v>
+      </c>
+      <c r="J504" t="s">
+        <v>484</v>
+      </c>
+      <c r="K504" s="2">
+        <v>35</v>
+      </c>
+      <c r="L504" s="2">
+        <v>15</v>
+      </c>
+      <c r="M504" s="2">
+        <f t="shared" si="10"/>
+        <v>345.8</v>
+      </c>
+      <c r="N504" t="s">
+        <v>395</v>
+      </c>
+      <c r="R504" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="505" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A505" t="s">
+        <v>721</v>
+      </c>
+      <c r="B505" t="s">
+        <v>2</v>
+      </c>
+      <c r="C505" t="s">
+        <v>732</v>
+      </c>
+      <c r="D505" s="8">
+        <v>43770.724097222221</v>
+      </c>
+      <c r="E505">
+        <v>285</v>
+      </c>
+      <c r="F505">
+        <v>28.5</v>
+      </c>
+      <c r="G505">
+        <v>2</v>
+      </c>
+      <c r="H505">
+        <v>100</v>
+      </c>
+      <c r="I505" s="2">
+        <v>371</v>
+      </c>
+      <c r="J505" t="s">
+        <v>484</v>
+      </c>
+      <c r="K505" s="2">
+        <v>35</v>
+      </c>
+      <c r="L505" s="2">
+        <v>15</v>
+      </c>
+      <c r="M505" s="2">
+        <f t="shared" ref="M505:M518" si="11">(F505)*(L505-G505)</f>
+        <v>370.5</v>
+      </c>
+      <c r="N505" t="s">
+        <v>395</v>
+      </c>
+      <c r="R505" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="506" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A506" t="s">
+        <v>721</v>
+      </c>
+      <c r="B506" t="s">
+        <v>2</v>
+      </c>
+      <c r="C506" t="s">
+        <v>733</v>
+      </c>
+      <c r="D506" s="8">
+        <v>43770.724004629628</v>
+      </c>
+      <c r="E506">
+        <v>510</v>
+      </c>
+      <c r="F506">
+        <v>51</v>
+      </c>
+      <c r="G506">
+        <v>2</v>
+      </c>
+      <c r="H506">
+        <v>100</v>
+      </c>
+      <c r="I506" s="2">
+        <v>286</v>
+      </c>
+      <c r="J506" t="s">
+        <v>484</v>
+      </c>
+      <c r="K506" s="2">
+        <v>35</v>
+      </c>
+      <c r="L506" s="2">
+        <v>15</v>
+      </c>
+      <c r="M506" s="2">
+        <f t="shared" si="11"/>
+        <v>663</v>
+      </c>
+      <c r="N506" t="s">
+        <v>395</v>
+      </c>
+      <c r="R506" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="507" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A507" t="s">
+        <v>721</v>
+      </c>
+      <c r="B507" t="s">
+        <v>2</v>
+      </c>
+      <c r="C507" t="s">
+        <v>734</v>
+      </c>
+      <c r="D507" s="8">
+        <v>43770.723900462966</v>
+      </c>
+      <c r="E507">
+        <v>177</v>
+      </c>
+      <c r="F507">
+        <v>17.7</v>
+      </c>
+      <c r="G507">
+        <v>2</v>
+      </c>
+      <c r="H507">
+        <v>100</v>
+      </c>
+      <c r="I507" s="2">
+        <v>278</v>
+      </c>
+      <c r="J507" t="s">
+        <v>484</v>
+      </c>
+      <c r="K507" s="2">
+        <v>35</v>
+      </c>
+      <c r="L507" s="2">
+        <v>15</v>
+      </c>
+      <c r="M507" s="2">
+        <f t="shared" si="11"/>
+        <v>230.1</v>
+      </c>
+      <c r="N507" t="s">
+        <v>395</v>
+      </c>
+      <c r="R507" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="508" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A508" t="s">
+        <v>721</v>
+      </c>
+      <c r="B508" t="s">
+        <v>2</v>
+      </c>
+      <c r="C508" t="s">
+        <v>735</v>
+      </c>
+      <c r="D508" s="8">
+        <v>43770.723796296297</v>
+      </c>
+      <c r="E508">
+        <v>284</v>
+      </c>
+      <c r="F508">
+        <v>28.4</v>
+      </c>
+      <c r="G508">
+        <v>2</v>
+      </c>
+      <c r="H508">
+        <v>100</v>
+      </c>
+      <c r="I508" s="2">
+        <v>254</v>
+      </c>
+      <c r="J508" t="s">
+        <v>484</v>
+      </c>
+      <c r="K508" s="2">
+        <v>35</v>
+      </c>
+      <c r="L508" s="2">
+        <v>15</v>
+      </c>
+      <c r="M508" s="2">
+        <f t="shared" si="11"/>
+        <v>369.2</v>
+      </c>
+      <c r="N508" t="s">
+        <v>395</v>
+      </c>
+      <c r="R508" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="509" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A509" t="s">
+        <v>721</v>
+      </c>
+      <c r="B509" t="s">
+        <v>2</v>
+      </c>
+      <c r="C509" t="s">
+        <v>736</v>
+      </c>
+      <c r="D509" s="8">
+        <v>43770.723692129628</v>
+      </c>
+      <c r="E509">
+        <v>420</v>
+      </c>
+      <c r="F509">
+        <v>42</v>
+      </c>
+      <c r="G509">
+        <v>2</v>
+      </c>
+      <c r="H509">
+        <v>100</v>
+      </c>
+      <c r="I509" s="2">
+        <v>203</v>
+      </c>
+      <c r="J509" t="s">
+        <v>484</v>
+      </c>
+      <c r="K509" s="2">
+        <v>35</v>
+      </c>
+      <c r="L509" s="2">
+        <v>15</v>
+      </c>
+      <c r="M509" s="2">
+        <f t="shared" si="11"/>
+        <v>546</v>
+      </c>
+      <c r="N509" t="s">
+        <v>395</v>
+      </c>
+      <c r="R509" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="510" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A510" t="s">
+        <v>721</v>
+      </c>
+      <c r="B510" t="s">
+        <v>2</v>
+      </c>
+      <c r="C510" t="s">
+        <v>737</v>
+      </c>
+      <c r="D510" s="8">
+        <v>43770.723587962966</v>
+      </c>
+      <c r="E510">
+        <v>444</v>
+      </c>
+      <c r="F510">
+        <v>44.4</v>
+      </c>
+      <c r="G510">
+        <v>2</v>
+      </c>
+      <c r="H510">
+        <v>100</v>
+      </c>
+      <c r="I510" s="2">
+        <v>216</v>
+      </c>
+      <c r="J510" t="s">
+        <v>484</v>
+      </c>
+      <c r="K510" s="2">
+        <v>35</v>
+      </c>
+      <c r="L510" s="2">
+        <v>15</v>
+      </c>
+      <c r="M510" s="2">
+        <f t="shared" si="11"/>
+        <v>577.19999999999993</v>
+      </c>
+      <c r="N510" t="s">
+        <v>395</v>
+      </c>
+      <c r="R510" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="511" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A511" t="s">
+        <v>721</v>
+      </c>
+      <c r="B511" t="s">
+        <v>2</v>
+      </c>
+      <c r="C511" t="s">
+        <v>738</v>
+      </c>
+      <c r="D511" s="8">
+        <v>43770.723483796297</v>
+      </c>
+      <c r="E511">
+        <v>315</v>
+      </c>
+      <c r="F511">
+        <v>31.5</v>
+      </c>
+      <c r="G511">
+        <v>2</v>
+      </c>
+      <c r="H511">
+        <v>100</v>
+      </c>
+      <c r="I511" s="2">
+        <v>245</v>
+      </c>
+      <c r="J511" t="s">
+        <v>484</v>
+      </c>
+      <c r="K511" s="2">
+        <v>35</v>
+      </c>
+      <c r="L511" s="2">
+        <v>15</v>
+      </c>
+      <c r="M511" s="2">
+        <f t="shared" si="11"/>
+        <v>409.5</v>
+      </c>
+      <c r="N511" t="s">
+        <v>395</v>
+      </c>
+      <c r="R511" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="512" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A512" t="s">
+        <v>721</v>
+      </c>
+      <c r="B512" t="s">
+        <v>2</v>
+      </c>
+      <c r="C512" t="s">
+        <v>739</v>
+      </c>
+      <c r="D512" s="8">
+        <v>43770.723379629628</v>
+      </c>
+      <c r="E512">
+        <v>203</v>
+      </c>
+      <c r="F512">
+        <v>20.3</v>
+      </c>
+      <c r="G512">
+        <v>2</v>
+      </c>
+      <c r="H512">
+        <v>100</v>
+      </c>
+      <c r="I512" s="2">
+        <v>239</v>
+      </c>
+      <c r="J512" t="s">
+        <v>484</v>
+      </c>
+      <c r="K512" s="2">
+        <v>35</v>
+      </c>
+      <c r="L512" s="2">
+        <v>15</v>
+      </c>
+      <c r="M512" s="2">
+        <f t="shared" si="11"/>
+        <v>263.90000000000003</v>
+      </c>
+      <c r="N512" t="s">
+        <v>395</v>
+      </c>
+      <c r="R512" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="513" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A513" t="s">
+        <v>721</v>
+      </c>
+      <c r="B513" t="s">
+        <v>2</v>
+      </c>
+      <c r="C513" t="s">
+        <v>740</v>
+      </c>
+      <c r="D513" s="8">
+        <v>43770.723275462966</v>
+      </c>
+      <c r="E513">
+        <v>125</v>
+      </c>
+      <c r="F513">
+        <v>12.5</v>
+      </c>
+      <c r="G513">
+        <v>2</v>
+      </c>
+      <c r="H513">
+        <v>100</v>
+      </c>
+      <c r="I513" s="2">
+        <v>218</v>
+      </c>
+      <c r="J513" t="s">
+        <v>484</v>
+      </c>
+      <c r="K513" s="2">
+        <v>35</v>
+      </c>
+      <c r="L513" s="2">
+        <v>15</v>
+      </c>
+      <c r="M513" s="2">
+        <f t="shared" si="11"/>
+        <v>162.5</v>
+      </c>
+      <c r="N513" t="s">
+        <v>395</v>
+      </c>
+      <c r="R513" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="514" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A514" t="s">
+        <v>721</v>
+      </c>
+      <c r="B514" t="s">
+        <v>2</v>
+      </c>
+      <c r="C514" t="s">
+        <v>741</v>
+      </c>
+      <c r="D514" s="8">
+        <v>43770.723182870373</v>
+      </c>
+      <c r="E514">
+        <v>316</v>
+      </c>
+      <c r="F514">
+        <v>31.6</v>
+      </c>
+      <c r="G514">
+        <v>2</v>
+      </c>
+      <c r="H514">
+        <v>100</v>
+      </c>
+      <c r="I514" s="2">
+        <v>250</v>
+      </c>
+      <c r="J514" t="s">
+        <v>484</v>
+      </c>
+      <c r="K514" s="2">
+        <v>35</v>
+      </c>
+      <c r="L514" s="2">
+        <v>15</v>
+      </c>
+      <c r="M514" s="2">
+        <f t="shared" si="11"/>
+        <v>410.8</v>
+      </c>
+      <c r="N514" t="s">
+        <v>395</v>
+      </c>
+      <c r="R514" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="515" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A515" t="s">
+        <v>721</v>
+      </c>
+      <c r="B515" t="s">
+        <v>2</v>
+      </c>
+      <c r="C515" t="s">
+        <v>742</v>
+      </c>
+      <c r="D515" s="8">
+        <v>43770.723067129627</v>
+      </c>
+      <c r="E515">
+        <v>287</v>
+      </c>
+      <c r="F515">
+        <v>28.7</v>
+      </c>
+      <c r="G515">
+        <v>2</v>
+      </c>
+      <c r="H515">
+        <v>100</v>
+      </c>
+      <c r="I515" s="2">
+        <v>316</v>
+      </c>
+      <c r="J515" t="s">
+        <v>484</v>
+      </c>
+      <c r="K515" s="2">
+        <v>35</v>
+      </c>
+      <c r="L515" s="2">
+        <v>15</v>
+      </c>
+      <c r="M515" s="2">
+        <f t="shared" si="11"/>
+        <v>373.09999999999997</v>
+      </c>
+      <c r="N515" t="s">
+        <v>395</v>
+      </c>
+      <c r="R515" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="516" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A516" t="s">
+        <v>721</v>
+      </c>
+      <c r="B516" t="s">
+        <v>2</v>
+      </c>
+      <c r="C516" t="s">
+        <v>743</v>
+      </c>
+      <c r="D516" s="8">
+        <v>43770.722974537035</v>
+      </c>
+      <c r="E516">
+        <v>272</v>
+      </c>
+      <c r="F516">
+        <v>27.2</v>
+      </c>
+      <c r="G516">
+        <v>2</v>
+      </c>
+      <c r="H516">
+        <v>100</v>
+      </c>
+      <c r="I516" s="2">
+        <v>257</v>
+      </c>
+      <c r="J516" t="s">
+        <v>484</v>
+      </c>
+      <c r="K516" s="2">
+        <v>35</v>
+      </c>
+      <c r="L516" s="2">
+        <v>15</v>
+      </c>
+      <c r="M516" s="2">
+        <f t="shared" si="11"/>
+        <v>353.59999999999997</v>
+      </c>
+      <c r="N516" t="s">
+        <v>395</v>
+      </c>
+      <c r="R516" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="517" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A517" t="s">
+        <v>721</v>
+      </c>
+      <c r="B517" t="s">
+        <v>2</v>
+      </c>
+      <c r="C517" t="s">
+        <v>744</v>
+      </c>
+      <c r="D517" s="8">
+        <v>43770.722881944443</v>
+      </c>
+      <c r="E517">
+        <v>280</v>
+      </c>
+      <c r="F517">
+        <v>28</v>
+      </c>
+      <c r="G517">
+        <v>2</v>
+      </c>
+      <c r="H517">
+        <v>100</v>
+      </c>
+      <c r="I517" s="2">
+        <v>228</v>
+      </c>
+      <c r="J517" t="s">
+        <v>484</v>
+      </c>
+      <c r="K517" s="2">
+        <v>35</v>
+      </c>
+      <c r="L517" s="2">
+        <v>15</v>
+      </c>
+      <c r="M517" s="2">
+        <f t="shared" si="11"/>
+        <v>364</v>
+      </c>
+      <c r="N517" t="s">
+        <v>395</v>
+      </c>
+      <c r="R517" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="518" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A518" t="s">
+        <v>721</v>
+      </c>
+      <c r="B518" t="s">
+        <v>2</v>
+      </c>
+      <c r="C518" t="s">
+        <v>745</v>
+      </c>
+      <c r="D518" s="8">
+        <v>43770.722777777781</v>
+      </c>
+      <c r="E518">
+        <v>129</v>
+      </c>
+      <c r="F518">
+        <v>12.9</v>
+      </c>
+      <c r="G518">
+        <v>2</v>
+      </c>
+      <c r="H518">
+        <v>100</v>
+      </c>
+      <c r="I518" s="2">
+        <v>220</v>
+      </c>
+      <c r="J518" t="s">
+        <v>484</v>
+      </c>
+      <c r="K518" s="2">
+        <v>35</v>
+      </c>
+      <c r="L518" s="2">
+        <v>15</v>
+      </c>
+      <c r="M518" s="2">
+        <f t="shared" si="11"/>
+        <v>167.70000000000002</v>
+      </c>
+      <c r="N518" t="s">
+        <v>395</v>
+      </c>
+      <c r="R518" t="s">
+        <v>746</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new qubit data
</commit_message>
<xml_diff>
--- a/analyses/master-qubit.xlsx
+++ b/analyses/master-qubit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A488026C-40E9-B446-BE45-484F3E93CD61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A82001-B3A9-224C-BACF-48EA6D3B2661}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="14900" xr2:uid="{C961D9B2-DEF5-3E45-BFAA-11F0CD1F34D4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3913" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3985" uniqueCount="762">
   <si>
     <t>tube_number</t>
   </si>
@@ -2275,6 +2275,51 @@
   </si>
   <si>
     <t>https://grace-ac.github.io/rna-extractions-day12-qubitresults/</t>
+  </si>
+  <si>
+    <t>2019-11-15_145544</t>
+  </si>
+  <si>
+    <t>Sample_#191115-145728</t>
+  </si>
+  <si>
+    <t>Sample_#191115-145719</t>
+  </si>
+  <si>
+    <t>Sample_#191115-145708</t>
+  </si>
+  <si>
+    <t>Sample_#191115-145700</t>
+  </si>
+  <si>
+    <t>Sample_#191115-145649</t>
+  </si>
+  <si>
+    <t>Sample_#191115-145640</t>
+  </si>
+  <si>
+    <t>Sample_#191115-145630</t>
+  </si>
+  <si>
+    <t>Sample_#191115-145622</t>
+  </si>
+  <si>
+    <t>Sample_#191115-145613</t>
+  </si>
+  <si>
+    <t>Sample_#191115-145604</t>
+  </si>
+  <si>
+    <t>2019-11-15_150415</t>
+  </si>
+  <si>
+    <t>Sample_#191115-150444</t>
+  </si>
+  <si>
+    <t>Sample_#191115-150435</t>
+  </si>
+  <si>
+    <t>https://grace-ac.github.io/rna-qubit-day9-setof12/</t>
   </si>
 </sst>
 </file>
@@ -2665,10 +2710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EE0E31-7CFF-2843-B4D6-D974DF19D232}">
-  <dimension ref="A1:U518"/>
+  <dimension ref="A1:U530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E482" zoomScale="75" workbookViewId="0">
-      <selection activeCell="P511" sqref="P511"/>
+    <sheetView tabSelected="1" topLeftCell="G501" zoomScale="75" workbookViewId="0">
+      <selection activeCell="Q526" sqref="Q526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26917,7 +26962,7 @@
         <v>15</v>
       </c>
       <c r="M505" s="2">
-        <f t="shared" ref="M505:M518" si="11">(F505)*(L505-G505)</f>
+        <f t="shared" ref="M505:M530" si="11">(F505)*(L505-G505)</f>
         <v>370.5</v>
       </c>
       <c r="N505" t="s">
@@ -27549,6 +27594,582 @@
       </c>
       <c r="R518" t="s">
         <v>746</v>
+      </c>
+    </row>
+    <row r="519" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A519" t="s">
+        <v>747</v>
+      </c>
+      <c r="B519" t="s">
+        <v>2</v>
+      </c>
+      <c r="C519" t="s">
+        <v>748</v>
+      </c>
+      <c r="D519" s="8">
+        <v>43784.623240740744</v>
+      </c>
+      <c r="E519">
+        <v>157</v>
+      </c>
+      <c r="F519">
+        <v>15.7</v>
+      </c>
+      <c r="G519">
+        <v>2</v>
+      </c>
+      <c r="H519">
+        <v>100</v>
+      </c>
+      <c r="I519" s="1">
+        <v>91</v>
+      </c>
+      <c r="J519" t="s">
+        <v>484</v>
+      </c>
+      <c r="K519" s="2">
+        <v>35</v>
+      </c>
+      <c r="L519" s="2">
+        <v>15</v>
+      </c>
+      <c r="M519" s="2">
+        <f t="shared" si="11"/>
+        <v>204.1</v>
+      </c>
+      <c r="N519" t="s">
+        <v>395</v>
+      </c>
+      <c r="R519" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="520" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A520" t="s">
+        <v>747</v>
+      </c>
+      <c r="B520" t="s">
+        <v>2</v>
+      </c>
+      <c r="C520" t="s">
+        <v>749</v>
+      </c>
+      <c r="D520" s="8">
+        <v>43784.623136574075</v>
+      </c>
+      <c r="E520">
+        <v>312</v>
+      </c>
+      <c r="F520">
+        <v>31.2</v>
+      </c>
+      <c r="G520">
+        <v>2</v>
+      </c>
+      <c r="H520">
+        <v>100</v>
+      </c>
+      <c r="I520" s="1">
+        <v>53</v>
+      </c>
+      <c r="J520" t="s">
+        <v>484</v>
+      </c>
+      <c r="K520" s="2">
+        <v>35</v>
+      </c>
+      <c r="L520" s="2">
+        <v>15</v>
+      </c>
+      <c r="M520" s="2">
+        <f t="shared" si="11"/>
+        <v>405.59999999999997</v>
+      </c>
+      <c r="N520" t="s">
+        <v>395</v>
+      </c>
+      <c r="R520" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="521" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A521" t="s">
+        <v>747</v>
+      </c>
+      <c r="B521" t="s">
+        <v>2</v>
+      </c>
+      <c r="C521" t="s">
+        <v>750</v>
+      </c>
+      <c r="D521" s="8">
+        <v>43784.62300925926</v>
+      </c>
+      <c r="E521">
+        <v>228</v>
+      </c>
+      <c r="F521">
+        <v>22.8</v>
+      </c>
+      <c r="G521">
+        <v>2</v>
+      </c>
+      <c r="H521">
+        <v>100</v>
+      </c>
+      <c r="I521" s="1">
+        <v>124</v>
+      </c>
+      <c r="J521" t="s">
+        <v>484</v>
+      </c>
+      <c r="K521" s="2">
+        <v>35</v>
+      </c>
+      <c r="L521" s="2">
+        <v>15</v>
+      </c>
+      <c r="M521" s="2">
+        <f t="shared" si="11"/>
+        <v>296.40000000000003</v>
+      </c>
+      <c r="N521" t="s">
+        <v>395</v>
+      </c>
+      <c r="R521" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="522" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A522" t="s">
+        <v>747</v>
+      </c>
+      <c r="B522" t="s">
+        <v>2</v>
+      </c>
+      <c r="C522" t="s">
+        <v>751</v>
+      </c>
+      <c r="D522" s="8">
+        <v>43784.622916666667</v>
+      </c>
+      <c r="E522">
+        <v>399</v>
+      </c>
+      <c r="F522">
+        <v>39.9</v>
+      </c>
+      <c r="G522">
+        <v>2</v>
+      </c>
+      <c r="H522">
+        <v>100</v>
+      </c>
+      <c r="I522" s="1">
+        <v>111</v>
+      </c>
+      <c r="J522" t="s">
+        <v>484</v>
+      </c>
+      <c r="K522" s="2">
+        <v>35</v>
+      </c>
+      <c r="L522" s="2">
+        <v>15</v>
+      </c>
+      <c r="M522" s="2">
+        <f t="shared" si="11"/>
+        <v>518.69999999999993</v>
+      </c>
+      <c r="N522" t="s">
+        <v>395</v>
+      </c>
+      <c r="R522" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="523" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A523" t="s">
+        <v>747</v>
+      </c>
+      <c r="B523" t="s">
+        <v>2</v>
+      </c>
+      <c r="C523" t="s">
+        <v>752</v>
+      </c>
+      <c r="D523" s="8">
+        <v>43784.622789351852</v>
+      </c>
+      <c r="E523">
+        <v>282</v>
+      </c>
+      <c r="F523">
+        <v>28.2</v>
+      </c>
+      <c r="G523">
+        <v>2</v>
+      </c>
+      <c r="H523">
+        <v>100</v>
+      </c>
+      <c r="I523" s="1">
+        <v>24</v>
+      </c>
+      <c r="J523" t="s">
+        <v>484</v>
+      </c>
+      <c r="K523" s="2">
+        <v>35</v>
+      </c>
+      <c r="L523" s="2">
+        <v>15</v>
+      </c>
+      <c r="M523" s="2">
+        <f t="shared" si="11"/>
+        <v>366.59999999999997</v>
+      </c>
+      <c r="N523" t="s">
+        <v>395</v>
+      </c>
+      <c r="R523" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="524" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A524" t="s">
+        <v>747</v>
+      </c>
+      <c r="B524" t="s">
+        <v>2</v>
+      </c>
+      <c r="C524" t="s">
+        <v>753</v>
+      </c>
+      <c r="D524" s="8">
+        <v>43784.622685185182</v>
+      </c>
+      <c r="E524">
+        <v>630</v>
+      </c>
+      <c r="F524">
+        <v>63</v>
+      </c>
+      <c r="G524">
+        <v>2</v>
+      </c>
+      <c r="H524">
+        <v>100</v>
+      </c>
+      <c r="I524" s="1">
+        <v>177</v>
+      </c>
+      <c r="J524" t="s">
+        <v>484</v>
+      </c>
+      <c r="K524" s="2">
+        <v>35</v>
+      </c>
+      <c r="L524" s="2">
+        <v>15</v>
+      </c>
+      <c r="M524" s="2">
+        <f t="shared" si="11"/>
+        <v>819</v>
+      </c>
+      <c r="N524" t="s">
+        <v>395</v>
+      </c>
+      <c r="R524" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="525" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A525" t="s">
+        <v>747</v>
+      </c>
+      <c r="B525" t="s">
+        <v>2</v>
+      </c>
+      <c r="C525" t="s">
+        <v>754</v>
+      </c>
+      <c r="D525" s="8">
+        <v>43784.622569444444</v>
+      </c>
+      <c r="E525">
+        <v>323</v>
+      </c>
+      <c r="F525">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="G525">
+        <v>2</v>
+      </c>
+      <c r="H525">
+        <v>100</v>
+      </c>
+      <c r="I525" s="1">
+        <v>119</v>
+      </c>
+      <c r="J525" t="s">
+        <v>484</v>
+      </c>
+      <c r="K525" s="2">
+        <v>35</v>
+      </c>
+      <c r="L525" s="2">
+        <v>15</v>
+      </c>
+      <c r="M525" s="2">
+        <f t="shared" si="11"/>
+        <v>419.9</v>
+      </c>
+      <c r="N525" t="s">
+        <v>395</v>
+      </c>
+      <c r="R525" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="526" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A526" t="s">
+        <v>747</v>
+      </c>
+      <c r="B526" t="s">
+        <v>2</v>
+      </c>
+      <c r="C526" t="s">
+        <v>755</v>
+      </c>
+      <c r="D526" s="8">
+        <v>43784.622476851851</v>
+      </c>
+      <c r="E526">
+        <v>331</v>
+      </c>
+      <c r="F526">
+        <v>33.1</v>
+      </c>
+      <c r="G526">
+        <v>2</v>
+      </c>
+      <c r="H526">
+        <v>100</v>
+      </c>
+      <c r="I526" s="1">
+        <v>29</v>
+      </c>
+      <c r="J526" t="s">
+        <v>484</v>
+      </c>
+      <c r="K526" s="2">
+        <v>35</v>
+      </c>
+      <c r="L526" s="2">
+        <v>15</v>
+      </c>
+      <c r="M526" s="2">
+        <f t="shared" si="11"/>
+        <v>430.3</v>
+      </c>
+      <c r="N526" t="s">
+        <v>395</v>
+      </c>
+      <c r="R526" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="527" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A527" t="s">
+        <v>747</v>
+      </c>
+      <c r="B527" t="s">
+        <v>2</v>
+      </c>
+      <c r="C527" t="s">
+        <v>756</v>
+      </c>
+      <c r="D527" s="8">
+        <v>43784.622372685182</v>
+      </c>
+      <c r="E527">
+        <v>229</v>
+      </c>
+      <c r="F527">
+        <v>22.9</v>
+      </c>
+      <c r="G527">
+        <v>2</v>
+      </c>
+      <c r="H527">
+        <v>100</v>
+      </c>
+      <c r="I527" s="1">
+        <v>10</v>
+      </c>
+      <c r="J527" t="s">
+        <v>484</v>
+      </c>
+      <c r="K527" s="2">
+        <v>35</v>
+      </c>
+      <c r="L527" s="2">
+        <v>15</v>
+      </c>
+      <c r="M527" s="2">
+        <f t="shared" si="11"/>
+        <v>297.7</v>
+      </c>
+      <c r="N527" t="s">
+        <v>395</v>
+      </c>
+      <c r="R527" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="528" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A528" t="s">
+        <v>747</v>
+      </c>
+      <c r="B528" t="s">
+        <v>2</v>
+      </c>
+      <c r="C528" t="s">
+        <v>757</v>
+      </c>
+      <c r="D528" s="8">
+        <v>43784.62226851852</v>
+      </c>
+      <c r="E528">
+        <v>281</v>
+      </c>
+      <c r="F528">
+        <v>28.1</v>
+      </c>
+      <c r="G528">
+        <v>2</v>
+      </c>
+      <c r="H528">
+        <v>100</v>
+      </c>
+      <c r="I528" s="1">
+        <v>169</v>
+      </c>
+      <c r="J528" t="s">
+        <v>484</v>
+      </c>
+      <c r="K528" s="2">
+        <v>35</v>
+      </c>
+      <c r="L528" s="2">
+        <v>15</v>
+      </c>
+      <c r="M528" s="2">
+        <f t="shared" si="11"/>
+        <v>365.3</v>
+      </c>
+      <c r="N528" t="s">
+        <v>395</v>
+      </c>
+      <c r="R528" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="529" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A529" t="s">
+        <v>758</v>
+      </c>
+      <c r="B529" t="s">
+        <v>2</v>
+      </c>
+      <c r="C529" t="s">
+        <v>759</v>
+      </c>
+      <c r="D529" s="8">
+        <v>43784.628287037034</v>
+      </c>
+      <c r="E529">
+        <v>221</v>
+      </c>
+      <c r="F529">
+        <v>22.1</v>
+      </c>
+      <c r="G529">
+        <v>2</v>
+      </c>
+      <c r="H529">
+        <v>100</v>
+      </c>
+      <c r="I529" s="1">
+        <v>28</v>
+      </c>
+      <c r="J529" t="s">
+        <v>484</v>
+      </c>
+      <c r="K529" s="2">
+        <v>35</v>
+      </c>
+      <c r="L529" s="2">
+        <v>15</v>
+      </c>
+      <c r="M529" s="2">
+        <f t="shared" si="11"/>
+        <v>287.3</v>
+      </c>
+      <c r="N529" t="s">
+        <v>395</v>
+      </c>
+      <c r="R529" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="530" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A530" t="s">
+        <v>758</v>
+      </c>
+      <c r="B530" t="s">
+        <v>2</v>
+      </c>
+      <c r="C530" t="s">
+        <v>760</v>
+      </c>
+      <c r="D530" s="8">
+        <v>43784.628182870372</v>
+      </c>
+      <c r="E530">
+        <v>510</v>
+      </c>
+      <c r="F530">
+        <v>51</v>
+      </c>
+      <c r="G530">
+        <v>2</v>
+      </c>
+      <c r="H530">
+        <v>100</v>
+      </c>
+      <c r="I530" s="1">
+        <v>81</v>
+      </c>
+      <c r="J530" t="s">
+        <v>484</v>
+      </c>
+      <c r="K530" s="2">
+        <v>35</v>
+      </c>
+      <c r="L530" s="2">
+        <v>15</v>
+      </c>
+      <c r="M530" s="2">
+        <f t="shared" si="11"/>
+        <v>663</v>
+      </c>
+      <c r="N530" t="s">
+        <v>395</v>
+      </c>
+      <c r="R530" t="s">
+        <v>761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>